<commit_message>
I have had to eliminate 2 entries and change two because of Ensembl playing around wqith IDs. It is incredible how many they change.
So, TPM2 entries (both) have changed IDs (both), while entries for ADD1 and the first TPM1 entry have been removed. Somewhere on the page we need to insist that these are GENCODE v27 identifiers and are not valid for any other annotation.

We arent adding TRIFID scores, but they were very useful to spot these errors.

Michael
</commit_message>
<xml_diff>
--- a/ws/functional_isoforms/data/FunctionalTableLong.xlsx
+++ b/ws/functional_isoforms/data/FunctionalTableLong.xlsx
@@ -1,16 +1,22 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="21721"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="10614"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/mtress/Documents/mtress/Proteomics/GENCODE27/TissueSpecificity/"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ECD28649-9E06-7C4E-876E-9453B61C7E6B}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="8660" yWindow="200" windowWidth="19640" windowHeight="15360" tabRatio="500" activeTab="1"/>
+    <workbookView xWindow="2680" yWindow="460" windowWidth="24460" windowHeight="15360" tabRatio="500" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="FunctionalTableLong.txt" sheetId="1" r:id="rId1"/>
     <sheet name="Sheet1" sheetId="2" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="140001" concurrentCalc="0"/>
+  <calcPr calcId="140001"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
       <mx:ArchID Flags="2"/>
@@ -20,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4572" uniqueCount="640">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4553" uniqueCount="634">
   <si>
     <t>ABI2</t>
   </si>
@@ -1810,12 +1816,6 @@
     <t>Urinary and others</t>
   </si>
   <si>
-    <t>Digestive, urinary and others</t>
-  </si>
-  <si>
-    <t>Muscle, nervous and others</t>
-  </si>
-  <si>
     <t>Muscle and others</t>
   </si>
   <si>
@@ -1849,27 +1849,9 @@
     <t>ENST00000317516</t>
   </si>
   <si>
-    <t>ENST00000647435</t>
-  </si>
-  <si>
-    <t>ENST00000645482</t>
-  </si>
-  <si>
     <t>HGNC</t>
   </si>
   <si>
-    <t>ADD1</t>
-  </si>
-  <si>
-    <t>ENSG00000087274</t>
-  </si>
-  <si>
-    <t>ENST00000355842</t>
-  </si>
-  <si>
-    <t>ENST00000651918</t>
-  </si>
-  <si>
     <t>PDLIM5</t>
   </si>
   <si>
@@ -1940,13 +1922,19 @@
   </si>
   <si>
     <t>This event is not clearly tissue specific, but has a lot of evidence</t>
+  </si>
+  <si>
+    <t>Tag</t>
+  </si>
+  <si>
+    <t>ENST00000329305</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="19" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="22" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -2069,6 +2057,23 @@
       <sz val="11"/>
       <name val="Calibri"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF333333"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="4">
@@ -2265,7 +2270,7 @@
     <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="40">
+  <cellXfs count="44">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
@@ -2306,6 +2311,10 @@
     <xf numFmtId="2" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="2" fontId="18" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="49" fontId="19" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="19" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="20" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="163">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
@@ -2474,6 +2483,14 @@
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleMedium4"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
@@ -2798,14 +2815,14 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:AN195"/>
   <sheetViews>
     <sheetView topLeftCell="B1" workbookViewId="0">
       <selection activeCell="R2" sqref="A1:AN195"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="5" max="19" width="4.33203125" customWidth="1"/>
     <col min="20" max="27" width="4.6640625" customWidth="1"/>
@@ -2813,7 +2830,7 @@
     <col min="29" max="40" width="8" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:40">
+    <row r="1" spans="1:40" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>528</v>
       </c>
@@ -2935,7 +2952,7 @@
         <v>207</v>
       </c>
     </row>
-    <row r="2" spans="1:40">
+    <row r="2" spans="1:40" x14ac:dyDescent="0.2">
       <c r="A2" s="1" t="s">
         <v>0</v>
       </c>
@@ -3042,7 +3059,7 @@
         <v>-0.39</v>
       </c>
     </row>
-    <row r="3" spans="1:40">
+    <row r="3" spans="1:40" x14ac:dyDescent="0.2">
       <c r="A3" s="17" t="s">
         <v>0</v>
       </c>
@@ -3154,7 +3171,7 @@
         <v>-0.47</v>
       </c>
     </row>
-    <row r="4" spans="1:40">
+    <row r="4" spans="1:40" x14ac:dyDescent="0.2">
       <c r="A4" s="1" t="s">
         <v>23</v>
       </c>
@@ -3249,7 +3266,7 @@
         <v>0.47</v>
       </c>
     </row>
-    <row r="5" spans="1:40">
+    <row r="5" spans="1:40" x14ac:dyDescent="0.2">
       <c r="A5" s="17" t="s">
         <v>23</v>
       </c>
@@ -3353,7 +3370,7 @@
         <v>0.28000000000000003</v>
       </c>
     </row>
-    <row r="6" spans="1:40">
+    <row r="6" spans="1:40" x14ac:dyDescent="0.2">
       <c r="A6" s="1" t="s">
         <v>38</v>
       </c>
@@ -3463,7 +3480,7 @@
         <v>-0.37</v>
       </c>
     </row>
-    <row r="7" spans="1:40">
+    <row r="7" spans="1:40" x14ac:dyDescent="0.2">
       <c r="A7" s="17" t="s">
         <v>38</v>
       </c>
@@ -3577,7 +3594,7 @@
         <v>0.05</v>
       </c>
     </row>
-    <row r="8" spans="1:40">
+    <row r="8" spans="1:40" x14ac:dyDescent="0.2">
       <c r="A8" s="1" t="s">
         <v>45</v>
       </c>
@@ -3681,7 +3698,7 @@
         <v>-0.54</v>
       </c>
     </row>
-    <row r="9" spans="1:40">
+    <row r="9" spans="1:40" x14ac:dyDescent="0.2">
       <c r="A9" s="17" t="s">
         <v>45</v>
       </c>
@@ -3791,7 +3808,7 @@
         <v>0.05</v>
       </c>
     </row>
-    <row r="10" spans="1:40">
+    <row r="10" spans="1:40" x14ac:dyDescent="0.2">
       <c r="A10" s="1" t="s">
         <v>54</v>
       </c>
@@ -3886,7 +3903,7 @@
         <v>-0.56999999999999995</v>
       </c>
     </row>
-    <row r="11" spans="1:40">
+    <row r="11" spans="1:40" x14ac:dyDescent="0.2">
       <c r="A11" s="17" t="s">
         <v>54</v>
       </c>
@@ -3990,7 +4007,7 @@
         <v>-0.38</v>
       </c>
     </row>
-    <row r="12" spans="1:40">
+    <row r="12" spans="1:40" x14ac:dyDescent="0.2">
       <c r="A12" s="1" t="s">
         <v>66</v>
       </c>
@@ -4100,7 +4117,7 @@
         <v>-0.45</v>
       </c>
     </row>
-    <row r="13" spans="1:40">
+    <row r="13" spans="1:40" x14ac:dyDescent="0.2">
       <c r="A13" s="17" t="s">
         <v>66</v>
       </c>
@@ -4214,7 +4231,7 @@
         <v>-0.21</v>
       </c>
     </row>
-    <row r="14" spans="1:40">
+    <row r="14" spans="1:40" x14ac:dyDescent="0.2">
       <c r="A14" s="1" t="s">
         <v>75</v>
       </c>
@@ -4321,7 +4338,7 @@
         <v>-0.34</v>
       </c>
     </row>
-    <row r="15" spans="1:40">
+    <row r="15" spans="1:40" x14ac:dyDescent="0.2">
       <c r="A15" s="17" t="s">
         <v>75</v>
       </c>
@@ -4433,7 +4450,7 @@
         <v>-0.59</v>
       </c>
     </row>
-    <row r="16" spans="1:40">
+    <row r="16" spans="1:40" x14ac:dyDescent="0.2">
       <c r="A16" s="1" t="s">
         <v>86</v>
       </c>
@@ -4537,7 +4554,7 @@
         <v>-0.8</v>
       </c>
     </row>
-    <row r="17" spans="1:40">
+    <row r="17" spans="1:40" x14ac:dyDescent="0.2">
       <c r="A17" s="17" t="s">
         <v>86</v>
       </c>
@@ -4647,7 +4664,7 @@
         <v>-0.01</v>
       </c>
     </row>
-    <row r="18" spans="1:40">
+    <row r="18" spans="1:40" x14ac:dyDescent="0.2">
       <c r="A18" s="1" t="s">
         <v>95</v>
       </c>
@@ -4751,7 +4768,7 @@
         <v>-0.46</v>
       </c>
     </row>
-    <row r="19" spans="1:40">
+    <row r="19" spans="1:40" x14ac:dyDescent="0.2">
       <c r="A19" s="17" t="s">
         <v>95</v>
       </c>
@@ -4861,7 +4878,7 @@
         <v>-7.0000000000000007E-2</v>
       </c>
     </row>
-    <row r="20" spans="1:40">
+    <row r="20" spans="1:40" x14ac:dyDescent="0.2">
       <c r="A20" s="17" t="s">
         <v>95</v>
       </c>
@@ -4971,7 +4988,7 @@
         <v>-0.11</v>
       </c>
     </row>
-    <row r="21" spans="1:40">
+    <row r="21" spans="1:40" x14ac:dyDescent="0.2">
       <c r="A21" s="17" t="s">
         <v>95</v>
       </c>
@@ -5081,7 +5098,7 @@
         <v>-0.11</v>
       </c>
     </row>
-    <row r="22" spans="1:40">
+    <row r="22" spans="1:40" x14ac:dyDescent="0.2">
       <c r="A22" s="1" t="s">
         <v>107</v>
       </c>
@@ -5191,7 +5208,7 @@
         <v>-7.0000000000000007E-2</v>
       </c>
     </row>
-    <row r="23" spans="1:40">
+    <row r="23" spans="1:40" x14ac:dyDescent="0.2">
       <c r="A23" s="17" t="s">
         <v>107</v>
       </c>
@@ -5305,7 +5322,7 @@
         <v>0.34</v>
       </c>
     </row>
-    <row r="24" spans="1:40">
+    <row r="24" spans="1:40" x14ac:dyDescent="0.2">
       <c r="A24" s="1" t="s">
         <v>118</v>
       </c>
@@ -5418,7 +5435,7 @@
         <v>-7.0000000000000007E-2</v>
       </c>
     </row>
-    <row r="25" spans="1:40">
+    <row r="25" spans="1:40" x14ac:dyDescent="0.2">
       <c r="A25" s="17" t="s">
         <v>118</v>
       </c>
@@ -5534,7 +5551,7 @@
         <v>0.37</v>
       </c>
     </row>
-    <row r="26" spans="1:40">
+    <row r="26" spans="1:40" x14ac:dyDescent="0.2">
       <c r="A26" s="1" t="s">
         <v>127</v>
       </c>
@@ -5644,7 +5661,7 @@
         <v>-0.34</v>
       </c>
     </row>
-    <row r="27" spans="1:40">
+    <row r="27" spans="1:40" x14ac:dyDescent="0.2">
       <c r="A27" s="17" t="s">
         <v>127</v>
       </c>
@@ -5758,7 +5775,7 @@
         <v>0.1</v>
       </c>
     </row>
-    <row r="28" spans="1:40">
+    <row r="28" spans="1:40" x14ac:dyDescent="0.2">
       <c r="A28" s="1" t="s">
         <v>132</v>
       </c>
@@ -5865,7 +5882,7 @@
         <v>0.2</v>
       </c>
     </row>
-    <row r="29" spans="1:40">
+    <row r="29" spans="1:40" x14ac:dyDescent="0.2">
       <c r="A29" s="17" t="s">
         <v>132</v>
       </c>
@@ -5977,7 +5994,7 @@
         <v>-0.67</v>
       </c>
     </row>
-    <row r="30" spans="1:40" ht="15" customHeight="1">
+    <row r="30" spans="1:40" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A30" s="9" t="s">
         <v>557</v>
       </c>
@@ -6079,7 +6096,7 @@
         <v>0.17326656590216999</v>
       </c>
     </row>
-    <row r="31" spans="1:40">
+    <row r="31" spans="1:40" x14ac:dyDescent="0.2">
       <c r="A31" s="19" t="s">
         <v>557</v>
       </c>
@@ -6185,7 +6202,7 @@
         <v>-0.32657694903582901</v>
       </c>
     </row>
-    <row r="32" spans="1:40">
+    <row r="32" spans="1:40" x14ac:dyDescent="0.2">
       <c r="A32" s="1" t="s">
         <v>143</v>
       </c>
@@ -6289,7 +6306,7 @@
         <v>-0.47</v>
       </c>
     </row>
-    <row r="33" spans="1:40">
+    <row r="33" spans="1:40" x14ac:dyDescent="0.2">
       <c r="A33" s="17" t="s">
         <v>143</v>
       </c>
@@ -6399,7 +6416,7 @@
         <v>-0.21</v>
       </c>
     </row>
-    <row r="34" spans="1:40">
+    <row r="34" spans="1:40" x14ac:dyDescent="0.2">
       <c r="A34" s="17" t="s">
         <v>143</v>
       </c>
@@ -6509,7 +6526,7 @@
         <v>-0.21</v>
       </c>
     </row>
-    <row r="35" spans="1:40">
+    <row r="35" spans="1:40" x14ac:dyDescent="0.2">
       <c r="A35" s="17" t="s">
         <v>143</v>
       </c>
@@ -6619,7 +6636,7 @@
         <v>-0.21</v>
       </c>
     </row>
-    <row r="36" spans="1:40">
+    <row r="36" spans="1:40" x14ac:dyDescent="0.2">
       <c r="A36" s="17" t="s">
         <v>143</v>
       </c>
@@ -6729,7 +6746,7 @@
         <v>-0.21</v>
       </c>
     </row>
-    <row r="37" spans="1:40">
+    <row r="37" spans="1:40" x14ac:dyDescent="0.2">
       <c r="A37" s="1" t="s">
         <v>154</v>
       </c>
@@ -6839,7 +6856,7 @@
         <v>-0.56999999999999995</v>
       </c>
     </row>
-    <row r="38" spans="1:40">
+    <row r="38" spans="1:40" x14ac:dyDescent="0.2">
       <c r="A38" s="17" t="s">
         <v>154</v>
       </c>
@@ -6953,7 +6970,7 @@
         <v>-0.5</v>
       </c>
     </row>
-    <row r="39" spans="1:40">
+    <row r="39" spans="1:40" x14ac:dyDescent="0.2">
       <c r="A39" s="1" t="s">
         <v>162</v>
       </c>
@@ -7039,7 +7056,7 @@
         <v>0.64</v>
       </c>
     </row>
-    <row r="40" spans="1:40">
+    <row r="40" spans="1:40" x14ac:dyDescent="0.2">
       <c r="A40" s="1" t="s">
         <v>162</v>
       </c>
@@ -7125,7 +7142,7 @@
         <v>0.64</v>
       </c>
     </row>
-    <row r="41" spans="1:40">
+    <row r="41" spans="1:40" x14ac:dyDescent="0.2">
       <c r="A41" s="1" t="s">
         <v>162</v>
       </c>
@@ -7211,7 +7228,7 @@
         <v>0.64</v>
       </c>
     </row>
-    <row r="42" spans="1:40">
+    <row r="42" spans="1:40" x14ac:dyDescent="0.2">
       <c r="A42" s="1" t="s">
         <v>162</v>
       </c>
@@ -7297,7 +7314,7 @@
         <v>0.64</v>
       </c>
     </row>
-    <row r="43" spans="1:40">
+    <row r="43" spans="1:40" x14ac:dyDescent="0.2">
       <c r="A43" s="1" t="s">
         <v>162</v>
       </c>
@@ -7383,7 +7400,7 @@
         <v>0.64</v>
       </c>
     </row>
-    <row r="44" spans="1:40">
+    <row r="44" spans="1:40" x14ac:dyDescent="0.2">
       <c r="A44" s="17" t="s">
         <v>162</v>
       </c>
@@ -7481,7 +7498,7 @@
         <v>1.03</v>
       </c>
     </row>
-    <row r="45" spans="1:40">
+    <row r="45" spans="1:40" x14ac:dyDescent="0.2">
       <c r="A45" s="17" t="s">
         <v>162</v>
       </c>
@@ -7579,7 +7596,7 @@
         <v>1.03</v>
       </c>
     </row>
-    <row r="46" spans="1:40">
+    <row r="46" spans="1:40" x14ac:dyDescent="0.2">
       <c r="A46" s="17" t="s">
         <v>162</v>
       </c>
@@ -7677,7 +7694,7 @@
         <v>1.07</v>
       </c>
     </row>
-    <row r="47" spans="1:40">
+    <row r="47" spans="1:40" x14ac:dyDescent="0.2">
       <c r="A47" s="17" t="s">
         <v>162</v>
       </c>
@@ -7775,7 +7792,7 @@
         <v>0.81</v>
       </c>
     </row>
-    <row r="48" spans="1:40">
+    <row r="48" spans="1:40" x14ac:dyDescent="0.2">
       <c r="A48" s="17" t="s">
         <v>162</v>
       </c>
@@ -7873,7 +7890,7 @@
         <v>0.81</v>
       </c>
     </row>
-    <row r="49" spans="1:40">
+    <row r="49" spans="1:40" x14ac:dyDescent="0.2">
       <c r="A49" s="17" t="s">
         <v>162</v>
       </c>
@@ -7971,7 +7988,7 @@
         <v>1.4</v>
       </c>
     </row>
-    <row r="50" spans="1:40">
+    <row r="50" spans="1:40" x14ac:dyDescent="0.2">
       <c r="A50" s="17" t="s">
         <v>162</v>
       </c>
@@ -8069,7 +8086,7 @@
         <v>1.4</v>
       </c>
     </row>
-    <row r="51" spans="1:40">
+    <row r="51" spans="1:40" x14ac:dyDescent="0.2">
       <c r="A51" s="17" t="s">
         <v>162</v>
       </c>
@@ -8167,7 +8184,7 @@
         <v>1.4</v>
       </c>
     </row>
-    <row r="52" spans="1:40">
+    <row r="52" spans="1:40" x14ac:dyDescent="0.2">
       <c r="A52" s="17" t="s">
         <v>162</v>
       </c>
@@ -8265,7 +8282,7 @@
         <v>1.3</v>
       </c>
     </row>
-    <row r="53" spans="1:40">
+    <row r="53" spans="1:40" x14ac:dyDescent="0.2">
       <c r="A53" s="17" t="s">
         <v>162</v>
       </c>
@@ -8363,7 +8380,7 @@
         <v>0.81</v>
       </c>
     </row>
-    <row r="54" spans="1:40">
+    <row r="54" spans="1:40" x14ac:dyDescent="0.2">
       <c r="A54" s="1" t="s">
         <v>185</v>
       </c>
@@ -8467,7 +8484,7 @@
         <v>-0.39</v>
       </c>
     </row>
-    <row r="55" spans="1:40">
+    <row r="55" spans="1:40" x14ac:dyDescent="0.2">
       <c r="A55" s="17" t="s">
         <v>185</v>
       </c>
@@ -8577,7 +8594,7 @@
         <v>-0.21</v>
       </c>
     </row>
-    <row r="56" spans="1:40">
+    <row r="56" spans="1:40" x14ac:dyDescent="0.2">
       <c r="A56" s="1" t="s">
         <v>194</v>
       </c>
@@ -8684,7 +8701,7 @@
         <v>-0.5</v>
       </c>
     </row>
-    <row r="57" spans="1:40">
+    <row r="57" spans="1:40" x14ac:dyDescent="0.2">
       <c r="A57" s="1" t="s">
         <v>194</v>
       </c>
@@ -8791,7 +8808,7 @@
         <v>-0.5</v>
       </c>
     </row>
-    <row r="58" spans="1:40">
+    <row r="58" spans="1:40" x14ac:dyDescent="0.2">
       <c r="A58" s="1" t="s">
         <v>194</v>
       </c>
@@ -8898,7 +8915,7 @@
         <v>-0.5</v>
       </c>
     </row>
-    <row r="59" spans="1:40">
+    <row r="59" spans="1:40" x14ac:dyDescent="0.2">
       <c r="A59" s="17" t="s">
         <v>194</v>
       </c>
@@ -9010,7 +9027,7 @@
         <v>2.58</v>
       </c>
     </row>
-    <row r="60" spans="1:40">
+    <row r="60" spans="1:40" x14ac:dyDescent="0.2">
       <c r="A60" s="17" t="s">
         <v>194</v>
       </c>
@@ -9122,7 +9139,7 @@
         <v>2.71</v>
       </c>
     </row>
-    <row r="61" spans="1:40">
+    <row r="61" spans="1:40" x14ac:dyDescent="0.2">
       <c r="A61" s="17" t="s">
         <v>194</v>
       </c>
@@ -9234,7 +9251,7 @@
         <v>2.61</v>
       </c>
     </row>
-    <row r="62" spans="1:40">
+    <row r="62" spans="1:40" x14ac:dyDescent="0.2">
       <c r="A62" s="17" t="s">
         <v>194</v>
       </c>
@@ -9346,7 +9363,7 @@
         <v>2.57</v>
       </c>
     </row>
-    <row r="63" spans="1:40">
+    <row r="63" spans="1:40" x14ac:dyDescent="0.2">
       <c r="A63" s="17" t="s">
         <v>194</v>
       </c>
@@ -9458,7 +9475,7 @@
         <v>2.71</v>
       </c>
     </row>
-    <row r="64" spans="1:40">
+    <row r="64" spans="1:40" x14ac:dyDescent="0.2">
       <c r="A64" s="1" t="s">
         <v>212</v>
       </c>
@@ -9553,7 +9570,7 @@
         <v>-0.49</v>
       </c>
     </row>
-    <row r="65" spans="1:40">
+    <row r="65" spans="1:40" x14ac:dyDescent="0.2">
       <c r="A65" s="1" t="s">
         <v>212</v>
       </c>
@@ -9648,7 +9665,7 @@
         <v>-0.49</v>
       </c>
     </row>
-    <row r="66" spans="1:40">
+    <row r="66" spans="1:40" x14ac:dyDescent="0.2">
       <c r="A66" s="17" t="s">
         <v>212</v>
       </c>
@@ -9752,7 +9769,7 @@
         <v>-0.27</v>
       </c>
     </row>
-    <row r="67" spans="1:40">
+    <row r="67" spans="1:40" x14ac:dyDescent="0.2">
       <c r="A67" s="17" t="s">
         <v>212</v>
       </c>
@@ -9856,7 +9873,7 @@
         <v>-0.27</v>
       </c>
     </row>
-    <row r="68" spans="1:40">
+    <row r="68" spans="1:40" x14ac:dyDescent="0.2">
       <c r="A68" s="1" t="s">
         <v>222</v>
       </c>
@@ -9960,7 +9977,7 @@
         <v>-0.2</v>
       </c>
     </row>
-    <row r="69" spans="1:40">
+    <row r="69" spans="1:40" x14ac:dyDescent="0.2">
       <c r="A69" s="17" t="s">
         <v>222</v>
       </c>
@@ -10070,7 +10087,7 @@
         <v>0.3</v>
       </c>
     </row>
-    <row r="70" spans="1:40">
+    <row r="70" spans="1:40" x14ac:dyDescent="0.2">
       <c r="A70" s="17" t="s">
         <v>222</v>
       </c>
@@ -10180,7 +10197,7 @@
         <v>0.36</v>
       </c>
     </row>
-    <row r="71" spans="1:40" ht="15" customHeight="1">
+    <row r="71" spans="1:40" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A71" s="17" t="s">
         <v>222</v>
       </c>
@@ -10290,7 +10307,7 @@
         <v>0.36</v>
       </c>
     </row>
-    <row r="72" spans="1:40">
+    <row r="72" spans="1:40" x14ac:dyDescent="0.2">
       <c r="A72" s="1" t="s">
         <v>234</v>
       </c>
@@ -10400,7 +10417,7 @@
         <v>-0.66</v>
       </c>
     </row>
-    <row r="73" spans="1:40">
+    <row r="73" spans="1:40" x14ac:dyDescent="0.2">
       <c r="A73" s="17" t="s">
         <v>234</v>
       </c>
@@ -10514,7 +10531,7 @@
         <v>-0.31</v>
       </c>
     </row>
-    <row r="74" spans="1:40">
+    <row r="74" spans="1:40" x14ac:dyDescent="0.2">
       <c r="A74" s="1" t="s">
         <v>245</v>
       </c>
@@ -10630,7 +10647,7 @@
         <v>-0.61</v>
       </c>
     </row>
-    <row r="75" spans="1:40">
+    <row r="75" spans="1:40" x14ac:dyDescent="0.2">
       <c r="A75" s="17" t="s">
         <v>245</v>
       </c>
@@ -10748,7 +10765,7 @@
         <v>1.07</v>
       </c>
     </row>
-    <row r="76" spans="1:40">
+    <row r="76" spans="1:40" x14ac:dyDescent="0.2">
       <c r="A76" s="1" t="s">
         <v>257</v>
       </c>
@@ -10843,7 +10860,7 @@
         <v>0.08</v>
       </c>
     </row>
-    <row r="77" spans="1:40">
+    <row r="77" spans="1:40" x14ac:dyDescent="0.2">
       <c r="A77" s="17" t="s">
         <v>257</v>
       </c>
@@ -10947,7 +10964,7 @@
         <v>0.15</v>
       </c>
     </row>
-    <row r="78" spans="1:40">
+    <row r="78" spans="1:40" x14ac:dyDescent="0.2">
       <c r="A78" s="1" t="s">
         <v>267</v>
       </c>
@@ -11042,7 +11059,7 @@
         <v>-0.34</v>
       </c>
     </row>
-    <row r="79" spans="1:40">
+    <row r="79" spans="1:40" x14ac:dyDescent="0.2">
       <c r="A79" s="17" t="s">
         <v>267</v>
       </c>
@@ -11146,7 +11163,7 @@
         <v>-0.23</v>
       </c>
     </row>
-    <row r="80" spans="1:40">
+    <row r="80" spans="1:40" x14ac:dyDescent="0.2">
       <c r="A80" s="1" t="s">
         <v>280</v>
       </c>
@@ -11256,7 +11273,7 @@
         <v>-0.5</v>
       </c>
     </row>
-    <row r="81" spans="1:40">
+    <row r="81" spans="1:40" x14ac:dyDescent="0.2">
       <c r="A81" s="1" t="s">
         <v>280</v>
       </c>
@@ -11366,7 +11383,7 @@
         <v>-0.5</v>
       </c>
     </row>
-    <row r="82" spans="1:40">
+    <row r="82" spans="1:40" x14ac:dyDescent="0.2">
       <c r="A82" s="17" t="s">
         <v>280</v>
       </c>
@@ -11480,7 +11497,7 @@
         <v>-0.06</v>
       </c>
     </row>
-    <row r="83" spans="1:40">
+    <row r="83" spans="1:40" x14ac:dyDescent="0.2">
       <c r="A83" s="1" t="s">
         <v>289</v>
       </c>
@@ -11590,7 +11607,7 @@
         <v>-0.27</v>
       </c>
     </row>
-    <row r="84" spans="1:40">
+    <row r="84" spans="1:40" x14ac:dyDescent="0.2">
       <c r="A84" s="17" t="s">
         <v>289</v>
       </c>
@@ -11704,7 +11721,7 @@
         <v>1.46</v>
       </c>
     </row>
-    <row r="85" spans="1:40">
+    <row r="85" spans="1:40" x14ac:dyDescent="0.2">
       <c r="A85" s="17" t="s">
         <v>289</v>
       </c>
@@ -11818,7 +11835,7 @@
         <v>1.46</v>
       </c>
     </row>
-    <row r="86" spans="1:40">
+    <row r="86" spans="1:40" x14ac:dyDescent="0.2">
       <c r="A86" s="1" t="s">
         <v>298</v>
       </c>
@@ -11925,7 +11942,7 @@
         <v>1.61</v>
       </c>
     </row>
-    <row r="87" spans="1:40">
+    <row r="87" spans="1:40" x14ac:dyDescent="0.2">
       <c r="A87" s="17" t="s">
         <v>298</v>
       </c>
@@ -12037,7 +12054,7 @@
         <v>1.17</v>
       </c>
     </row>
-    <row r="88" spans="1:40">
+    <row r="88" spans="1:40" x14ac:dyDescent="0.2">
       <c r="A88" s="17" t="s">
         <v>298</v>
       </c>
@@ -12149,7 +12166,7 @@
         <v>1.17</v>
       </c>
     </row>
-    <row r="89" spans="1:40">
+    <row r="89" spans="1:40" x14ac:dyDescent="0.2">
       <c r="A89" s="17" t="s">
         <v>298</v>
       </c>
@@ -12261,7 +12278,7 @@
         <v>1.31</v>
       </c>
     </row>
-    <row r="90" spans="1:40">
+    <row r="90" spans="1:40" x14ac:dyDescent="0.2">
       <c r="A90" s="17" t="s">
         <v>298</v>
       </c>
@@ -12373,7 +12390,7 @@
         <v>0.94</v>
       </c>
     </row>
-    <row r="91" spans="1:40">
+    <row r="91" spans="1:40" x14ac:dyDescent="0.2">
       <c r="A91" s="17" t="s">
         <v>298</v>
       </c>
@@ -12485,7 +12502,7 @@
         <v>0.94</v>
       </c>
     </row>
-    <row r="92" spans="1:40">
+    <row r="92" spans="1:40" x14ac:dyDescent="0.2">
       <c r="A92" s="17" t="s">
         <v>298</v>
       </c>
@@ -12597,7 +12614,7 @@
         <v>1.17</v>
       </c>
     </row>
-    <row r="93" spans="1:40">
+    <row r="93" spans="1:40" x14ac:dyDescent="0.2">
       <c r="A93" s="17" t="s">
         <v>298</v>
       </c>
@@ -12709,7 +12726,7 @@
         <v>1.17</v>
       </c>
     </row>
-    <row r="94" spans="1:40">
+    <row r="94" spans="1:40" x14ac:dyDescent="0.2">
       <c r="A94" s="17" t="s">
         <v>298</v>
       </c>
@@ -12821,7 +12838,7 @@
         <v>1.17</v>
       </c>
     </row>
-    <row r="95" spans="1:40">
+    <row r="95" spans="1:40" x14ac:dyDescent="0.2">
       <c r="A95" s="1" t="s">
         <v>312</v>
       </c>
@@ -12931,7 +12948,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="96" spans="1:40">
+    <row r="96" spans="1:40" x14ac:dyDescent="0.2">
       <c r="A96" s="17" t="s">
         <v>312</v>
       </c>
@@ -13045,7 +13062,7 @@
         <v>-0.45</v>
       </c>
     </row>
-    <row r="97" spans="1:40">
+    <row r="97" spans="1:40" x14ac:dyDescent="0.2">
       <c r="A97" s="1" t="s">
         <v>320</v>
       </c>
@@ -13152,7 +13169,7 @@
         <v>-0.21</v>
       </c>
     </row>
-    <row r="98" spans="1:40">
+    <row r="98" spans="1:40" x14ac:dyDescent="0.2">
       <c r="A98" s="1" t="s">
         <v>320</v>
       </c>
@@ -13259,7 +13276,7 @@
         <v>-0.21</v>
       </c>
     </row>
-    <row r="99" spans="1:40">
+    <row r="99" spans="1:40" x14ac:dyDescent="0.2">
       <c r="A99" s="1" t="s">
         <v>320</v>
       </c>
@@ -13366,7 +13383,7 @@
         <v>-0.21</v>
       </c>
     </row>
-    <row r="100" spans="1:40">
+    <row r="100" spans="1:40" x14ac:dyDescent="0.2">
       <c r="A100" s="1" t="s">
         <v>320</v>
       </c>
@@ -13473,7 +13490,7 @@
         <v>-0.21</v>
       </c>
     </row>
-    <row r="101" spans="1:40">
+    <row r="101" spans="1:40" x14ac:dyDescent="0.2">
       <c r="A101" s="17" t="s">
         <v>320</v>
       </c>
@@ -13585,7 +13602,7 @@
         <v>0.54</v>
       </c>
     </row>
-    <row r="102" spans="1:40">
+    <row r="102" spans="1:40" x14ac:dyDescent="0.2">
       <c r="A102" s="17" t="s">
         <v>320</v>
       </c>
@@ -13697,7 +13714,7 @@
         <v>0.54</v>
       </c>
     </row>
-    <row r="103" spans="1:40">
+    <row r="103" spans="1:40" x14ac:dyDescent="0.2">
       <c r="A103" s="17" t="s">
         <v>320</v>
       </c>
@@ -13809,7 +13826,7 @@
         <v>0.54</v>
       </c>
     </row>
-    <row r="104" spans="1:40">
+    <row r="104" spans="1:40" x14ac:dyDescent="0.2">
       <c r="A104" s="17" t="s">
         <v>320</v>
       </c>
@@ -13921,7 +13938,7 @@
         <v>0.54</v>
       </c>
     </row>
-    <row r="105" spans="1:40">
+    <row r="105" spans="1:40" x14ac:dyDescent="0.2">
       <c r="A105" s="17" t="s">
         <v>320</v>
       </c>
@@ -14033,7 +14050,7 @@
         <v>0.54</v>
       </c>
     </row>
-    <row r="106" spans="1:40">
+    <row r="106" spans="1:40" x14ac:dyDescent="0.2">
       <c r="A106" s="1" t="s">
         <v>334</v>
       </c>
@@ -14140,7 +14157,7 @@
         <v>0.2</v>
       </c>
     </row>
-    <row r="107" spans="1:40">
+    <row r="107" spans="1:40" x14ac:dyDescent="0.2">
       <c r="A107" s="17" t="s">
         <v>334</v>
       </c>
@@ -14252,7 +14269,7 @@
         <v>0.24</v>
       </c>
     </row>
-    <row r="108" spans="1:40">
+    <row r="108" spans="1:40" x14ac:dyDescent="0.2">
       <c r="A108" s="1" t="s">
         <v>344</v>
       </c>
@@ -14356,7 +14373,7 @@
         <v>-0.11</v>
       </c>
     </row>
-    <row r="109" spans="1:40">
+    <row r="109" spans="1:40" x14ac:dyDescent="0.2">
       <c r="A109" s="1" t="s">
         <v>344</v>
       </c>
@@ -14460,7 +14477,7 @@
         <v>0.17</v>
       </c>
     </row>
-    <row r="110" spans="1:40">
+    <row r="110" spans="1:40" x14ac:dyDescent="0.2">
       <c r="A110" s="1" t="s">
         <v>344</v>
       </c>
@@ -14564,7 +14581,7 @@
         <v>0.17</v>
       </c>
     </row>
-    <row r="111" spans="1:40">
+    <row r="111" spans="1:40" x14ac:dyDescent="0.2">
       <c r="A111" s="17" t="s">
         <v>344</v>
       </c>
@@ -14674,7 +14691,7 @@
         <v>-0.46</v>
       </c>
     </row>
-    <row r="112" spans="1:40">
+    <row r="112" spans="1:40" x14ac:dyDescent="0.2">
       <c r="A112" s="17" t="s">
         <v>344</v>
       </c>
@@ -14784,7 +14801,7 @@
         <v>-0.36</v>
       </c>
     </row>
-    <row r="113" spans="1:40">
+    <row r="113" spans="1:40" x14ac:dyDescent="0.2">
       <c r="A113" s="17" t="s">
         <v>344</v>
       </c>
@@ -14894,7 +14911,7 @@
         <v>-0.36</v>
       </c>
     </row>
-    <row r="114" spans="1:40">
+    <row r="114" spans="1:40" x14ac:dyDescent="0.2">
       <c r="A114" s="17" t="s">
         <v>344</v>
       </c>
@@ -15004,7 +15021,7 @@
         <v>-0.53</v>
       </c>
     </row>
-    <row r="115" spans="1:40">
+    <row r="115" spans="1:40" x14ac:dyDescent="0.2">
       <c r="A115" s="17" t="s">
         <v>344</v>
       </c>
@@ -15114,7 +15131,7 @@
         <v>-0.46</v>
       </c>
     </row>
-    <row r="116" spans="1:40">
+    <row r="116" spans="1:40" x14ac:dyDescent="0.2">
       <c r="A116" s="17" t="s">
         <v>344</v>
       </c>
@@ -15224,7 +15241,7 @@
         <v>-0.47</v>
       </c>
     </row>
-    <row r="117" spans="1:40">
+    <row r="117" spans="1:40" x14ac:dyDescent="0.2">
       <c r="A117" s="17" t="s">
         <v>344</v>
       </c>
@@ -15334,7 +15351,7 @@
         <v>-0.4</v>
       </c>
     </row>
-    <row r="118" spans="1:40">
+    <row r="118" spans="1:40" x14ac:dyDescent="0.2">
       <c r="A118" s="17" t="s">
         <v>344</v>
       </c>
@@ -15444,7 +15461,7 @@
         <v>-0.42</v>
       </c>
     </row>
-    <row r="119" spans="1:40">
+    <row r="119" spans="1:40" x14ac:dyDescent="0.2">
       <c r="A119" s="17" t="s">
         <v>344</v>
       </c>
@@ -15554,7 +15571,7 @@
         <v>-0.28999999999999998</v>
       </c>
     </row>
-    <row r="120" spans="1:40">
+    <row r="120" spans="1:40" x14ac:dyDescent="0.2">
       <c r="A120" s="1" t="s">
         <v>365</v>
       </c>
@@ -15670,7 +15687,7 @@
         <v>-0.16</v>
       </c>
     </row>
-    <row r="121" spans="1:40">
+    <row r="121" spans="1:40" x14ac:dyDescent="0.2">
       <c r="A121" s="17" t="s">
         <v>365</v>
       </c>
@@ -15788,7 +15805,7 @@
         <v>-0.41</v>
       </c>
     </row>
-    <row r="122" spans="1:40">
+    <row r="122" spans="1:40" x14ac:dyDescent="0.2">
       <c r="A122" s="17" t="s">
         <v>365</v>
       </c>
@@ -15906,7 +15923,7 @@
         <v>-0.41</v>
       </c>
     </row>
-    <row r="123" spans="1:40">
+    <row r="123" spans="1:40" x14ac:dyDescent="0.2">
       <c r="A123" s="17" t="s">
         <v>365</v>
       </c>
@@ -16024,7 +16041,7 @@
         <v>-0.41</v>
       </c>
     </row>
-    <row r="124" spans="1:40">
+    <row r="124" spans="1:40" x14ac:dyDescent="0.2">
       <c r="A124" s="17" t="s">
         <v>365</v>
       </c>
@@ -16142,7 +16159,7 @@
         <v>-0.41</v>
       </c>
     </row>
-    <row r="125" spans="1:40">
+    <row r="125" spans="1:40" x14ac:dyDescent="0.2">
       <c r="A125" s="17" t="s">
         <v>365</v>
       </c>
@@ -16260,7 +16277,7 @@
         <v>-0.41</v>
       </c>
     </row>
-    <row r="126" spans="1:40">
+    <row r="126" spans="1:40" x14ac:dyDescent="0.2">
       <c r="A126" s="17" t="s">
         <v>365</v>
       </c>
@@ -16378,7 +16395,7 @@
         <v>-0.41</v>
       </c>
     </row>
-    <row r="127" spans="1:40">
+    <row r="127" spans="1:40" x14ac:dyDescent="0.2">
       <c r="A127" s="17" t="s">
         <v>365</v>
       </c>
@@ -16496,7 +16513,7 @@
         <v>-0.41</v>
       </c>
     </row>
-    <row r="128" spans="1:40">
+    <row r="128" spans="1:40" x14ac:dyDescent="0.2">
       <c r="A128" s="17" t="s">
         <v>365</v>
       </c>
@@ -16614,7 +16631,7 @@
         <v>-0.41</v>
       </c>
     </row>
-    <row r="129" spans="1:40">
+    <row r="129" spans="1:40" x14ac:dyDescent="0.2">
       <c r="A129" s="17" t="s">
         <v>365</v>
       </c>
@@ -16732,7 +16749,7 @@
         <v>-0.34</v>
       </c>
     </row>
-    <row r="130" spans="1:40">
+    <row r="130" spans="1:40" x14ac:dyDescent="0.2">
       <c r="A130" s="17" t="s">
         <v>365</v>
       </c>
@@ -16850,7 +16867,7 @@
         <v>-0.41</v>
       </c>
     </row>
-    <row r="131" spans="1:40">
+    <row r="131" spans="1:40" x14ac:dyDescent="0.2">
       <c r="A131" s="17" t="s">
         <v>365</v>
       </c>
@@ -16968,7 +16985,7 @@
         <v>-0.41</v>
       </c>
     </row>
-    <row r="132" spans="1:40">
+    <row r="132" spans="1:40" x14ac:dyDescent="0.2">
       <c r="A132" s="17" t="s">
         <v>365</v>
       </c>
@@ -17086,7 +17103,7 @@
         <v>-0.41</v>
       </c>
     </row>
-    <row r="133" spans="1:40">
+    <row r="133" spans="1:40" x14ac:dyDescent="0.2">
       <c r="A133" s="17" t="s">
         <v>365</v>
       </c>
@@ -17204,7 +17221,7 @@
         <v>-0.41</v>
       </c>
     </row>
-    <row r="134" spans="1:40">
+    <row r="134" spans="1:40" x14ac:dyDescent="0.2">
       <c r="A134" s="17" t="s">
         <v>365</v>
       </c>
@@ -17322,7 +17339,7 @@
         <v>-0.41</v>
       </c>
     </row>
-    <row r="135" spans="1:40">
+    <row r="135" spans="1:40" x14ac:dyDescent="0.2">
       <c r="A135" s="17" t="s">
         <v>365</v>
       </c>
@@ -17440,7 +17457,7 @@
         <v>-0.41</v>
       </c>
     </row>
-    <row r="136" spans="1:40">
+    <row r="136" spans="1:40" x14ac:dyDescent="0.2">
       <c r="A136" s="17" t="s">
         <v>365</v>
       </c>
@@ -17558,7 +17575,7 @@
         <v>-0.41</v>
       </c>
     </row>
-    <row r="137" spans="1:40">
+    <row r="137" spans="1:40" x14ac:dyDescent="0.2">
       <c r="A137" s="17" t="s">
         <v>365</v>
       </c>
@@ -17676,7 +17693,7 @@
         <v>-0.41</v>
       </c>
     </row>
-    <row r="138" spans="1:40">
+    <row r="138" spans="1:40" x14ac:dyDescent="0.2">
       <c r="A138" s="17" t="s">
         <v>365</v>
       </c>
@@ -17794,7 +17811,7 @@
         <v>-0.41</v>
       </c>
     </row>
-    <row r="139" spans="1:40">
+    <row r="139" spans="1:40" x14ac:dyDescent="0.2">
       <c r="A139" s="17" t="s">
         <v>365</v>
       </c>
@@ -17912,7 +17929,7 @@
         <v>-0.41</v>
       </c>
     </row>
-    <row r="140" spans="1:40">
+    <row r="140" spans="1:40" x14ac:dyDescent="0.2">
       <c r="A140" s="17" t="s">
         <v>365</v>
       </c>
@@ -18030,7 +18047,7 @@
         <v>-0.41</v>
       </c>
     </row>
-    <row r="141" spans="1:40">
+    <row r="141" spans="1:40" x14ac:dyDescent="0.2">
       <c r="A141" s="17" t="s">
         <v>365</v>
       </c>
@@ -18148,7 +18165,7 @@
         <v>-0.41</v>
       </c>
     </row>
-    <row r="142" spans="1:40">
+    <row r="142" spans="1:40" x14ac:dyDescent="0.2">
       <c r="A142" s="17" t="s">
         <v>365</v>
       </c>
@@ -18266,7 +18283,7 @@
         <v>-0.41</v>
       </c>
     </row>
-    <row r="143" spans="1:40">
+    <row r="143" spans="1:40" x14ac:dyDescent="0.2">
       <c r="A143" s="17" t="s">
         <v>365</v>
       </c>
@@ -18384,7 +18401,7 @@
         <v>-0.39</v>
       </c>
     </row>
-    <row r="144" spans="1:40">
+    <row r="144" spans="1:40" x14ac:dyDescent="0.2">
       <c r="A144" s="17" t="s">
         <v>365</v>
       </c>
@@ -18502,7 +18519,7 @@
         <v>-0.41</v>
       </c>
     </row>
-    <row r="145" spans="1:40">
+    <row r="145" spans="1:40" x14ac:dyDescent="0.2">
       <c r="A145" s="17" t="s">
         <v>365</v>
       </c>
@@ -18620,7 +18637,7 @@
         <v>-0.41</v>
       </c>
     </row>
-    <row r="146" spans="1:40">
+    <row r="146" spans="1:40" x14ac:dyDescent="0.2">
       <c r="A146" s="17" t="s">
         <v>365</v>
       </c>
@@ -18738,7 +18755,7 @@
         <v>-0.41</v>
       </c>
     </row>
-    <row r="147" spans="1:40">
+    <row r="147" spans="1:40" x14ac:dyDescent="0.2">
       <c r="A147" s="17" t="s">
         <v>365</v>
       </c>
@@ -18856,7 +18873,7 @@
         <v>-0.41</v>
       </c>
     </row>
-    <row r="148" spans="1:40">
+    <row r="148" spans="1:40" x14ac:dyDescent="0.2">
       <c r="A148" s="17" t="s">
         <v>365</v>
       </c>
@@ -18974,7 +18991,7 @@
         <v>-0.41</v>
       </c>
     </row>
-    <row r="149" spans="1:40">
+    <row r="149" spans="1:40" x14ac:dyDescent="0.2">
       <c r="A149" s="1" t="s">
         <v>393</v>
       </c>
@@ -19081,7 +19098,7 @@
         <v>-0.22</v>
       </c>
     </row>
-    <row r="150" spans="1:40">
+    <row r="150" spans="1:40" x14ac:dyDescent="0.2">
       <c r="A150" s="17" t="s">
         <v>393</v>
       </c>
@@ -19193,7 +19210,7 @@
         <v>-0.19</v>
       </c>
     </row>
-    <row r="151" spans="1:40">
+    <row r="151" spans="1:40" x14ac:dyDescent="0.2">
       <c r="A151" s="1" t="s">
         <v>401</v>
       </c>
@@ -19294,7 +19311,7 @@
         <v>0.06</v>
       </c>
     </row>
-    <row r="152" spans="1:40">
+    <row r="152" spans="1:40" x14ac:dyDescent="0.2">
       <c r="A152" s="17" t="s">
         <v>401</v>
       </c>
@@ -19402,7 +19419,7 @@
         <v>0.01</v>
       </c>
     </row>
-    <row r="153" spans="1:40">
+    <row r="153" spans="1:40" x14ac:dyDescent="0.2">
       <c r="A153" s="1" t="s">
         <v>409</v>
       </c>
@@ -19503,7 +19520,7 @@
         <v>-0.31</v>
       </c>
     </row>
-    <row r="154" spans="1:40">
+    <row r="154" spans="1:40" x14ac:dyDescent="0.2">
       <c r="A154" s="17" t="s">
         <v>409</v>
       </c>
@@ -19611,7 +19628,7 @@
         <v>-0.7</v>
       </c>
     </row>
-    <row r="155" spans="1:40">
+    <row r="155" spans="1:40" x14ac:dyDescent="0.2">
       <c r="A155" s="17" t="s">
         <v>409</v>
       </c>
@@ -19719,7 +19736,7 @@
         <v>-0.7</v>
       </c>
     </row>
-    <row r="156" spans="1:40">
+    <row r="156" spans="1:40" x14ac:dyDescent="0.2">
       <c r="A156" s="1" t="s">
         <v>417</v>
       </c>
@@ -19829,7 +19846,7 @@
         <v>0.31</v>
       </c>
     </row>
-    <row r="157" spans="1:40">
+    <row r="157" spans="1:40" x14ac:dyDescent="0.2">
       <c r="A157" s="17" t="s">
         <v>417</v>
       </c>
@@ -19943,7 +19960,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="158" spans="1:40">
+    <row r="158" spans="1:40" x14ac:dyDescent="0.2">
       <c r="A158" s="1" t="s">
         <v>427</v>
       </c>
@@ -20047,7 +20064,7 @@
         <v>-0.63</v>
       </c>
     </row>
-    <row r="159" spans="1:40">
+    <row r="159" spans="1:40" x14ac:dyDescent="0.2">
       <c r="A159" s="17" t="s">
         <v>427</v>
       </c>
@@ -20157,7 +20174,7 @@
         <v>-0.55000000000000004</v>
       </c>
     </row>
-    <row r="160" spans="1:40">
+    <row r="160" spans="1:40" x14ac:dyDescent="0.2">
       <c r="A160" s="1" t="s">
         <v>435</v>
       </c>
@@ -20255,7 +20272,7 @@
         <v>-0.59</v>
       </c>
     </row>
-    <row r="161" spans="1:40">
+    <row r="161" spans="1:40" x14ac:dyDescent="0.2">
       <c r="A161" s="17" t="s">
         <v>435</v>
       </c>
@@ -20361,7 +20378,7 @@
         <v>-0.39</v>
       </c>
     </row>
-    <row r="162" spans="1:40">
+    <row r="162" spans="1:40" x14ac:dyDescent="0.2">
       <c r="A162" s="1" t="s">
         <v>444</v>
       </c>
@@ -20459,7 +20476,7 @@
         <v>0.08</v>
       </c>
     </row>
-    <row r="163" spans="1:40">
+    <row r="163" spans="1:40" x14ac:dyDescent="0.2">
       <c r="A163" s="17" t="s">
         <v>444</v>
       </c>
@@ -20565,7 +20582,7 @@
         <v>0.49</v>
       </c>
     </row>
-    <row r="164" spans="1:40">
+    <row r="164" spans="1:40" x14ac:dyDescent="0.2">
       <c r="A164" s="1" t="s">
         <v>453</v>
       </c>
@@ -20666,7 +20683,7 @@
         <v>-0.26</v>
       </c>
     </row>
-    <row r="165" spans="1:40">
+    <row r="165" spans="1:40" x14ac:dyDescent="0.2">
       <c r="A165" s="17" t="s">
         <v>453</v>
       </c>
@@ -20774,7 +20791,7 @@
         <v>0.49</v>
       </c>
     </row>
-    <row r="166" spans="1:40">
+    <row r="166" spans="1:40" x14ac:dyDescent="0.2">
       <c r="A166" s="1" t="s">
         <v>460</v>
       </c>
@@ -20875,7 +20892,7 @@
         <v>-0.1</v>
       </c>
     </row>
-    <row r="167" spans="1:40">
+    <row r="167" spans="1:40" x14ac:dyDescent="0.2">
       <c r="A167" s="17" t="s">
         <v>460</v>
       </c>
@@ -20983,7 +21000,7 @@
         <v>-0.09</v>
       </c>
     </row>
-    <row r="168" spans="1:40">
+    <row r="168" spans="1:40" x14ac:dyDescent="0.2">
       <c r="A168" s="1" t="s">
         <v>467</v>
       </c>
@@ -21090,7 +21107,7 @@
         <v>-0.22</v>
       </c>
     </row>
-    <row r="169" spans="1:40">
+    <row r="169" spans="1:40" x14ac:dyDescent="0.2">
       <c r="A169" s="17" t="s">
         <v>467</v>
       </c>
@@ -21202,7 +21219,7 @@
         <v>0.08</v>
       </c>
     </row>
-    <row r="170" spans="1:40">
+    <row r="170" spans="1:40" x14ac:dyDescent="0.2">
       <c r="A170" s="1" t="s">
         <v>473</v>
       </c>
@@ -21312,7 +21329,7 @@
         <v>-0.22</v>
       </c>
     </row>
-    <row r="171" spans="1:40">
+    <row r="171" spans="1:40" x14ac:dyDescent="0.2">
       <c r="A171" s="17" t="s">
         <v>473</v>
       </c>
@@ -21426,7 +21443,7 @@
         <v>0.08</v>
       </c>
     </row>
-    <row r="172" spans="1:40">
+    <row r="172" spans="1:40" x14ac:dyDescent="0.2">
       <c r="A172" s="1" t="s">
         <v>475</v>
       </c>
@@ -21530,7 +21547,7 @@
         <v>2.69</v>
       </c>
     </row>
-    <row r="173" spans="1:40">
+    <row r="173" spans="1:40" x14ac:dyDescent="0.2">
       <c r="A173" s="17" t="s">
         <v>475</v>
       </c>
@@ -21640,7 +21657,7 @@
         <v>-7.0000000000000007E-2</v>
       </c>
     </row>
-    <row r="174" spans="1:40">
+    <row r="174" spans="1:40" x14ac:dyDescent="0.2">
       <c r="A174" s="1" t="s">
         <v>484</v>
       </c>
@@ -21744,7 +21761,7 @@
         <v>2.71</v>
       </c>
     </row>
-    <row r="175" spans="1:40">
+    <row r="175" spans="1:40" x14ac:dyDescent="0.2">
       <c r="A175" s="17" t="s">
         <v>484</v>
       </c>
@@ -21854,7 +21871,7 @@
         <v>-0.1</v>
       </c>
     </row>
-    <row r="176" spans="1:40">
+    <row r="176" spans="1:40" x14ac:dyDescent="0.2">
       <c r="A176" s="1" t="s">
         <v>488</v>
       </c>
@@ -21961,7 +21978,7 @@
         <v>2.0099999999999998</v>
       </c>
     </row>
-    <row r="177" spans="1:40">
+    <row r="177" spans="1:40" x14ac:dyDescent="0.2">
       <c r="A177" s="17" t="s">
         <v>488</v>
       </c>
@@ -22073,7 +22090,7 @@
         <v>-0.45</v>
       </c>
     </row>
-    <row r="178" spans="1:40">
+    <row r="178" spans="1:40" x14ac:dyDescent="0.2">
       <c r="A178" s="1" t="s">
         <v>496</v>
       </c>
@@ -22177,7 +22194,7 @@
         <v>2.4900000000000002</v>
       </c>
     </row>
-    <row r="179" spans="1:40">
+    <row r="179" spans="1:40" x14ac:dyDescent="0.2">
       <c r="A179" s="17" t="s">
         <v>496</v>
       </c>
@@ -22287,7 +22304,7 @@
         <v>-0.4</v>
       </c>
     </row>
-    <row r="180" spans="1:40">
+    <row r="180" spans="1:40" x14ac:dyDescent="0.2">
       <c r="A180" s="1" t="s">
         <v>503</v>
       </c>
@@ -22394,7 +22411,7 @@
         <v>2.64</v>
       </c>
     </row>
-    <row r="181" spans="1:40">
+    <row r="181" spans="1:40" x14ac:dyDescent="0.2">
       <c r="A181" s="17" t="s">
         <v>503</v>
       </c>
@@ -22506,7 +22523,7 @@
         <v>-0.46</v>
       </c>
     </row>
-    <row r="182" spans="1:40">
+    <row r="182" spans="1:40" x14ac:dyDescent="0.2">
       <c r="A182" s="1" t="s">
         <v>509</v>
       </c>
@@ -22607,7 +22624,7 @@
         <v>1.06</v>
       </c>
     </row>
-    <row r="183" spans="1:40">
+    <row r="183" spans="1:40" x14ac:dyDescent="0.2">
       <c r="A183" s="1" t="s">
         <v>509</v>
       </c>
@@ -22708,7 +22725,7 @@
         <v>1.06</v>
       </c>
     </row>
-    <row r="184" spans="1:40">
+    <row r="184" spans="1:40" x14ac:dyDescent="0.2">
       <c r="A184" s="1" t="s">
         <v>509</v>
       </c>
@@ -22809,7 +22826,7 @@
         <v>1.06</v>
       </c>
     </row>
-    <row r="185" spans="1:40">
+    <row r="185" spans="1:40" x14ac:dyDescent="0.2">
       <c r="A185" s="1" t="s">
         <v>509</v>
       </c>
@@ -22910,7 +22927,7 @@
         <v>1.06</v>
       </c>
     </row>
-    <row r="186" spans="1:40">
+    <row r="186" spans="1:40" x14ac:dyDescent="0.2">
       <c r="A186" s="1" t="s">
         <v>509</v>
       </c>
@@ -23011,7 +23028,7 @@
         <v>1.06</v>
       </c>
     </row>
-    <row r="187" spans="1:40">
+    <row r="187" spans="1:40" x14ac:dyDescent="0.2">
       <c r="A187" s="1" t="s">
         <v>509</v>
       </c>
@@ -23112,7 +23129,7 @@
         <v>1.25</v>
       </c>
     </row>
-    <row r="188" spans="1:40">
+    <row r="188" spans="1:40" x14ac:dyDescent="0.2">
       <c r="A188" s="17" t="s">
         <v>509</v>
       </c>
@@ -23220,7 +23237,7 @@
         <v>-0.32</v>
       </c>
     </row>
-    <row r="189" spans="1:40">
+    <row r="189" spans="1:40" x14ac:dyDescent="0.2">
       <c r="A189" s="17" t="s">
         <v>509</v>
       </c>
@@ -23328,7 +23345,7 @@
         <v>-0.32</v>
       </c>
     </row>
-    <row r="190" spans="1:40">
+    <row r="190" spans="1:40" x14ac:dyDescent="0.2">
       <c r="A190" s="17" t="s">
         <v>509</v>
       </c>
@@ -23436,7 +23453,7 @@
         <v>-0.32</v>
       </c>
     </row>
-    <row r="191" spans="1:40">
+    <row r="191" spans="1:40" x14ac:dyDescent="0.2">
       <c r="A191" s="17" t="s">
         <v>509</v>
       </c>
@@ -23544,7 +23561,7 @@
         <v>-0.32</v>
       </c>
     </row>
-    <row r="192" spans="1:40">
+    <row r="192" spans="1:40" x14ac:dyDescent="0.2">
       <c r="A192" s="17" t="s">
         <v>509</v>
       </c>
@@ -23652,7 +23669,7 @@
         <v>-0.32</v>
       </c>
     </row>
-    <row r="193" spans="1:40">
+    <row r="193" spans="1:40" x14ac:dyDescent="0.2">
       <c r="A193" s="17" t="s">
         <v>509</v>
       </c>
@@ -23760,7 +23777,7 @@
         <v>-0.32</v>
       </c>
     </row>
-    <row r="194" spans="1:40" ht="16" customHeight="1">
+    <row r="194" spans="1:40" ht="16" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A194" s="17" t="s">
         <v>509</v>
       </c>
@@ -23868,7 +23885,7 @@
         <v>-0.32</v>
       </c>
     </row>
-    <row r="195" spans="1:40">
+    <row r="195" spans="1:40" x14ac:dyDescent="0.2">
       <c r="A195" s="17" t="s">
         <v>509</v>
       </c>
@@ -23977,7 +23994,7 @@
       </c>
     </row>
   </sheetData>
-  <sortState ref="A2:AN274">
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:AN274">
     <sortCondition ref="A2:A274"/>
   </sortState>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
@@ -23991,48 +24008,48 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:K54"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
+  <dimension ref="A1:L52"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A4" sqref="A4"/>
+    <sheetView tabSelected="1" zoomScale="92" zoomScaleNormal="92" workbookViewId="0">
+      <selection activeCell="G34" sqref="G34"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="2" max="2" width="16.1640625" customWidth="1"/>
+    <col min="2" max="2" width="6.1640625" customWidth="1"/>
     <col min="3" max="3" width="17.1640625" customWidth="1"/>
-    <col min="4" max="4" width="13.5" customWidth="1"/>
-    <col min="5" max="5" width="9.83203125" customWidth="1"/>
-    <col min="6" max="6" width="17.6640625" customWidth="1"/>
+    <col min="4" max="6" width="7.1640625" customWidth="1"/>
     <col min="7" max="7" width="16.6640625" customWidth="1"/>
-    <col min="8" max="11" width="9.83203125" customWidth="1"/>
+    <col min="8" max="10" width="6" customWidth="1"/>
+    <col min="11" max="11" width="9.83203125" customWidth="1"/>
+    <col min="16" max="16" width="4" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" s="31" customFormat="1">
+    <row r="1" spans="1:12" s="31" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A1" s="33" t="s">
+        <v>607</v>
+      </c>
+      <c r="B1" s="33" t="s">
+        <v>612</v>
+      </c>
+      <c r="C1" s="38" t="s">
+        <v>613</v>
+      </c>
+      <c r="D1" s="34" t="s">
+        <v>614</v>
+      </c>
+      <c r="E1" s="33" t="s">
+        <v>610</v>
+      </c>
+      <c r="F1" s="33" t="s">
         <v>611</v>
       </c>
-      <c r="B1" s="33" t="s">
-        <v>620</v>
-      </c>
-      <c r="C1" s="38" t="s">
-        <v>621</v>
-      </c>
-      <c r="D1" s="34" t="s">
-        <v>622</v>
-      </c>
-      <c r="E1" s="33" t="s">
-        <v>618</v>
-      </c>
-      <c r="F1" s="33" t="s">
-        <v>619</v>
-      </c>
       <c r="G1" s="34" t="s">
-        <v>623</v>
+        <v>615</v>
       </c>
       <c r="H1" s="34" t="s">
-        <v>624</v>
+        <v>616</v>
       </c>
       <c r="I1" s="33" t="s">
         <v>535</v>
@@ -24043,8 +24060,11 @@
       <c r="K1" s="37" t="s">
         <v>565</v>
       </c>
+      <c r="L1" s="31" t="s">
+        <v>632</v>
+      </c>
     </row>
-    <row r="2" spans="1:11">
+    <row r="2" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A2" s="32" t="s">
         <v>0</v>
       </c>
@@ -24058,7 +24078,7 @@
         <v>567</v>
       </c>
       <c r="E2" s="35" t="s">
-        <v>626</v>
+        <v>618</v>
       </c>
       <c r="F2" s="35" t="s">
         <v>1</v>
@@ -24079,7 +24099,7 @@
         <v>568</v>
       </c>
     </row>
-    <row r="3" spans="1:11">
+    <row r="3" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A3" s="32" t="s">
         <v>23</v>
       </c>
@@ -24093,10 +24113,10 @@
         <v>569</v>
       </c>
       <c r="E3" s="35" t="s">
-        <v>625</v>
+        <v>617</v>
       </c>
       <c r="F3" s="35" t="s">
-        <v>630</v>
+        <v>622</v>
       </c>
       <c r="G3" s="35" t="s">
         <v>27</v>
@@ -24110,7 +24130,7 @@
       </c>
       <c r="K3" s="7"/>
     </row>
-    <row r="4" spans="1:11">
+    <row r="4" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A4" s="32" t="s">
         <v>38</v>
       </c>
@@ -24124,10 +24144,10 @@
         <v>572</v>
       </c>
       <c r="E4" s="35" t="s">
-        <v>625</v>
+        <v>617</v>
       </c>
       <c r="F4" s="35" t="s">
-        <v>630</v>
+        <v>622</v>
       </c>
       <c r="G4" s="35" t="s">
         <v>46</v>
@@ -24143,7 +24163,7 @@
       </c>
       <c r="K4" s="7"/>
     </row>
-    <row r="5" spans="1:11">
+    <row r="5" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A5" s="32" t="s">
         <v>38</v>
       </c>
@@ -24157,7 +24177,7 @@
         <v>572</v>
       </c>
       <c r="E5" s="35" t="s">
-        <v>626</v>
+        <v>618</v>
       </c>
       <c r="F5" s="35" t="s">
         <v>1</v>
@@ -24178,112 +24198,112 @@
         <v>573</v>
       </c>
     </row>
-    <row r="6" spans="1:11">
-      <c r="A6" s="35" t="s">
-        <v>612</v>
+    <row r="6" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A6" s="32" t="s">
+        <v>54</v>
       </c>
       <c r="B6" s="35" t="s">
-        <v>613</v>
+        <v>58</v>
       </c>
       <c r="C6" s="39" t="s">
-        <v>615</v>
+        <v>63</v>
       </c>
       <c r="D6" s="35" t="s">
         <v>567</v>
       </c>
       <c r="E6" s="35" t="s">
-        <v>109</v>
+        <v>618</v>
       </c>
       <c r="F6" s="35" t="s">
-        <v>1</v>
+        <v>625</v>
       </c>
       <c r="G6" s="35" t="s">
-        <v>614</v>
+        <v>602</v>
       </c>
       <c r="H6" s="35" t="s">
+        <v>567</v>
+      </c>
+      <c r="I6" s="35"/>
+      <c r="J6" s="35" t="s">
+        <v>2</v>
+      </c>
+      <c r="K6" s="7" t="s">
+        <v>574</v>
+      </c>
+    </row>
+    <row r="7" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A7" s="32" t="s">
+        <v>66</v>
+      </c>
+      <c r="B7" s="35" t="s">
+        <v>67</v>
+      </c>
+      <c r="C7" s="39" t="s">
+        <v>71</v>
+      </c>
+      <c r="D7" s="35" t="s">
+        <v>575</v>
+      </c>
+      <c r="E7" s="35" t="s">
+        <v>618</v>
+      </c>
+      <c r="F7" s="35" t="s">
+        <v>625</v>
+      </c>
+      <c r="G7" s="35" t="s">
+        <v>68</v>
+      </c>
+      <c r="H7" s="35" t="s">
         <v>570</v>
-      </c>
-      <c r="I6" s="32" t="s">
-        <v>2</v>
-      </c>
-      <c r="J6" s="35" t="s">
-        <v>2</v>
-      </c>
-      <c r="K6" s="7"/>
-    </row>
-    <row r="7" spans="1:11">
-      <c r="A7" s="32" t="s">
-        <v>54</v>
-      </c>
-      <c r="B7" s="35" t="s">
-        <v>58</v>
-      </c>
-      <c r="C7" s="39" t="s">
-        <v>63</v>
-      </c>
-      <c r="D7" s="35" t="s">
-        <v>567</v>
-      </c>
-      <c r="E7" s="35" t="s">
-        <v>626</v>
-      </c>
-      <c r="F7" s="35" t="s">
-        <v>633</v>
-      </c>
-      <c r="G7" s="35" t="s">
-        <v>604</v>
-      </c>
-      <c r="H7" s="35" t="s">
-        <v>567</v>
       </c>
       <c r="I7" s="35"/>
       <c r="J7" s="35" t="s">
         <v>2</v>
       </c>
-      <c r="K7" s="7" t="s">
-        <v>574</v>
-      </c>
+      <c r="K7" s="7"/>
     </row>
-    <row r="8" spans="1:11">
+    <row r="8" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A8" s="32" t="s">
-        <v>66</v>
+        <v>75</v>
       </c>
       <c r="B8" s="35" t="s">
-        <v>67</v>
+        <v>79</v>
       </c>
       <c r="C8" s="39" t="s">
-        <v>71</v>
+        <v>82</v>
       </c>
       <c r="D8" s="35" t="s">
-        <v>575</v>
+        <v>567</v>
       </c>
       <c r="E8" s="35" t="s">
-        <v>626</v>
+        <v>77</v>
       </c>
       <c r="F8" s="35" t="s">
-        <v>633</v>
+        <v>619</v>
       </c>
       <c r="G8" s="35" t="s">
-        <v>68</v>
+        <v>80</v>
       </c>
       <c r="H8" s="35" t="s">
-        <v>570</v>
+        <v>566</v>
       </c>
       <c r="I8" s="35"/>
       <c r="J8" s="35" t="s">
         <v>2</v>
       </c>
-      <c r="K8" s="7"/>
+      <c r="K8" s="7" t="s">
+        <v>578</v>
+      </c>
     </row>
-    <row r="9" spans="1:11">
+    <row r="9" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A9" s="32" t="s">
-        <v>75</v>
+        <v>86</v>
       </c>
       <c r="B9" s="35" t="s">
-        <v>79</v>
+        <v>87</v>
       </c>
       <c r="C9" s="39" t="s">
-        <v>82</v>
+        <v>92</v>
       </c>
       <c r="D9" s="35" t="s">
         <v>567</v>
@@ -24292,112 +24312,114 @@
         <v>77</v>
       </c>
       <c r="F9" s="35" t="s">
-        <v>627</v>
+        <v>619</v>
       </c>
       <c r="G9" s="35" t="s">
-        <v>80</v>
+        <v>88</v>
       </c>
       <c r="H9" s="35" t="s">
-        <v>566</v>
-      </c>
-      <c r="I9" s="35"/>
+        <v>577</v>
+      </c>
+      <c r="I9" s="35" t="s">
+        <v>2</v>
+      </c>
       <c r="J9" s="35" t="s">
         <v>2</v>
       </c>
       <c r="K9" s="7" t="s">
-        <v>578</v>
+        <v>579</v>
       </c>
     </row>
-    <row r="10" spans="1:11">
+    <row r="10" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A10" s="32" t="s">
-        <v>86</v>
+        <v>95</v>
       </c>
       <c r="B10" s="35" t="s">
-        <v>87</v>
+        <v>98</v>
       </c>
       <c r="C10" s="39" t="s">
-        <v>92</v>
+        <v>103</v>
       </c>
       <c r="D10" s="35" t="s">
+        <v>576</v>
+      </c>
+      <c r="E10" s="35" t="s">
+        <v>617</v>
+      </c>
+      <c r="F10" s="35" t="s">
+        <v>626</v>
+      </c>
+      <c r="G10" s="35" t="s">
+        <v>99</v>
+      </c>
+      <c r="H10" s="35" t="s">
+        <v>570</v>
+      </c>
+      <c r="I10" s="35"/>
+      <c r="J10" s="35" t="s">
+        <v>2</v>
+      </c>
+      <c r="K10" s="7"/>
+    </row>
+    <row r="11" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A11" s="32" t="s">
+        <v>107</v>
+      </c>
+      <c r="B11" s="35" t="s">
+        <v>110</v>
+      </c>
+      <c r="C11" s="39" t="s">
+        <v>115</v>
+      </c>
+      <c r="D11" s="35" t="s">
+        <v>571</v>
+      </c>
+      <c r="E11" s="35" t="s">
+        <v>109</v>
+      </c>
+      <c r="F11" s="35" t="s">
+        <v>1</v>
+      </c>
+      <c r="G11" s="35" t="s">
+        <v>111</v>
+      </c>
+      <c r="H11" s="35" t="s">
         <v>567</v>
       </c>
-      <c r="E10" s="35" t="s">
-        <v>77</v>
-      </c>
-      <c r="F10" s="35" t="s">
-        <v>627</v>
-      </c>
-      <c r="G10" s="35" t="s">
-        <v>88</v>
-      </c>
-      <c r="H10" s="35" t="s">
-        <v>577</v>
-      </c>
-      <c r="I10" s="35" t="s">
-        <v>2</v>
-      </c>
-      <c r="J10" s="35" t="s">
-        <v>2</v>
-      </c>
-      <c r="K10" s="7" t="s">
-        <v>579</v>
+      <c r="I11" s="35" t="s">
+        <v>2</v>
+      </c>
+      <c r="J11" s="35" t="s">
+        <v>2</v>
+      </c>
+      <c r="K11" s="7" t="s">
+        <v>580</v>
       </c>
     </row>
-    <row r="11" spans="1:11">
-      <c r="A11" s="32" t="s">
-        <v>95</v>
-      </c>
-      <c r="B11" s="35" t="s">
-        <v>98</v>
-      </c>
-      <c r="C11" s="39" t="s">
-        <v>103</v>
-      </c>
-      <c r="D11" s="35" t="s">
-        <v>576</v>
-      </c>
-      <c r="E11" s="35" t="s">
-        <v>625</v>
-      </c>
-      <c r="F11" s="35" t="s">
-        <v>634</v>
-      </c>
-      <c r="G11" s="35" t="s">
-        <v>99</v>
-      </c>
-      <c r="H11" s="35" t="s">
-        <v>570</v>
-      </c>
-      <c r="I11" s="35"/>
-      <c r="J11" s="35" t="s">
-        <v>2</v>
-      </c>
-      <c r="K11" s="7"/>
-    </row>
-    <row r="12" spans="1:11">
+    <row r="12" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A12" s="32" t="s">
-        <v>107</v>
+        <v>118</v>
       </c>
       <c r="B12" s="35" t="s">
-        <v>110</v>
+        <v>120</v>
       </c>
       <c r="C12" s="39" t="s">
-        <v>115</v>
+        <v>124</v>
       </c>
       <c r="D12" s="35" t="s">
-        <v>571</v>
+        <v>567</v>
       </c>
       <c r="E12" s="35" t="s">
-        <v>109</v>
+        <v>618</v>
       </c>
       <c r="F12" s="35" t="s">
         <v>1</v>
       </c>
       <c r="G12" s="35" t="s">
-        <v>111</v>
+        <v>121</v>
       </c>
       <c r="H12" s="35" t="s">
-        <v>567</v>
+        <v>570</v>
       </c>
       <c r="I12" s="35" t="s">
         <v>2</v>
@@ -24405,11 +24427,9 @@
       <c r="J12" s="35" t="s">
         <v>2</v>
       </c>
-      <c r="K12" s="7" t="s">
-        <v>580</v>
-      </c>
+      <c r="K12" s="7"/>
     </row>
-    <row r="13" spans="1:11">
+    <row r="13" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A13" s="32" t="s">
         <v>118</v>
       </c>
@@ -24423,13 +24443,13 @@
         <v>567</v>
       </c>
       <c r="E13" s="35" t="s">
+        <v>617</v>
+      </c>
+      <c r="F13" s="35" t="s">
         <v>626</v>
       </c>
-      <c r="F13" s="35" t="s">
-        <v>1</v>
-      </c>
       <c r="G13" s="35" t="s">
-        <v>121</v>
+        <v>129</v>
       </c>
       <c r="H13" s="35" t="s">
         <v>570</v>
@@ -24442,30 +24462,30 @@
       </c>
       <c r="K13" s="7"/>
     </row>
-    <row r="14" spans="1:11" ht="15" customHeight="1">
+    <row r="14" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A14" s="32" t="s">
-        <v>118</v>
+        <v>132</v>
       </c>
       <c r="B14" s="35" t="s">
-        <v>120</v>
+        <v>134</v>
       </c>
       <c r="C14" s="39" t="s">
-        <v>124</v>
+        <v>141</v>
       </c>
       <c r="D14" s="35" t="s">
+        <v>570</v>
+      </c>
+      <c r="E14" s="35" t="s">
+        <v>618</v>
+      </c>
+      <c r="F14" s="35" t="s">
+        <v>1</v>
+      </c>
+      <c r="G14" s="35" t="s">
+        <v>135</v>
+      </c>
+      <c r="H14" s="35" t="s">
         <v>567</v>
-      </c>
-      <c r="E14" s="35" t="s">
-        <v>625</v>
-      </c>
-      <c r="F14" s="35" t="s">
-        <v>634</v>
-      </c>
-      <c r="G14" s="35" t="s">
-        <v>129</v>
-      </c>
-      <c r="H14" s="35" t="s">
-        <v>570</v>
       </c>
       <c r="I14" s="35" t="s">
         <v>2</v>
@@ -24475,30 +24495,30 @@
       </c>
       <c r="K14" s="7"/>
     </row>
-    <row r="15" spans="1:11">
+    <row r="15" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A15" s="32" t="s">
-        <v>132</v>
+        <v>143</v>
       </c>
       <c r="B15" s="35" t="s">
-        <v>134</v>
+        <v>144</v>
       </c>
       <c r="C15" s="39" t="s">
-        <v>141</v>
+        <v>148</v>
       </c>
       <c r="D15" s="35" t="s">
+        <v>567</v>
+      </c>
+      <c r="E15" s="35" t="s">
+        <v>77</v>
+      </c>
+      <c r="F15" s="35" t="s">
+        <v>619</v>
+      </c>
+      <c r="G15" s="35" t="s">
+        <v>145</v>
+      </c>
+      <c r="H15" s="35" t="s">
         <v>570</v>
-      </c>
-      <c r="E15" s="35" t="s">
-        <v>626</v>
-      </c>
-      <c r="F15" s="35" t="s">
-        <v>1</v>
-      </c>
-      <c r="G15" s="35" t="s">
-        <v>135</v>
-      </c>
-      <c r="H15" s="35" t="s">
-        <v>567</v>
       </c>
       <c r="I15" s="35" t="s">
         <v>2</v>
@@ -24508,392 +24528,394 @@
       </c>
       <c r="K15" s="7"/>
     </row>
-    <row r="16" spans="1:11" ht="15" customHeight="1">
+    <row r="16" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A16" s="32" t="s">
-        <v>143</v>
+        <v>598</v>
       </c>
       <c r="B16" s="35" t="s">
-        <v>144</v>
+        <v>599</v>
       </c>
       <c r="C16" s="39" t="s">
-        <v>148</v>
+        <v>601</v>
       </c>
       <c r="D16" s="35" t="s">
         <v>567</v>
       </c>
       <c r="E16" s="35" t="s">
-        <v>77</v>
+        <v>618</v>
       </c>
       <c r="F16" s="35" t="s">
-        <v>627</v>
+        <v>1</v>
       </c>
       <c r="G16" s="35" t="s">
-        <v>145</v>
+        <v>600</v>
       </c>
       <c r="H16" s="35" t="s">
         <v>570</v>
       </c>
-      <c r="I16" s="35" t="s">
-        <v>2</v>
-      </c>
-      <c r="J16" s="35" t="s">
+      <c r="I16" s="32" t="s">
+        <v>2</v>
+      </c>
+      <c r="J16" s="36" t="s">
         <v>2</v>
       </c>
       <c r="K16" s="7"/>
     </row>
-    <row r="17" spans="1:11">
+    <row r="17" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A17" s="32" t="s">
-        <v>600</v>
+        <v>609</v>
       </c>
       <c r="B17" s="35" t="s">
-        <v>601</v>
+        <v>156</v>
       </c>
       <c r="C17" s="39" t="s">
-        <v>603</v>
+        <v>160</v>
       </c>
       <c r="D17" s="35" t="s">
-        <v>567</v>
+        <v>581</v>
       </c>
       <c r="E17" s="35" t="s">
-        <v>626</v>
+        <v>618</v>
       </c>
       <c r="F17" s="35" t="s">
         <v>1</v>
       </c>
       <c r="G17" s="35" t="s">
-        <v>602</v>
+        <v>157</v>
       </c>
       <c r="H17" s="35" t="s">
         <v>570</v>
       </c>
-      <c r="I17" s="32" t="s">
-        <v>2</v>
-      </c>
-      <c r="J17" s="36" t="s">
+      <c r="I17" s="35" t="s">
+        <v>2</v>
+      </c>
+      <c r="J17" s="35" t="s">
         <v>2</v>
       </c>
       <c r="K17" s="7"/>
     </row>
-    <row r="18" spans="1:11">
+    <row r="18" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A18" s="32" t="s">
+        <v>162</v>
+      </c>
+      <c r="B18" s="35" t="s">
+        <v>163</v>
+      </c>
+      <c r="C18" s="39" t="s">
+        <v>173</v>
+      </c>
+      <c r="D18" s="35" t="s">
+        <v>582</v>
+      </c>
+      <c r="E18" s="35" t="s">
+        <v>77</v>
+      </c>
+      <c r="F18" s="35" t="s">
+        <v>619</v>
+      </c>
+      <c r="G18" s="35" t="s">
+        <v>164</v>
+      </c>
+      <c r="H18" s="35" t="s">
+        <v>582</v>
+      </c>
+      <c r="I18" s="35"/>
+      <c r="J18" s="35" t="s">
+        <v>2</v>
+      </c>
+      <c r="K18" s="7" t="s">
+        <v>583</v>
+      </c>
+    </row>
+    <row r="19" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A19" s="32" t="s">
+        <v>185</v>
+      </c>
+      <c r="B19" s="35" t="s">
+        <v>186</v>
+      </c>
+      <c r="C19" s="39" t="s">
+        <v>191</v>
+      </c>
+      <c r="D19" s="35" t="s">
+        <v>576</v>
+      </c>
+      <c r="E19" s="35" t="s">
         <v>617</v>
       </c>
-      <c r="B18" s="35" t="s">
-        <v>156</v>
-      </c>
-      <c r="C18" s="39" t="s">
-        <v>160</v>
-      </c>
-      <c r="D18" s="35" t="s">
-        <v>581</v>
-      </c>
-      <c r="E18" s="35" t="s">
-        <v>626</v>
-      </c>
-      <c r="F18" s="35" t="s">
-        <v>1</v>
-      </c>
-      <c r="G18" s="35" t="s">
-        <v>157</v>
-      </c>
-      <c r="H18" s="35" t="s">
+      <c r="F19" s="35" t="s">
+        <v>622</v>
+      </c>
+      <c r="G19" s="35" t="s">
+        <v>187</v>
+      </c>
+      <c r="H19" s="35" t="s">
         <v>570</v>
       </c>
-      <c r="I18" s="35" t="s">
-        <v>2</v>
-      </c>
-      <c r="J18" s="35" t="s">
-        <v>2</v>
-      </c>
-      <c r="K18" s="7"/>
+      <c r="I19" s="35" t="s">
+        <v>2</v>
+      </c>
+      <c r="J19" s="35" t="s">
+        <v>2</v>
+      </c>
+      <c r="K19" s="7"/>
     </row>
-    <row r="19" spans="1:11">
-      <c r="A19" s="32" t="s">
-        <v>162</v>
-      </c>
-      <c r="B19" s="35" t="s">
-        <v>163</v>
-      </c>
-      <c r="C19" s="39" t="s">
-        <v>173</v>
-      </c>
-      <c r="D19" s="35" t="s">
-        <v>582</v>
-      </c>
-      <c r="E19" s="35" t="s">
+    <row r="20" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A20" s="32" t="s">
+        <v>194</v>
+      </c>
+      <c r="B20" s="35" t="s">
+        <v>196</v>
+      </c>
+      <c r="C20" s="39" t="s">
+        <v>203</v>
+      </c>
+      <c r="D20" s="35" t="s">
+        <v>570</v>
+      </c>
+      <c r="E20" s="35" t="s">
         <v>77</v>
       </c>
-      <c r="F19" s="35" t="s">
-        <v>627</v>
-      </c>
-      <c r="G19" s="35" t="s">
-        <v>164</v>
-      </c>
-      <c r="H19" s="35" t="s">
-        <v>582</v>
-      </c>
-      <c r="I19" s="35"/>
-      <c r="J19" s="35" t="s">
-        <v>2</v>
-      </c>
-      <c r="K19" s="7" t="s">
-        <v>583</v>
-      </c>
-    </row>
-    <row r="20" spans="1:11">
-      <c r="A20" s="32" t="s">
-        <v>185</v>
-      </c>
-      <c r="B20" s="35" t="s">
-        <v>186</v>
-      </c>
-      <c r="C20" s="39" t="s">
-        <v>191</v>
-      </c>
-      <c r="D20" s="35" t="s">
-        <v>576</v>
-      </c>
-      <c r="E20" s="35" t="s">
-        <v>625</v>
-      </c>
       <c r="F20" s="35" t="s">
-        <v>630</v>
+        <v>620</v>
       </c>
       <c r="G20" s="35" t="s">
-        <v>187</v>
+        <v>197</v>
       </c>
       <c r="H20" s="35" t="s">
-        <v>570</v>
-      </c>
-      <c r="I20" s="35" t="s">
-        <v>2</v>
-      </c>
+        <v>567</v>
+      </c>
+      <c r="I20" s="35"/>
       <c r="J20" s="35" t="s">
         <v>2</v>
       </c>
       <c r="K20" s="7"/>
     </row>
-    <row r="21" spans="1:11">
+    <row r="21" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A21" s="32" t="s">
-        <v>194</v>
+        <v>212</v>
       </c>
       <c r="B21" s="35" t="s">
-        <v>196</v>
+        <v>213</v>
       </c>
       <c r="C21" s="39" t="s">
-        <v>203</v>
+        <v>218</v>
       </c>
       <c r="D21" s="35" t="s">
-        <v>570</v>
+        <v>567</v>
       </c>
       <c r="E21" s="35" t="s">
-        <v>77</v>
+        <v>617</v>
       </c>
       <c r="F21" s="35" t="s">
-        <v>628</v>
+        <v>622</v>
       </c>
       <c r="G21" s="35" t="s">
-        <v>197</v>
+        <v>214</v>
       </c>
       <c r="H21" s="35" t="s">
-        <v>567</v>
+        <v>584</v>
       </c>
       <c r="I21" s="35"/>
       <c r="J21" s="35" t="s">
         <v>2</v>
       </c>
-      <c r="K21" s="7"/>
+      <c r="K21" s="7" t="s">
+        <v>585</v>
+      </c>
     </row>
-    <row r="22" spans="1:11">
+    <row r="22" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A22" s="32" t="s">
-        <v>212</v>
+        <v>222</v>
       </c>
       <c r="B22" s="35" t="s">
-        <v>213</v>
+        <v>223</v>
       </c>
       <c r="C22" s="39" t="s">
-        <v>218</v>
+        <v>229</v>
       </c>
       <c r="D22" s="35" t="s">
-        <v>567</v>
+        <v>572</v>
       </c>
       <c r="E22" s="35" t="s">
-        <v>625</v>
+        <v>617</v>
       </c>
       <c r="F22" s="35" t="s">
-        <v>630</v>
+        <v>622</v>
       </c>
       <c r="G22" s="35" t="s">
-        <v>214</v>
+        <v>224</v>
       </c>
       <c r="H22" s="35" t="s">
-        <v>584</v>
+        <v>586</v>
       </c>
       <c r="I22" s="35"/>
       <c r="J22" s="35" t="s">
         <v>2</v>
       </c>
       <c r="K22" s="7" t="s">
-        <v>585</v>
+        <v>587</v>
       </c>
     </row>
-    <row r="23" spans="1:11">
+    <row r="23" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A23" s="32" t="s">
-        <v>222</v>
+        <v>234</v>
       </c>
       <c r="B23" s="35" t="s">
-        <v>223</v>
+        <v>237</v>
       </c>
       <c r="C23" s="39" t="s">
-        <v>229</v>
+        <v>242</v>
       </c>
       <c r="D23" s="35" t="s">
-        <v>572</v>
+        <v>567</v>
       </c>
       <c r="E23" s="35" t="s">
-        <v>625</v>
+        <v>618</v>
       </c>
       <c r="F23" s="35" t="s">
-        <v>630</v>
+        <v>1</v>
       </c>
       <c r="G23" s="35" t="s">
-        <v>224</v>
+        <v>238</v>
       </c>
       <c r="H23" s="35" t="s">
-        <v>586</v>
-      </c>
-      <c r="I23" s="35"/>
+        <v>570</v>
+      </c>
+      <c r="I23" s="35" t="s">
+        <v>2</v>
+      </c>
       <c r="J23" s="35" t="s">
         <v>2</v>
       </c>
-      <c r="K23" s="7" t="s">
-        <v>587</v>
-      </c>
+      <c r="K23" s="7"/>
     </row>
-    <row r="24" spans="1:11">
+    <row r="24" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A24" s="32" t="s">
-        <v>234</v>
+        <v>245</v>
       </c>
       <c r="B24" s="35" t="s">
-        <v>237</v>
+        <v>249</v>
       </c>
       <c r="C24" s="39" t="s">
-        <v>242</v>
+        <v>254</v>
       </c>
       <c r="D24" s="35" t="s">
+        <v>570</v>
+      </c>
+      <c r="E24" s="35" t="s">
+        <v>618</v>
+      </c>
+      <c r="F24" s="35" t="s">
+        <v>623</v>
+      </c>
+      <c r="G24" s="35" t="s">
+        <v>250</v>
+      </c>
+      <c r="H24" s="35" t="s">
         <v>567</v>
       </c>
-      <c r="E24" s="35" t="s">
-        <v>626</v>
-      </c>
-      <c r="F24" s="35" t="s">
-        <v>1</v>
-      </c>
-      <c r="G24" s="35" t="s">
-        <v>238</v>
-      </c>
-      <c r="H24" s="35" t="s">
-        <v>570</v>
-      </c>
       <c r="I24" s="35" t="s">
         <v>2</v>
       </c>
       <c r="J24" s="35" t="s">
         <v>2</v>
       </c>
-      <c r="K24" s="7"/>
+      <c r="K24" s="7" t="s">
+        <v>588</v>
+      </c>
     </row>
-    <row r="25" spans="1:11">
+    <row r="25" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A25" s="32" t="s">
-        <v>245</v>
+        <v>257</v>
       </c>
       <c r="B25" s="35" t="s">
-        <v>249</v>
+        <v>259</v>
       </c>
       <c r="C25" s="39" t="s">
-        <v>254</v>
+        <v>264</v>
       </c>
       <c r="D25" s="35" t="s">
-        <v>570</v>
+        <v>582</v>
       </c>
       <c r="E25" s="35" t="s">
-        <v>626</v>
+        <v>618</v>
       </c>
       <c r="F25" s="35" t="s">
+        <v>629</v>
+      </c>
+      <c r="G25" s="35" t="s">
+        <v>260</v>
+      </c>
+      <c r="H25" s="35" t="s">
+        <v>582</v>
+      </c>
+      <c r="I25" s="35" t="s">
+        <v>2</v>
+      </c>
+      <c r="J25" s="35" t="s">
+        <v>2</v>
+      </c>
+      <c r="K25" s="7" t="s">
         <v>631</v>
       </c>
-      <c r="G25" s="35" t="s">
-        <v>250</v>
-      </c>
-      <c r="H25" s="35" t="s">
+    </row>
+    <row r="26" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A26" s="32" t="s">
+        <v>267</v>
+      </c>
+      <c r="B26" s="35" t="s">
+        <v>268</v>
+      </c>
+      <c r="C26" s="39" t="s">
+        <v>273</v>
+      </c>
+      <c r="D26" s="35" t="s">
+        <v>576</v>
+      </c>
+      <c r="E26" s="35" t="s">
+        <v>77</v>
+      </c>
+      <c r="F26" s="35" t="s">
+        <v>619</v>
+      </c>
+      <c r="G26" s="35" t="s">
+        <v>269</v>
+      </c>
+      <c r="H26" s="35" t="s">
         <v>567</v>
       </c>
-      <c r="I25" s="35" t="s">
-        <v>2</v>
-      </c>
-      <c r="J25" s="35" t="s">
-        <v>2</v>
-      </c>
-      <c r="K25" s="7" t="s">
-        <v>588</v>
+      <c r="I26" s="35" t="s">
+        <v>2</v>
+      </c>
+      <c r="J26" s="35" t="s">
+        <v>2</v>
+      </c>
+      <c r="K26" s="7" t="s">
+        <v>589</v>
       </c>
     </row>
-    <row r="26" spans="1:11">
-      <c r="A26" s="32" t="s">
-        <v>257</v>
-      </c>
-      <c r="B26" s="35" t="s">
-        <v>259</v>
-      </c>
-      <c r="C26" s="39" t="s">
-        <v>264</v>
-      </c>
-      <c r="D26" s="35" t="s">
-        <v>582</v>
-      </c>
-      <c r="E26" s="35" t="s">
-        <v>626</v>
-      </c>
-      <c r="F26" s="35" t="s">
-        <v>637</v>
-      </c>
-      <c r="G26" s="35" t="s">
-        <v>260</v>
-      </c>
-      <c r="H26" s="35" t="s">
-        <v>582</v>
-      </c>
-      <c r="I26" s="35" t="s">
-        <v>2</v>
-      </c>
-      <c r="J26" s="35" t="s">
-        <v>2</v>
-      </c>
-      <c r="K26" s="7" t="s">
-        <v>639</v>
-      </c>
-    </row>
-    <row r="27" spans="1:11" ht="15" customHeight="1">
+    <row r="27" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A27" s="32" t="s">
-        <v>267</v>
+        <v>280</v>
       </c>
       <c r="B27" s="35" t="s">
-        <v>268</v>
+        <v>281</v>
       </c>
       <c r="C27" s="39" t="s">
-        <v>273</v>
+        <v>287</v>
       </c>
       <c r="D27" s="35" t="s">
-        <v>576</v>
+        <v>584</v>
       </c>
       <c r="E27" s="35" t="s">
         <v>77</v>
       </c>
       <c r="F27" s="35" t="s">
-        <v>627</v>
+        <v>619</v>
       </c>
       <c r="G27" s="35" t="s">
-        <v>269</v>
+        <v>282</v>
       </c>
       <c r="H27" s="35" t="s">
         <v>567</v>
@@ -24904,95 +24926,93 @@
       <c r="J27" s="35" t="s">
         <v>2</v>
       </c>
-      <c r="K27" s="7" t="s">
-        <v>589</v>
-      </c>
+      <c r="K27" s="7"/>
     </row>
-    <row r="28" spans="1:11">
+    <row r="28" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A28" s="32" t="s">
-        <v>280</v>
+        <v>289</v>
       </c>
       <c r="B28" s="35" t="s">
-        <v>281</v>
+        <v>290</v>
       </c>
       <c r="C28" s="39" t="s">
-        <v>287</v>
+        <v>295</v>
       </c>
       <c r="D28" s="35" t="s">
-        <v>584</v>
+        <v>567</v>
       </c>
       <c r="E28" s="35" t="s">
-        <v>77</v>
+        <v>618</v>
       </c>
       <c r="F28" s="35" t="s">
-        <v>627</v>
+        <v>1</v>
       </c>
       <c r="G28" s="35" t="s">
-        <v>282</v>
+        <v>291</v>
       </c>
       <c r="H28" s="35" t="s">
-        <v>567</v>
-      </c>
-      <c r="I28" s="35" t="s">
-        <v>2</v>
-      </c>
+        <v>586</v>
+      </c>
+      <c r="I28" s="35"/>
       <c r="J28" s="35" t="s">
         <v>2</v>
       </c>
       <c r="K28" s="7"/>
     </row>
-    <row r="29" spans="1:11">
+    <row r="29" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A29" s="32" t="s">
-        <v>289</v>
+        <v>298</v>
       </c>
       <c r="B29" s="35" t="s">
-        <v>290</v>
+        <v>299</v>
       </c>
       <c r="C29" s="39" t="s">
-        <v>295</v>
+        <v>303</v>
       </c>
       <c r="D29" s="35" t="s">
         <v>567</v>
       </c>
       <c r="E29" s="35" t="s">
-        <v>626</v>
+        <v>617</v>
       </c>
       <c r="F29" s="35" t="s">
-        <v>1</v>
+        <v>622</v>
       </c>
       <c r="G29" s="35" t="s">
-        <v>291</v>
+        <v>300</v>
       </c>
       <c r="H29" s="35" t="s">
         <v>586</v>
       </c>
-      <c r="I29" s="35"/>
+      <c r="I29" s="35" t="s">
+        <v>2</v>
+      </c>
       <c r="J29" s="35" t="s">
         <v>2</v>
       </c>
       <c r="K29" s="7"/>
     </row>
-    <row r="30" spans="1:11">
+    <row r="30" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A30" s="32" t="s">
-        <v>298</v>
+        <v>608</v>
       </c>
       <c r="B30" s="35" t="s">
-        <v>299</v>
+        <v>314</v>
       </c>
       <c r="C30" s="39" t="s">
-        <v>303</v>
+        <v>318</v>
       </c>
       <c r="D30" s="35" t="s">
         <v>567</v>
       </c>
       <c r="E30" s="35" t="s">
-        <v>625</v>
+        <v>77</v>
       </c>
       <c r="F30" s="35" t="s">
-        <v>630</v>
+        <v>620</v>
       </c>
       <c r="G30" s="35" t="s">
-        <v>300</v>
+        <v>315</v>
       </c>
       <c r="H30" s="35" t="s">
         <v>586</v>
@@ -25005,30 +25025,30 @@
       </c>
       <c r="K30" s="7"/>
     </row>
-    <row r="31" spans="1:11">
+    <row r="31" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A31" s="32" t="s">
-        <v>616</v>
+        <v>320</v>
       </c>
       <c r="B31" s="35" t="s">
-        <v>314</v>
+        <v>321</v>
       </c>
       <c r="C31" s="39" t="s">
-        <v>318</v>
+        <v>328</v>
       </c>
       <c r="D31" s="35" t="s">
         <v>567</v>
       </c>
       <c r="E31" s="35" t="s">
-        <v>77</v>
+        <v>617</v>
       </c>
       <c r="F31" s="35" t="s">
-        <v>628</v>
+        <v>622</v>
       </c>
       <c r="G31" s="35" t="s">
-        <v>315</v>
+        <v>322</v>
       </c>
       <c r="H31" s="35" t="s">
-        <v>586</v>
+        <v>570</v>
       </c>
       <c r="I31" s="35" t="s">
         <v>2</v>
@@ -25038,60 +25058,58 @@
       </c>
       <c r="K31" s="7"/>
     </row>
-    <row r="32" spans="1:11">
+    <row r="32" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A32" s="32" t="s">
-        <v>320</v>
+        <v>334</v>
       </c>
       <c r="B32" s="35" t="s">
-        <v>321</v>
+        <v>336</v>
       </c>
       <c r="C32" s="39" t="s">
-        <v>328</v>
+        <v>341</v>
       </c>
       <c r="D32" s="35" t="s">
+        <v>586</v>
+      </c>
+      <c r="E32" s="35" t="s">
+        <v>277</v>
+      </c>
+      <c r="F32" s="35" t="s">
+        <v>624</v>
+      </c>
+      <c r="G32" s="35" t="s">
+        <v>337</v>
+      </c>
+      <c r="H32" s="35" t="s">
         <v>567</v>
       </c>
-      <c r="E32" s="35" t="s">
-        <v>625</v>
-      </c>
-      <c r="F32" s="35" t="s">
-        <v>630</v>
-      </c>
-      <c r="G32" s="35" t="s">
-        <v>322</v>
-      </c>
-      <c r="H32" s="35" t="s">
-        <v>570</v>
-      </c>
-      <c r="I32" s="35" t="s">
-        <v>2</v>
-      </c>
+      <c r="I32" s="35"/>
       <c r="J32" s="35" t="s">
         <v>2</v>
       </c>
       <c r="K32" s="7"/>
     </row>
-    <row r="33" spans="1:11">
+    <row r="33" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A33" s="32" t="s">
-        <v>334</v>
+        <v>344</v>
       </c>
       <c r="B33" s="35" t="s">
-        <v>336</v>
+        <v>347</v>
       </c>
       <c r="C33" s="39" t="s">
-        <v>341</v>
+        <v>354</v>
       </c>
       <c r="D33" s="35" t="s">
         <v>586</v>
       </c>
       <c r="E33" s="35" t="s">
-        <v>277</v>
+        <v>346</v>
       </c>
       <c r="F33" s="35" t="s">
-        <v>632</v>
+        <v>345</v>
       </c>
       <c r="G33" s="35" t="s">
-        <v>337</v>
+        <v>348</v>
       </c>
       <c r="H33" s="35" t="s">
         <v>567</v>
@@ -25102,125 +25120,125 @@
       </c>
       <c r="K33" s="7"/>
     </row>
-    <row r="34" spans="1:11">
+    <row r="34" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A34" s="32" t="s">
-        <v>344</v>
+        <v>365</v>
       </c>
       <c r="B34" s="35" t="s">
-        <v>347</v>
+        <v>368</v>
       </c>
       <c r="C34" s="39" t="s">
-        <v>354</v>
+        <v>373</v>
       </c>
       <c r="D34" s="35" t="s">
-        <v>586</v>
+        <v>570</v>
       </c>
       <c r="E34" s="35" t="s">
-        <v>346</v>
+        <v>618</v>
       </c>
       <c r="F34" s="35" t="s">
-        <v>345</v>
+        <v>1</v>
       </c>
       <c r="G34" s="35" t="s">
-        <v>348</v>
+        <v>369</v>
       </c>
       <c r="H34" s="35" t="s">
-        <v>567</v>
-      </c>
-      <c r="I34" s="35"/>
-      <c r="J34" s="35" t="s">
-        <v>2</v>
-      </c>
+        <v>590</v>
+      </c>
+      <c r="I34" s="35" t="s">
+        <v>2</v>
+      </c>
+      <c r="J34" s="35"/>
       <c r="K34" s="7"/>
     </row>
-    <row r="35" spans="1:11">
+    <row r="35" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A35" s="32" t="s">
-        <v>365</v>
+        <v>394</v>
       </c>
       <c r="B35" s="35" t="s">
-        <v>368</v>
+        <v>395</v>
       </c>
       <c r="C35" s="39" t="s">
-        <v>373</v>
+        <v>398</v>
       </c>
       <c r="D35" s="35" t="s">
-        <v>570</v>
+        <v>576</v>
       </c>
       <c r="E35" s="35" t="s">
-        <v>626</v>
+        <v>618</v>
       </c>
       <c r="F35" s="35" t="s">
         <v>1</v>
       </c>
       <c r="G35" s="35" t="s">
-        <v>369</v>
+        <v>396</v>
       </c>
       <c r="H35" s="35" t="s">
-        <v>590</v>
+        <v>570</v>
       </c>
       <c r="I35" s="35" t="s">
         <v>2</v>
       </c>
-      <c r="J35" s="35"/>
+      <c r="J35" s="35" t="s">
+        <v>2</v>
+      </c>
       <c r="K35" s="7"/>
     </row>
-    <row r="36" spans="1:11">
+    <row r="36" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A36" s="32" t="s">
-        <v>394</v>
+        <v>401</v>
       </c>
       <c r="B36" s="35" t="s">
-        <v>395</v>
+        <v>402</v>
       </c>
       <c r="C36" s="39" t="s">
-        <v>398</v>
+        <v>406</v>
       </c>
       <c r="D36" s="35" t="s">
-        <v>576</v>
+        <v>567</v>
       </c>
       <c r="E36" s="35" t="s">
-        <v>626</v>
+        <v>617</v>
       </c>
       <c r="F36" s="35" t="s">
-        <v>1</v>
+        <v>622</v>
       </c>
       <c r="G36" s="35" t="s">
-        <v>396</v>
+        <v>403</v>
       </c>
       <c r="H36" s="35" t="s">
-        <v>570</v>
-      </c>
-      <c r="I36" s="35" t="s">
-        <v>2</v>
-      </c>
+        <v>586</v>
+      </c>
+      <c r="I36" s="35"/>
       <c r="J36" s="35" t="s">
         <v>2</v>
       </c>
       <c r="K36" s="7"/>
     </row>
-    <row r="37" spans="1:11">
+    <row r="37" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A37" s="32" t="s">
-        <v>401</v>
+        <v>409</v>
       </c>
       <c r="B37" s="35" t="s">
-        <v>402</v>
+        <v>410</v>
       </c>
       <c r="C37" s="39" t="s">
-        <v>406</v>
+        <v>413</v>
       </c>
       <c r="D37" s="35" t="s">
         <v>567</v>
       </c>
       <c r="E37" s="35" t="s">
-        <v>625</v>
+        <v>77</v>
       </c>
       <c r="F37" s="35" t="s">
-        <v>630</v>
+        <v>619</v>
       </c>
       <c r="G37" s="35" t="s">
-        <v>403</v>
+        <v>411</v>
       </c>
       <c r="H37" s="35" t="s">
-        <v>586</v>
+        <v>570</v>
       </c>
       <c r="I37" s="35"/>
       <c r="J37" s="35" t="s">
@@ -25228,58 +25246,60 @@
       </c>
       <c r="K37" s="7"/>
     </row>
-    <row r="38" spans="1:11">
+    <row r="38" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A38" s="32" t="s">
-        <v>409</v>
+        <v>417</v>
       </c>
       <c r="B38" s="35" t="s">
-        <v>410</v>
+        <v>418</v>
       </c>
       <c r="C38" s="39" t="s">
-        <v>413</v>
+        <v>424</v>
       </c>
       <c r="D38" s="35" t="s">
+        <v>586</v>
+      </c>
+      <c r="E38" s="35" t="s">
+        <v>277</v>
+      </c>
+      <c r="F38" s="35" t="s">
+        <v>624</v>
+      </c>
+      <c r="G38" s="35" t="s">
+        <v>419</v>
+      </c>
+      <c r="H38" s="35" t="s">
         <v>567</v>
       </c>
-      <c r="E38" s="35" t="s">
-        <v>77</v>
-      </c>
-      <c r="F38" s="35" t="s">
-        <v>627</v>
-      </c>
-      <c r="G38" s="35" t="s">
-        <v>411</v>
-      </c>
-      <c r="H38" s="35" t="s">
-        <v>570</v>
-      </c>
-      <c r="I38" s="35"/>
+      <c r="I38" s="35" t="s">
+        <v>2</v>
+      </c>
       <c r="J38" s="35" t="s">
         <v>2</v>
       </c>
       <c r="K38" s="7"/>
     </row>
-    <row r="39" spans="1:11">
+    <row r="39" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A39" s="32" t="s">
-        <v>417</v>
+        <v>427</v>
       </c>
       <c r="B39" s="35" t="s">
-        <v>418</v>
+        <v>429</v>
       </c>
       <c r="C39" s="39" t="s">
-        <v>424</v>
+        <v>432</v>
       </c>
       <c r="D39" s="35" t="s">
-        <v>586</v>
+        <v>570</v>
       </c>
       <c r="E39" s="35" t="s">
-        <v>277</v>
+        <v>618</v>
       </c>
       <c r="F39" s="35" t="s">
-        <v>632</v>
+        <v>428</v>
       </c>
       <c r="G39" s="35" t="s">
-        <v>419</v>
+        <v>430</v>
       </c>
       <c r="H39" s="35" t="s">
         <v>567</v>
@@ -25292,73 +25312,73 @@
       </c>
       <c r="K39" s="7"/>
     </row>
-    <row r="40" spans="1:11" ht="15" customHeight="1">
+    <row r="40" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A40" s="32" t="s">
-        <v>427</v>
+        <v>435</v>
       </c>
       <c r="B40" s="35" t="s">
-        <v>429</v>
+        <v>437</v>
       </c>
       <c r="C40" s="39" t="s">
-        <v>432</v>
+        <v>442</v>
       </c>
       <c r="D40" s="35" t="s">
-        <v>570</v>
+        <v>582</v>
       </c>
       <c r="E40" s="35" t="s">
-        <v>626</v>
+        <v>77</v>
       </c>
       <c r="F40" s="35" t="s">
-        <v>428</v>
+        <v>620</v>
       </c>
       <c r="G40" s="35" t="s">
-        <v>430</v>
+        <v>438</v>
       </c>
       <c r="H40" s="35" t="s">
-        <v>567</v>
+        <v>582</v>
       </c>
       <c r="I40" s="35" t="s">
         <v>2</v>
       </c>
-      <c r="J40" s="35" t="s">
-        <v>2</v>
-      </c>
-      <c r="K40" s="7"/>
+      <c r="J40" s="35"/>
+      <c r="K40" s="7" t="s">
+        <v>591</v>
+      </c>
     </row>
-    <row r="41" spans="1:11">
+    <row r="41" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A41" s="32" t="s">
-        <v>435</v>
+        <v>444</v>
       </c>
       <c r="B41" s="35" t="s">
-        <v>437</v>
+        <v>446</v>
       </c>
       <c r="C41" s="39" t="s">
-        <v>442</v>
+        <v>447</v>
       </c>
       <c r="D41" s="35" t="s">
-        <v>582</v>
+        <v>595</v>
       </c>
       <c r="E41" s="35" t="s">
         <v>77</v>
       </c>
       <c r="F41" s="35" t="s">
-        <v>628</v>
+        <v>619</v>
       </c>
       <c r="G41" s="35" t="s">
-        <v>438</v>
+        <v>606</v>
       </c>
       <c r="H41" s="35" t="s">
-        <v>582</v>
+        <v>570</v>
       </c>
       <c r="I41" s="35" t="s">
         <v>2</v>
       </c>
-      <c r="J41" s="35"/>
-      <c r="K41" s="7" t="s">
-        <v>591</v>
-      </c>
+      <c r="J41" s="35" t="s">
+        <v>2</v>
+      </c>
+      <c r="K41" s="7"/>
     </row>
-    <row r="42" spans="1:11">
+    <row r="42" spans="1:12" ht="16" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A42" s="32" t="s">
         <v>444</v>
       </c>
@@ -25366,22 +25386,22 @@
         <v>446</v>
       </c>
       <c r="C42" s="39" t="s">
-        <v>450</v>
+        <v>603</v>
       </c>
       <c r="D42" s="35" t="s">
-        <v>596</v>
+        <v>567</v>
       </c>
       <c r="E42" s="35" t="s">
-        <v>77</v>
+        <v>277</v>
       </c>
       <c r="F42" s="35" t="s">
-        <v>627</v>
+        <v>621</v>
       </c>
       <c r="G42" s="35" t="s">
-        <v>468</v>
+        <v>604</v>
       </c>
       <c r="H42" s="35" t="s">
-        <v>597</v>
+        <v>593</v>
       </c>
       <c r="I42" s="35" t="s">
         <v>2</v>
@@ -25391,7 +25411,7 @@
       </c>
       <c r="K42" s="7"/>
     </row>
-    <row r="43" spans="1:11">
+    <row r="43" spans="1:12" ht="16" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A43" s="32" t="s">
         <v>444</v>
       </c>
@@ -25399,120 +25419,120 @@
         <v>446</v>
       </c>
       <c r="C43" s="39" t="s">
-        <v>447</v>
+        <v>455</v>
       </c>
       <c r="D43" s="35" t="s">
-        <v>595</v>
+        <v>596</v>
       </c>
       <c r="E43" s="35" t="s">
+        <v>617</v>
+      </c>
+      <c r="F43" s="35" t="s">
+        <v>622</v>
+      </c>
+      <c r="G43" s="35" t="s">
+        <v>605</v>
+      </c>
+      <c r="H43" s="35" t="s">
+        <v>590</v>
+      </c>
+      <c r="I43" s="35" t="s">
+        <v>2</v>
+      </c>
+      <c r="J43" s="35" t="s">
+        <v>2</v>
+      </c>
+      <c r="K43" s="7" t="s">
+        <v>594</v>
+      </c>
+    </row>
+    <row r="44" spans="1:12" s="40" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A44" s="41" t="s">
+        <v>475</v>
+      </c>
+      <c r="B44" s="42" t="s">
+        <v>476</v>
+      </c>
+      <c r="C44" s="43" t="s">
+        <v>477</v>
+      </c>
+      <c r="D44" s="42" t="s">
+        <v>567</v>
+      </c>
+      <c r="E44" s="42" t="s">
         <v>77</v>
       </c>
-      <c r="F43" s="35" t="s">
-        <v>627</v>
-      </c>
-      <c r="G43" s="35" t="s">
-        <v>608</v>
-      </c>
-      <c r="H43" s="35" t="s">
-        <v>570</v>
-      </c>
-      <c r="I43" s="35" t="s">
-        <v>2</v>
-      </c>
-      <c r="J43" s="35" t="s">
-        <v>2</v>
-      </c>
-      <c r="K43" s="7"/>
+      <c r="F44" s="42" t="s">
+        <v>619</v>
+      </c>
+      <c r="G44" s="43" t="s">
+        <v>633</v>
+      </c>
+      <c r="H44" s="42" t="s">
+        <v>586</v>
+      </c>
+      <c r="I44" s="42" t="s">
+        <v>2</v>
+      </c>
+      <c r="J44" s="42" t="s">
+        <v>2</v>
+      </c>
+      <c r="L44"/>
     </row>
-    <row r="44" spans="1:11" ht="16" customHeight="1">
-      <c r="A44" s="32" t="s">
-        <v>444</v>
-      </c>
-      <c r="B44" s="35" t="s">
-        <v>446</v>
-      </c>
-      <c r="C44" s="39" t="s">
-        <v>605</v>
-      </c>
-      <c r="D44" s="35" t="s">
+    <row r="45" spans="1:12" s="40" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A45" s="41" t="s">
+        <v>475</v>
+      </c>
+      <c r="B45" s="42" t="s">
+        <v>476</v>
+      </c>
+      <c r="C45" s="43" t="s">
+        <v>481</v>
+      </c>
+      <c r="D45" s="42" t="s">
         <v>567</v>
       </c>
-      <c r="E44" s="35" t="s">
-        <v>277</v>
-      </c>
-      <c r="F44" s="35" t="s">
-        <v>629</v>
-      </c>
-      <c r="G44" s="35" t="s">
-        <v>606</v>
-      </c>
-      <c r="H44" s="35" t="s">
-        <v>593</v>
-      </c>
-      <c r="I44" s="35" t="s">
-        <v>2</v>
-      </c>
-      <c r="J44" s="35" t="s">
-        <v>2</v>
-      </c>
-      <c r="K44" s="7"/>
+      <c r="E45" s="42" t="s">
+        <v>617</v>
+      </c>
+      <c r="F45" s="42" t="s">
+        <v>622</v>
+      </c>
+      <c r="G45" s="43" t="s">
+        <v>633</v>
+      </c>
+      <c r="H45" s="42" t="s">
+        <v>586</v>
+      </c>
+      <c r="I45" s="42" t="s">
+        <v>2</v>
+      </c>
+      <c r="J45" s="42" t="s">
+        <v>2</v>
+      </c>
+      <c r="L45"/>
     </row>
-    <row r="45" spans="1:11" ht="16" customHeight="1">
-      <c r="A45" s="32" t="s">
-        <v>444</v>
-      </c>
-      <c r="B45" s="35" t="s">
-        <v>446</v>
-      </c>
-      <c r="C45" s="39" t="s">
-        <v>455</v>
-      </c>
-      <c r="D45" s="35" t="s">
-        <v>598</v>
-      </c>
-      <c r="E45" s="35" t="s">
-        <v>625</v>
-      </c>
-      <c r="F45" s="35" t="s">
-        <v>630</v>
-      </c>
-      <c r="G45" s="35" t="s">
-        <v>607</v>
-      </c>
-      <c r="H45" s="35" t="s">
-        <v>590</v>
-      </c>
-      <c r="I45" s="35" t="s">
-        <v>2</v>
-      </c>
-      <c r="J45" s="35" t="s">
-        <v>2</v>
-      </c>
-      <c r="K45" s="7" t="s">
-        <v>594</v>
-      </c>
-    </row>
-    <row r="46" spans="1:11" ht="15" customHeight="1">
+    <row r="46" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A46" s="32" t="s">
-        <v>475</v>
+        <v>488</v>
       </c>
       <c r="B46" s="35" t="s">
-        <v>476</v>
+        <v>489</v>
       </c>
       <c r="C46" s="39" t="s">
-        <v>609</v>
+        <v>494</v>
       </c>
       <c r="D46" s="35" t="s">
-        <v>567</v>
+        <v>592</v>
       </c>
       <c r="E46" s="35" t="s">
         <v>77</v>
       </c>
       <c r="F46" s="35" t="s">
-        <v>627</v>
+        <v>619</v>
       </c>
       <c r="G46" s="35" t="s">
-        <v>481</v>
+        <v>504</v>
       </c>
       <c r="H46" s="35" t="s">
         <v>586</v>
@@ -25525,27 +25545,27 @@
       </c>
       <c r="K46" s="7"/>
     </row>
-    <row r="47" spans="1:11">
+    <row r="47" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A47" s="32" t="s">
-        <v>475</v>
+        <v>488</v>
       </c>
       <c r="B47" s="35" t="s">
-        <v>476</v>
+        <v>489</v>
       </c>
       <c r="C47" s="39" t="s">
-        <v>609</v>
+        <v>494</v>
       </c>
       <c r="D47" s="35" t="s">
         <v>567</v>
       </c>
       <c r="E47" s="35" t="s">
-        <v>625</v>
+        <v>277</v>
       </c>
       <c r="F47" s="35" t="s">
-        <v>630</v>
+        <v>621</v>
       </c>
       <c r="G47" s="35" t="s">
-        <v>610</v>
+        <v>490</v>
       </c>
       <c r="H47" s="35" t="s">
         <v>586</v>
@@ -25558,7 +25578,7 @@
       </c>
       <c r="K47" s="7"/>
     </row>
-    <row r="48" spans="1:11">
+    <row r="48" spans="1:12" ht="16" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A48" s="32" t="s">
         <v>488</v>
       </c>
@@ -25569,19 +25589,19 @@
         <v>494</v>
       </c>
       <c r="D48" s="35" t="s">
-        <v>592</v>
+        <v>567</v>
       </c>
       <c r="E48" s="35" t="s">
-        <v>77</v>
+        <v>617</v>
       </c>
       <c r="F48" s="35" t="s">
-        <v>627</v>
+        <v>622</v>
       </c>
       <c r="G48" s="35" t="s">
-        <v>504</v>
+        <v>497</v>
       </c>
       <c r="H48" s="35" t="s">
-        <v>586</v>
+        <v>570</v>
       </c>
       <c r="I48" s="35" t="s">
         <v>2</v>
@@ -25591,15 +25611,15 @@
       </c>
       <c r="K48" s="7"/>
     </row>
-    <row r="49" spans="1:11">
+    <row r="49" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A49" s="32" t="s">
-        <v>488</v>
+        <v>509</v>
       </c>
       <c r="B49" s="35" t="s">
-        <v>489</v>
+        <v>510</v>
       </c>
       <c r="C49" s="39" t="s">
-        <v>494</v>
+        <v>520</v>
       </c>
       <c r="D49" s="35" t="s">
         <v>567</v>
@@ -25608,13 +25628,13 @@
         <v>277</v>
       </c>
       <c r="F49" s="35" t="s">
-        <v>629</v>
+        <v>621</v>
       </c>
       <c r="G49" s="35" t="s">
-        <v>490</v>
+        <v>511</v>
       </c>
       <c r="H49" s="35" t="s">
-        <v>586</v>
+        <v>597</v>
       </c>
       <c r="I49" s="35" t="s">
         <v>2</v>
@@ -25624,115 +25644,49 @@
       </c>
       <c r="K49" s="7"/>
     </row>
-    <row r="50" spans="1:11" ht="16" customHeight="1">
+    <row r="50" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A50" s="32" t="s">
-        <v>488</v>
+        <v>257</v>
       </c>
       <c r="B50" s="35" t="s">
-        <v>489</v>
+        <v>259</v>
       </c>
       <c r="C50" s="39" t="s">
-        <v>494</v>
+        <v>264</v>
       </c>
       <c r="D50" s="35" t="s">
-        <v>567</v>
-      </c>
-      <c r="E50" s="35" t="s">
-        <v>625</v>
+        <v>582</v>
+      </c>
+      <c r="E50" s="7" t="s">
+        <v>77</v>
       </c>
       <c r="F50" s="35" t="s">
+        <v>628</v>
+      </c>
+      <c r="G50" s="13" t="s">
+        <v>627</v>
+      </c>
+      <c r="H50" s="35" t="s">
+        <v>582</v>
+      </c>
+      <c r="I50" s="35" t="s">
+        <v>2</v>
+      </c>
+      <c r="J50" s="35" t="s">
+        <v>2</v>
+      </c>
+      <c r="K50" s="7" t="s">
+        <v>631</v>
+      </c>
+    </row>
+    <row r="52" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A52" s="32" t="s">
         <v>630</v>
-      </c>
-      <c r="G50" s="35" t="s">
-        <v>497</v>
-      </c>
-      <c r="H50" s="35" t="s">
-        <v>570</v>
-      </c>
-      <c r="I50" s="35" t="s">
-        <v>2</v>
-      </c>
-      <c r="J50" s="35" t="s">
-        <v>2</v>
-      </c>
-      <c r="K50" s="7"/>
-    </row>
-    <row r="51" spans="1:11">
-      <c r="A51" s="32" t="s">
-        <v>509</v>
-      </c>
-      <c r="B51" s="35" t="s">
-        <v>510</v>
-      </c>
-      <c r="C51" s="39" t="s">
-        <v>520</v>
-      </c>
-      <c r="D51" s="35" t="s">
-        <v>567</v>
-      </c>
-      <c r="E51" s="35" t="s">
-        <v>277</v>
-      </c>
-      <c r="F51" s="35" t="s">
-        <v>629</v>
-      </c>
-      <c r="G51" s="35" t="s">
-        <v>511</v>
-      </c>
-      <c r="H51" s="35" t="s">
-        <v>599</v>
-      </c>
-      <c r="I51" s="35" t="s">
-        <v>2</v>
-      </c>
-      <c r="J51" s="35" t="s">
-        <v>2</v>
-      </c>
-      <c r="K51" s="7"/>
-    </row>
-    <row r="52" spans="1:11">
-      <c r="A52" s="32" t="s">
-        <v>257</v>
-      </c>
-      <c r="B52" s="35" t="s">
-        <v>259</v>
-      </c>
-      <c r="C52" s="39" t="s">
-        <v>264</v>
-      </c>
-      <c r="D52" s="35" t="s">
-        <v>582</v>
-      </c>
-      <c r="E52" s="7" t="s">
-        <v>77</v>
-      </c>
-      <c r="F52" s="35" t="s">
-        <v>636</v>
-      </c>
-      <c r="G52" s="13" t="s">
-        <v>635</v>
-      </c>
-      <c r="H52" s="35" t="s">
-        <v>582</v>
-      </c>
-      <c r="I52" s="35" t="s">
-        <v>2</v>
-      </c>
-      <c r="J52" s="35" t="s">
-        <v>2</v>
-      </c>
-      <c r="K52" s="7" t="s">
-        <v>639</v>
-      </c>
-    </row>
-    <row r="54" spans="1:11">
-      <c r="A54" s="32" t="s">
-        <v>638</v>
       </c>
     </row>
   </sheetData>
-  <sortState ref="A2:K51">
-    <sortCondition ref="A2:A51"/>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:K49">
+    <sortCondition ref="A2:A49"/>
   </sortState>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>

</xml_diff>

<commit_message>
Update table of functional isoforms
</commit_message>
<xml_diff>
--- a/ws/functional_isoforms/data/FunctionalTableLong.xlsx
+++ b/ws/functional_isoforms/data/FunctionalTableLong.xlsx
@@ -8,13 +8,14 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/mtress/Documents/mtress/Proteomics/GENCODE27/TissueSpecificity/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ECD28649-9E06-7C4E-876E-9453B61C7E6B}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3271C016-1540-9447-A625-63C61C303881}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2680" yWindow="460" windowWidth="24460" windowHeight="15360" tabRatio="500" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="2680" yWindow="460" windowWidth="24460" windowHeight="15360" tabRatio="500" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="FunctionalTableLong.txt" sheetId="1" r:id="rId1"/>
     <sheet name="Sheet1" sheetId="2" r:id="rId2"/>
+    <sheet name="For APPRIS" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="140001"/>
   <extLst>
@@ -26,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4553" uniqueCount="634">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4888" uniqueCount="637">
   <si>
     <t>ABI2</t>
   </si>
@@ -1928,13 +1929,22 @@
   </si>
   <si>
     <t>ENST00000329305</t>
+  </si>
+  <si>
+    <t>Main Transcript</t>
+  </si>
+  <si>
+    <t>Principal transcript most expressed in fat at RNA level</t>
+  </si>
+  <si>
+    <t>These transcripts differ by two events</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="22" x14ac:knownFonts="1">
+  <fonts count="22">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -2270,7 +2280,7 @@
     <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="44">
+  <cellXfs count="50">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
@@ -2315,6 +2325,12 @@
     <xf numFmtId="49" fontId="19" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="19" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="20" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="2" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="49" fontId="19" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="163">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
@@ -2822,7 +2838,7 @@
       <selection activeCell="R2" sqref="A1:AN195"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
   <cols>
     <col min="5" max="19" width="4.33203125" customWidth="1"/>
     <col min="20" max="27" width="4.6640625" customWidth="1"/>
@@ -2830,7 +2846,7 @@
     <col min="29" max="40" width="8" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:40" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:40">
       <c r="A1" t="s">
         <v>528</v>
       </c>
@@ -2952,7 +2968,7 @@
         <v>207</v>
       </c>
     </row>
-    <row r="2" spans="1:40" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:40">
       <c r="A2" s="1" t="s">
         <v>0</v>
       </c>
@@ -3059,7 +3075,7 @@
         <v>-0.39</v>
       </c>
     </row>
-    <row r="3" spans="1:40" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:40">
       <c r="A3" s="17" t="s">
         <v>0</v>
       </c>
@@ -3171,7 +3187,7 @@
         <v>-0.47</v>
       </c>
     </row>
-    <row r="4" spans="1:40" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:40">
       <c r="A4" s="1" t="s">
         <v>23</v>
       </c>
@@ -3266,7 +3282,7 @@
         <v>0.47</v>
       </c>
     </row>
-    <row r="5" spans="1:40" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:40">
       <c r="A5" s="17" t="s">
         <v>23</v>
       </c>
@@ -3370,7 +3386,7 @@
         <v>0.28000000000000003</v>
       </c>
     </row>
-    <row r="6" spans="1:40" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:40">
       <c r="A6" s="1" t="s">
         <v>38</v>
       </c>
@@ -3480,7 +3496,7 @@
         <v>-0.37</v>
       </c>
     </row>
-    <row r="7" spans="1:40" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:40">
       <c r="A7" s="17" t="s">
         <v>38</v>
       </c>
@@ -3594,7 +3610,7 @@
         <v>0.05</v>
       </c>
     </row>
-    <row r="8" spans="1:40" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:40">
       <c r="A8" s="1" t="s">
         <v>45</v>
       </c>
@@ -3698,7 +3714,7 @@
         <v>-0.54</v>
       </c>
     </row>
-    <row r="9" spans="1:40" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:40">
       <c r="A9" s="17" t="s">
         <v>45</v>
       </c>
@@ -3808,7 +3824,7 @@
         <v>0.05</v>
       </c>
     </row>
-    <row r="10" spans="1:40" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:40">
       <c r="A10" s="1" t="s">
         <v>54</v>
       </c>
@@ -3903,7 +3919,7 @@
         <v>-0.56999999999999995</v>
       </c>
     </row>
-    <row r="11" spans="1:40" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:40">
       <c r="A11" s="17" t="s">
         <v>54</v>
       </c>
@@ -4007,7 +4023,7 @@
         <v>-0.38</v>
       </c>
     </row>
-    <row r="12" spans="1:40" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:40">
       <c r="A12" s="1" t="s">
         <v>66</v>
       </c>
@@ -4117,7 +4133,7 @@
         <v>-0.45</v>
       </c>
     </row>
-    <row r="13" spans="1:40" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:40">
       <c r="A13" s="17" t="s">
         <v>66</v>
       </c>
@@ -4231,7 +4247,7 @@
         <v>-0.21</v>
       </c>
     </row>
-    <row r="14" spans="1:40" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:40">
       <c r="A14" s="1" t="s">
         <v>75</v>
       </c>
@@ -4338,7 +4354,7 @@
         <v>-0.34</v>
       </c>
     </row>
-    <row r="15" spans="1:40" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:40">
       <c r="A15" s="17" t="s">
         <v>75</v>
       </c>
@@ -4450,7 +4466,7 @@
         <v>-0.59</v>
       </c>
     </row>
-    <row r="16" spans="1:40" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:40">
       <c r="A16" s="1" t="s">
         <v>86</v>
       </c>
@@ -4554,7 +4570,7 @@
         <v>-0.8</v>
       </c>
     </row>
-    <row r="17" spans="1:40" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:40">
       <c r="A17" s="17" t="s">
         <v>86</v>
       </c>
@@ -4664,7 +4680,7 @@
         <v>-0.01</v>
       </c>
     </row>
-    <row r="18" spans="1:40" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:40">
       <c r="A18" s="1" t="s">
         <v>95</v>
       </c>
@@ -4768,7 +4784,7 @@
         <v>-0.46</v>
       </c>
     </row>
-    <row r="19" spans="1:40" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:40">
       <c r="A19" s="17" t="s">
         <v>95</v>
       </c>
@@ -4878,7 +4894,7 @@
         <v>-7.0000000000000007E-2</v>
       </c>
     </row>
-    <row r="20" spans="1:40" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:40">
       <c r="A20" s="17" t="s">
         <v>95</v>
       </c>
@@ -4988,7 +5004,7 @@
         <v>-0.11</v>
       </c>
     </row>
-    <row r="21" spans="1:40" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:40">
       <c r="A21" s="17" t="s">
         <v>95</v>
       </c>
@@ -5098,7 +5114,7 @@
         <v>-0.11</v>
       </c>
     </row>
-    <row r="22" spans="1:40" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:40">
       <c r="A22" s="1" t="s">
         <v>107</v>
       </c>
@@ -5208,7 +5224,7 @@
         <v>-7.0000000000000007E-2</v>
       </c>
     </row>
-    <row r="23" spans="1:40" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:40">
       <c r="A23" s="17" t="s">
         <v>107</v>
       </c>
@@ -5322,7 +5338,7 @@
         <v>0.34</v>
       </c>
     </row>
-    <row r="24" spans="1:40" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:40">
       <c r="A24" s="1" t="s">
         <v>118</v>
       </c>
@@ -5435,7 +5451,7 @@
         <v>-7.0000000000000007E-2</v>
       </c>
     </row>
-    <row r="25" spans="1:40" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:40">
       <c r="A25" s="17" t="s">
         <v>118</v>
       </c>
@@ -5551,7 +5567,7 @@
         <v>0.37</v>
       </c>
     </row>
-    <row r="26" spans="1:40" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:40">
       <c r="A26" s="1" t="s">
         <v>127</v>
       </c>
@@ -5661,7 +5677,7 @@
         <v>-0.34</v>
       </c>
     </row>
-    <row r="27" spans="1:40" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:40">
       <c r="A27" s="17" t="s">
         <v>127</v>
       </c>
@@ -5775,7 +5791,7 @@
         <v>0.1</v>
       </c>
     </row>
-    <row r="28" spans="1:40" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:40">
       <c r="A28" s="1" t="s">
         <v>132</v>
       </c>
@@ -5882,7 +5898,7 @@
         <v>0.2</v>
       </c>
     </row>
-    <row r="29" spans="1:40" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:40">
       <c r="A29" s="17" t="s">
         <v>132</v>
       </c>
@@ -5994,7 +6010,7 @@
         <v>-0.67</v>
       </c>
     </row>
-    <row r="30" spans="1:40" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:40" ht="15" customHeight="1">
       <c r="A30" s="9" t="s">
         <v>557</v>
       </c>
@@ -6096,7 +6112,7 @@
         <v>0.17326656590216999</v>
       </c>
     </row>
-    <row r="31" spans="1:40" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:40">
       <c r="A31" s="19" t="s">
         <v>557</v>
       </c>
@@ -6202,7 +6218,7 @@
         <v>-0.32657694903582901</v>
       </c>
     </row>
-    <row r="32" spans="1:40" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:40">
       <c r="A32" s="1" t="s">
         <v>143</v>
       </c>
@@ -6306,7 +6322,7 @@
         <v>-0.47</v>
       </c>
     </row>
-    <row r="33" spans="1:40" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:40">
       <c r="A33" s="17" t="s">
         <v>143</v>
       </c>
@@ -6416,7 +6432,7 @@
         <v>-0.21</v>
       </c>
     </row>
-    <row r="34" spans="1:40" x14ac:dyDescent="0.2">
+    <row r="34" spans="1:40">
       <c r="A34" s="17" t="s">
         <v>143</v>
       </c>
@@ -6526,7 +6542,7 @@
         <v>-0.21</v>
       </c>
     </row>
-    <row r="35" spans="1:40" x14ac:dyDescent="0.2">
+    <row r="35" spans="1:40">
       <c r="A35" s="17" t="s">
         <v>143</v>
       </c>
@@ -6636,7 +6652,7 @@
         <v>-0.21</v>
       </c>
     </row>
-    <row r="36" spans="1:40" x14ac:dyDescent="0.2">
+    <row r="36" spans="1:40">
       <c r="A36" s="17" t="s">
         <v>143</v>
       </c>
@@ -6746,7 +6762,7 @@
         <v>-0.21</v>
       </c>
     </row>
-    <row r="37" spans="1:40" x14ac:dyDescent="0.2">
+    <row r="37" spans="1:40">
       <c r="A37" s="1" t="s">
         <v>154</v>
       </c>
@@ -6856,7 +6872,7 @@
         <v>-0.56999999999999995</v>
       </c>
     </row>
-    <row r="38" spans="1:40" x14ac:dyDescent="0.2">
+    <row r="38" spans="1:40">
       <c r="A38" s="17" t="s">
         <v>154</v>
       </c>
@@ -6970,7 +6986,7 @@
         <v>-0.5</v>
       </c>
     </row>
-    <row r="39" spans="1:40" x14ac:dyDescent="0.2">
+    <row r="39" spans="1:40">
       <c r="A39" s="1" t="s">
         <v>162</v>
       </c>
@@ -7056,7 +7072,7 @@
         <v>0.64</v>
       </c>
     </row>
-    <row r="40" spans="1:40" x14ac:dyDescent="0.2">
+    <row r="40" spans="1:40">
       <c r="A40" s="1" t="s">
         <v>162</v>
       </c>
@@ -7142,7 +7158,7 @@
         <v>0.64</v>
       </c>
     </row>
-    <row r="41" spans="1:40" x14ac:dyDescent="0.2">
+    <row r="41" spans="1:40">
       <c r="A41" s="1" t="s">
         <v>162</v>
       </c>
@@ -7228,7 +7244,7 @@
         <v>0.64</v>
       </c>
     </row>
-    <row r="42" spans="1:40" x14ac:dyDescent="0.2">
+    <row r="42" spans="1:40">
       <c r="A42" s="1" t="s">
         <v>162</v>
       </c>
@@ -7314,7 +7330,7 @@
         <v>0.64</v>
       </c>
     </row>
-    <row r="43" spans="1:40" x14ac:dyDescent="0.2">
+    <row r="43" spans="1:40">
       <c r="A43" s="1" t="s">
         <v>162</v>
       </c>
@@ -7400,7 +7416,7 @@
         <v>0.64</v>
       </c>
     </row>
-    <row r="44" spans="1:40" x14ac:dyDescent="0.2">
+    <row r="44" spans="1:40">
       <c r="A44" s="17" t="s">
         <v>162</v>
       </c>
@@ -7498,7 +7514,7 @@
         <v>1.03</v>
       </c>
     </row>
-    <row r="45" spans="1:40" x14ac:dyDescent="0.2">
+    <row r="45" spans="1:40">
       <c r="A45" s="17" t="s">
         <v>162</v>
       </c>
@@ -7596,7 +7612,7 @@
         <v>1.03</v>
       </c>
     </row>
-    <row r="46" spans="1:40" x14ac:dyDescent="0.2">
+    <row r="46" spans="1:40">
       <c r="A46" s="17" t="s">
         <v>162</v>
       </c>
@@ -7694,7 +7710,7 @@
         <v>1.07</v>
       </c>
     </row>
-    <row r="47" spans="1:40" x14ac:dyDescent="0.2">
+    <row r="47" spans="1:40">
       <c r="A47" s="17" t="s">
         <v>162</v>
       </c>
@@ -7792,7 +7808,7 @@
         <v>0.81</v>
       </c>
     </row>
-    <row r="48" spans="1:40" x14ac:dyDescent="0.2">
+    <row r="48" spans="1:40">
       <c r="A48" s="17" t="s">
         <v>162</v>
       </c>
@@ -7890,7 +7906,7 @@
         <v>0.81</v>
       </c>
     </row>
-    <row r="49" spans="1:40" x14ac:dyDescent="0.2">
+    <row r="49" spans="1:40">
       <c r="A49" s="17" t="s">
         <v>162</v>
       </c>
@@ -7988,7 +8004,7 @@
         <v>1.4</v>
       </c>
     </row>
-    <row r="50" spans="1:40" x14ac:dyDescent="0.2">
+    <row r="50" spans="1:40">
       <c r="A50" s="17" t="s">
         <v>162</v>
       </c>
@@ -8086,7 +8102,7 @@
         <v>1.4</v>
       </c>
     </row>
-    <row r="51" spans="1:40" x14ac:dyDescent="0.2">
+    <row r="51" spans="1:40">
       <c r="A51" s="17" t="s">
         <v>162</v>
       </c>
@@ -8184,7 +8200,7 @@
         <v>1.4</v>
       </c>
     </row>
-    <row r="52" spans="1:40" x14ac:dyDescent="0.2">
+    <row r="52" spans="1:40">
       <c r="A52" s="17" t="s">
         <v>162</v>
       </c>
@@ -8282,7 +8298,7 @@
         <v>1.3</v>
       </c>
     </row>
-    <row r="53" spans="1:40" x14ac:dyDescent="0.2">
+    <row r="53" spans="1:40">
       <c r="A53" s="17" t="s">
         <v>162</v>
       </c>
@@ -8380,7 +8396,7 @@
         <v>0.81</v>
       </c>
     </row>
-    <row r="54" spans="1:40" x14ac:dyDescent="0.2">
+    <row r="54" spans="1:40">
       <c r="A54" s="1" t="s">
         <v>185</v>
       </c>
@@ -8484,7 +8500,7 @@
         <v>-0.39</v>
       </c>
     </row>
-    <row r="55" spans="1:40" x14ac:dyDescent="0.2">
+    <row r="55" spans="1:40">
       <c r="A55" s="17" t="s">
         <v>185</v>
       </c>
@@ -8594,7 +8610,7 @@
         <v>-0.21</v>
       </c>
     </row>
-    <row r="56" spans="1:40" x14ac:dyDescent="0.2">
+    <row r="56" spans="1:40">
       <c r="A56" s="1" t="s">
         <v>194</v>
       </c>
@@ -8701,7 +8717,7 @@
         <v>-0.5</v>
       </c>
     </row>
-    <row r="57" spans="1:40" x14ac:dyDescent="0.2">
+    <row r="57" spans="1:40">
       <c r="A57" s="1" t="s">
         <v>194</v>
       </c>
@@ -8808,7 +8824,7 @@
         <v>-0.5</v>
       </c>
     </row>
-    <row r="58" spans="1:40" x14ac:dyDescent="0.2">
+    <row r="58" spans="1:40">
       <c r="A58" s="1" t="s">
         <v>194</v>
       </c>
@@ -8915,7 +8931,7 @@
         <v>-0.5</v>
       </c>
     </row>
-    <row r="59" spans="1:40" x14ac:dyDescent="0.2">
+    <row r="59" spans="1:40">
       <c r="A59" s="17" t="s">
         <v>194</v>
       </c>
@@ -9027,7 +9043,7 @@
         <v>2.58</v>
       </c>
     </row>
-    <row r="60" spans="1:40" x14ac:dyDescent="0.2">
+    <row r="60" spans="1:40">
       <c r="A60" s="17" t="s">
         <v>194</v>
       </c>
@@ -9139,7 +9155,7 @@
         <v>2.71</v>
       </c>
     </row>
-    <row r="61" spans="1:40" x14ac:dyDescent="0.2">
+    <row r="61" spans="1:40">
       <c r="A61" s="17" t="s">
         <v>194</v>
       </c>
@@ -9251,7 +9267,7 @@
         <v>2.61</v>
       </c>
     </row>
-    <row r="62" spans="1:40" x14ac:dyDescent="0.2">
+    <row r="62" spans="1:40">
       <c r="A62" s="17" t="s">
         <v>194</v>
       </c>
@@ -9363,7 +9379,7 @@
         <v>2.57</v>
       </c>
     </row>
-    <row r="63" spans="1:40" x14ac:dyDescent="0.2">
+    <row r="63" spans="1:40">
       <c r="A63" s="17" t="s">
         <v>194</v>
       </c>
@@ -9475,7 +9491,7 @@
         <v>2.71</v>
       </c>
     </row>
-    <row r="64" spans="1:40" x14ac:dyDescent="0.2">
+    <row r="64" spans="1:40">
       <c r="A64" s="1" t="s">
         <v>212</v>
       </c>
@@ -9570,7 +9586,7 @@
         <v>-0.49</v>
       </c>
     </row>
-    <row r="65" spans="1:40" x14ac:dyDescent="0.2">
+    <row r="65" spans="1:40">
       <c r="A65" s="1" t="s">
         <v>212</v>
       </c>
@@ -9665,7 +9681,7 @@
         <v>-0.49</v>
       </c>
     </row>
-    <row r="66" spans="1:40" x14ac:dyDescent="0.2">
+    <row r="66" spans="1:40">
       <c r="A66" s="17" t="s">
         <v>212</v>
       </c>
@@ -9769,7 +9785,7 @@
         <v>-0.27</v>
       </c>
     </row>
-    <row r="67" spans="1:40" x14ac:dyDescent="0.2">
+    <row r="67" spans="1:40">
       <c r="A67" s="17" t="s">
         <v>212</v>
       </c>
@@ -9873,7 +9889,7 @@
         <v>-0.27</v>
       </c>
     </row>
-    <row r="68" spans="1:40" x14ac:dyDescent="0.2">
+    <row r="68" spans="1:40">
       <c r="A68" s="1" t="s">
         <v>222</v>
       </c>
@@ -9977,7 +9993,7 @@
         <v>-0.2</v>
       </c>
     </row>
-    <row r="69" spans="1:40" x14ac:dyDescent="0.2">
+    <row r="69" spans="1:40">
       <c r="A69" s="17" t="s">
         <v>222</v>
       </c>
@@ -10087,7 +10103,7 @@
         <v>0.3</v>
       </c>
     </row>
-    <row r="70" spans="1:40" x14ac:dyDescent="0.2">
+    <row r="70" spans="1:40">
       <c r="A70" s="17" t="s">
         <v>222</v>
       </c>
@@ -10197,7 +10213,7 @@
         <v>0.36</v>
       </c>
     </row>
-    <row r="71" spans="1:40" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="71" spans="1:40" ht="15" customHeight="1">
       <c r="A71" s="17" t="s">
         <v>222</v>
       </c>
@@ -10307,7 +10323,7 @@
         <v>0.36</v>
       </c>
     </row>
-    <row r="72" spans="1:40" x14ac:dyDescent="0.2">
+    <row r="72" spans="1:40">
       <c r="A72" s="1" t="s">
         <v>234</v>
       </c>
@@ -10417,7 +10433,7 @@
         <v>-0.66</v>
       </c>
     </row>
-    <row r="73" spans="1:40" x14ac:dyDescent="0.2">
+    <row r="73" spans="1:40">
       <c r="A73" s="17" t="s">
         <v>234</v>
       </c>
@@ -10531,7 +10547,7 @@
         <v>-0.31</v>
       </c>
     </row>
-    <row r="74" spans="1:40" x14ac:dyDescent="0.2">
+    <row r="74" spans="1:40">
       <c r="A74" s="1" t="s">
         <v>245</v>
       </c>
@@ -10647,7 +10663,7 @@
         <v>-0.61</v>
       </c>
     </row>
-    <row r="75" spans="1:40" x14ac:dyDescent="0.2">
+    <row r="75" spans="1:40">
       <c r="A75" s="17" t="s">
         <v>245</v>
       </c>
@@ -10765,7 +10781,7 @@
         <v>1.07</v>
       </c>
     </row>
-    <row r="76" spans="1:40" x14ac:dyDescent="0.2">
+    <row r="76" spans="1:40">
       <c r="A76" s="1" t="s">
         <v>257</v>
       </c>
@@ -10860,7 +10876,7 @@
         <v>0.08</v>
       </c>
     </row>
-    <row r="77" spans="1:40" x14ac:dyDescent="0.2">
+    <row r="77" spans="1:40">
       <c r="A77" s="17" t="s">
         <v>257</v>
       </c>
@@ -10964,7 +10980,7 @@
         <v>0.15</v>
       </c>
     </row>
-    <row r="78" spans="1:40" x14ac:dyDescent="0.2">
+    <row r="78" spans="1:40">
       <c r="A78" s="1" t="s">
         <v>267</v>
       </c>
@@ -11059,7 +11075,7 @@
         <v>-0.34</v>
       </c>
     </row>
-    <row r="79" spans="1:40" x14ac:dyDescent="0.2">
+    <row r="79" spans="1:40">
       <c r="A79" s="17" t="s">
         <v>267</v>
       </c>
@@ -11163,7 +11179,7 @@
         <v>-0.23</v>
       </c>
     </row>
-    <row r="80" spans="1:40" x14ac:dyDescent="0.2">
+    <row r="80" spans="1:40">
       <c r="A80" s="1" t="s">
         <v>280</v>
       </c>
@@ -11273,7 +11289,7 @@
         <v>-0.5</v>
       </c>
     </row>
-    <row r="81" spans="1:40" x14ac:dyDescent="0.2">
+    <row r="81" spans="1:40">
       <c r="A81" s="1" t="s">
         <v>280</v>
       </c>
@@ -11383,7 +11399,7 @@
         <v>-0.5</v>
       </c>
     </row>
-    <row r="82" spans="1:40" x14ac:dyDescent="0.2">
+    <row r="82" spans="1:40">
       <c r="A82" s="17" t="s">
         <v>280</v>
       </c>
@@ -11497,7 +11513,7 @@
         <v>-0.06</v>
       </c>
     </row>
-    <row r="83" spans="1:40" x14ac:dyDescent="0.2">
+    <row r="83" spans="1:40">
       <c r="A83" s="1" t="s">
         <v>289</v>
       </c>
@@ -11607,7 +11623,7 @@
         <v>-0.27</v>
       </c>
     </row>
-    <row r="84" spans="1:40" x14ac:dyDescent="0.2">
+    <row r="84" spans="1:40">
       <c r="A84" s="17" t="s">
         <v>289</v>
       </c>
@@ -11721,7 +11737,7 @@
         <v>1.46</v>
       </c>
     </row>
-    <row r="85" spans="1:40" x14ac:dyDescent="0.2">
+    <row r="85" spans="1:40">
       <c r="A85" s="17" t="s">
         <v>289</v>
       </c>
@@ -11835,7 +11851,7 @@
         <v>1.46</v>
       </c>
     </row>
-    <row r="86" spans="1:40" x14ac:dyDescent="0.2">
+    <row r="86" spans="1:40">
       <c r="A86" s="1" t="s">
         <v>298</v>
       </c>
@@ -11942,7 +11958,7 @@
         <v>1.61</v>
       </c>
     </row>
-    <row r="87" spans="1:40" x14ac:dyDescent="0.2">
+    <row r="87" spans="1:40">
       <c r="A87" s="17" t="s">
         <v>298</v>
       </c>
@@ -12054,7 +12070,7 @@
         <v>1.17</v>
       </c>
     </row>
-    <row r="88" spans="1:40" x14ac:dyDescent="0.2">
+    <row r="88" spans="1:40">
       <c r="A88" s="17" t="s">
         <v>298</v>
       </c>
@@ -12166,7 +12182,7 @@
         <v>1.17</v>
       </c>
     </row>
-    <row r="89" spans="1:40" x14ac:dyDescent="0.2">
+    <row r="89" spans="1:40">
       <c r="A89" s="17" t="s">
         <v>298</v>
       </c>
@@ -12278,7 +12294,7 @@
         <v>1.31</v>
       </c>
     </row>
-    <row r="90" spans="1:40" x14ac:dyDescent="0.2">
+    <row r="90" spans="1:40">
       <c r="A90" s="17" t="s">
         <v>298</v>
       </c>
@@ -12390,7 +12406,7 @@
         <v>0.94</v>
       </c>
     </row>
-    <row r="91" spans="1:40" x14ac:dyDescent="0.2">
+    <row r="91" spans="1:40">
       <c r="A91" s="17" t="s">
         <v>298</v>
       </c>
@@ -12502,7 +12518,7 @@
         <v>0.94</v>
       </c>
     </row>
-    <row r="92" spans="1:40" x14ac:dyDescent="0.2">
+    <row r="92" spans="1:40">
       <c r="A92" s="17" t="s">
         <v>298</v>
       </c>
@@ -12614,7 +12630,7 @@
         <v>1.17</v>
       </c>
     </row>
-    <row r="93" spans="1:40" x14ac:dyDescent="0.2">
+    <row r="93" spans="1:40">
       <c r="A93" s="17" t="s">
         <v>298</v>
       </c>
@@ -12726,7 +12742,7 @@
         <v>1.17</v>
       </c>
     </row>
-    <row r="94" spans="1:40" x14ac:dyDescent="0.2">
+    <row r="94" spans="1:40">
       <c r="A94" s="17" t="s">
         <v>298</v>
       </c>
@@ -12838,7 +12854,7 @@
         <v>1.17</v>
       </c>
     </row>
-    <row r="95" spans="1:40" x14ac:dyDescent="0.2">
+    <row r="95" spans="1:40">
       <c r="A95" s="1" t="s">
         <v>312</v>
       </c>
@@ -12948,7 +12964,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="96" spans="1:40" x14ac:dyDescent="0.2">
+    <row r="96" spans="1:40">
       <c r="A96" s="17" t="s">
         <v>312</v>
       </c>
@@ -13062,7 +13078,7 @@
         <v>-0.45</v>
       </c>
     </row>
-    <row r="97" spans="1:40" x14ac:dyDescent="0.2">
+    <row r="97" spans="1:40">
       <c r="A97" s="1" t="s">
         <v>320</v>
       </c>
@@ -13169,7 +13185,7 @@
         <v>-0.21</v>
       </c>
     </row>
-    <row r="98" spans="1:40" x14ac:dyDescent="0.2">
+    <row r="98" spans="1:40">
       <c r="A98" s="1" t="s">
         <v>320</v>
       </c>
@@ -13276,7 +13292,7 @@
         <v>-0.21</v>
       </c>
     </row>
-    <row r="99" spans="1:40" x14ac:dyDescent="0.2">
+    <row r="99" spans="1:40">
       <c r="A99" s="1" t="s">
         <v>320</v>
       </c>
@@ -13383,7 +13399,7 @@
         <v>-0.21</v>
       </c>
     </row>
-    <row r="100" spans="1:40" x14ac:dyDescent="0.2">
+    <row r="100" spans="1:40">
       <c r="A100" s="1" t="s">
         <v>320</v>
       </c>
@@ -13490,7 +13506,7 @@
         <v>-0.21</v>
       </c>
     </row>
-    <row r="101" spans="1:40" x14ac:dyDescent="0.2">
+    <row r="101" spans="1:40">
       <c r="A101" s="17" t="s">
         <v>320</v>
       </c>
@@ -13602,7 +13618,7 @@
         <v>0.54</v>
       </c>
     </row>
-    <row r="102" spans="1:40" x14ac:dyDescent="0.2">
+    <row r="102" spans="1:40">
       <c r="A102" s="17" t="s">
         <v>320</v>
       </c>
@@ -13714,7 +13730,7 @@
         <v>0.54</v>
       </c>
     </row>
-    <row r="103" spans="1:40" x14ac:dyDescent="0.2">
+    <row r="103" spans="1:40">
       <c r="A103" s="17" t="s">
         <v>320</v>
       </c>
@@ -13826,7 +13842,7 @@
         <v>0.54</v>
       </c>
     </row>
-    <row r="104" spans="1:40" x14ac:dyDescent="0.2">
+    <row r="104" spans="1:40">
       <c r="A104" s="17" t="s">
         <v>320</v>
       </c>
@@ -13938,7 +13954,7 @@
         <v>0.54</v>
       </c>
     </row>
-    <row r="105" spans="1:40" x14ac:dyDescent="0.2">
+    <row r="105" spans="1:40">
       <c r="A105" s="17" t="s">
         <v>320</v>
       </c>
@@ -14050,7 +14066,7 @@
         <v>0.54</v>
       </c>
     </row>
-    <row r="106" spans="1:40" x14ac:dyDescent="0.2">
+    <row r="106" spans="1:40">
       <c r="A106" s="1" t="s">
         <v>334</v>
       </c>
@@ -14157,7 +14173,7 @@
         <v>0.2</v>
       </c>
     </row>
-    <row r="107" spans="1:40" x14ac:dyDescent="0.2">
+    <row r="107" spans="1:40">
       <c r="A107" s="17" t="s">
         <v>334</v>
       </c>
@@ -14269,7 +14285,7 @@
         <v>0.24</v>
       </c>
     </row>
-    <row r="108" spans="1:40" x14ac:dyDescent="0.2">
+    <row r="108" spans="1:40">
       <c r="A108" s="1" t="s">
         <v>344</v>
       </c>
@@ -14373,7 +14389,7 @@
         <v>-0.11</v>
       </c>
     </row>
-    <row r="109" spans="1:40" x14ac:dyDescent="0.2">
+    <row r="109" spans="1:40">
       <c r="A109" s="1" t="s">
         <v>344</v>
       </c>
@@ -14477,7 +14493,7 @@
         <v>0.17</v>
       </c>
     </row>
-    <row r="110" spans="1:40" x14ac:dyDescent="0.2">
+    <row r="110" spans="1:40">
       <c r="A110" s="1" t="s">
         <v>344</v>
       </c>
@@ -14581,7 +14597,7 @@
         <v>0.17</v>
       </c>
     </row>
-    <row r="111" spans="1:40" x14ac:dyDescent="0.2">
+    <row r="111" spans="1:40">
       <c r="A111" s="17" t="s">
         <v>344</v>
       </c>
@@ -14691,7 +14707,7 @@
         <v>-0.46</v>
       </c>
     </row>
-    <row r="112" spans="1:40" x14ac:dyDescent="0.2">
+    <row r="112" spans="1:40">
       <c r="A112" s="17" t="s">
         <v>344</v>
       </c>
@@ -14801,7 +14817,7 @@
         <v>-0.36</v>
       </c>
     </row>
-    <row r="113" spans="1:40" x14ac:dyDescent="0.2">
+    <row r="113" spans="1:40">
       <c r="A113" s="17" t="s">
         <v>344</v>
       </c>
@@ -14911,7 +14927,7 @@
         <v>-0.36</v>
       </c>
     </row>
-    <row r="114" spans="1:40" x14ac:dyDescent="0.2">
+    <row r="114" spans="1:40">
       <c r="A114" s="17" t="s">
         <v>344</v>
       </c>
@@ -15021,7 +15037,7 @@
         <v>-0.53</v>
       </c>
     </row>
-    <row r="115" spans="1:40" x14ac:dyDescent="0.2">
+    <row r="115" spans="1:40">
       <c r="A115" s="17" t="s">
         <v>344</v>
       </c>
@@ -15131,7 +15147,7 @@
         <v>-0.46</v>
       </c>
     </row>
-    <row r="116" spans="1:40" x14ac:dyDescent="0.2">
+    <row r="116" spans="1:40">
       <c r="A116" s="17" t="s">
         <v>344</v>
       </c>
@@ -15241,7 +15257,7 @@
         <v>-0.47</v>
       </c>
     </row>
-    <row r="117" spans="1:40" x14ac:dyDescent="0.2">
+    <row r="117" spans="1:40">
       <c r="A117" s="17" t="s">
         <v>344</v>
       </c>
@@ -15351,7 +15367,7 @@
         <v>-0.4</v>
       </c>
     </row>
-    <row r="118" spans="1:40" x14ac:dyDescent="0.2">
+    <row r="118" spans="1:40">
       <c r="A118" s="17" t="s">
         <v>344</v>
       </c>
@@ -15461,7 +15477,7 @@
         <v>-0.42</v>
       </c>
     </row>
-    <row r="119" spans="1:40" x14ac:dyDescent="0.2">
+    <row r="119" spans="1:40">
       <c r="A119" s="17" t="s">
         <v>344</v>
       </c>
@@ -15571,7 +15587,7 @@
         <v>-0.28999999999999998</v>
       </c>
     </row>
-    <row r="120" spans="1:40" x14ac:dyDescent="0.2">
+    <row r="120" spans="1:40">
       <c r="A120" s="1" t="s">
         <v>365</v>
       </c>
@@ -15687,7 +15703,7 @@
         <v>-0.16</v>
       </c>
     </row>
-    <row r="121" spans="1:40" x14ac:dyDescent="0.2">
+    <row r="121" spans="1:40">
       <c r="A121" s="17" t="s">
         <v>365</v>
       </c>
@@ -15805,7 +15821,7 @@
         <v>-0.41</v>
       </c>
     </row>
-    <row r="122" spans="1:40" x14ac:dyDescent="0.2">
+    <row r="122" spans="1:40">
       <c r="A122" s="17" t="s">
         <v>365</v>
       </c>
@@ -15923,7 +15939,7 @@
         <v>-0.41</v>
       </c>
     </row>
-    <row r="123" spans="1:40" x14ac:dyDescent="0.2">
+    <row r="123" spans="1:40">
       <c r="A123" s="17" t="s">
         <v>365</v>
       </c>
@@ -16041,7 +16057,7 @@
         <v>-0.41</v>
       </c>
     </row>
-    <row r="124" spans="1:40" x14ac:dyDescent="0.2">
+    <row r="124" spans="1:40">
       <c r="A124" s="17" t="s">
         <v>365</v>
       </c>
@@ -16159,7 +16175,7 @@
         <v>-0.41</v>
       </c>
     </row>
-    <row r="125" spans="1:40" x14ac:dyDescent="0.2">
+    <row r="125" spans="1:40">
       <c r="A125" s="17" t="s">
         <v>365</v>
       </c>
@@ -16277,7 +16293,7 @@
         <v>-0.41</v>
       </c>
     </row>
-    <row r="126" spans="1:40" x14ac:dyDescent="0.2">
+    <row r="126" spans="1:40">
       <c r="A126" s="17" t="s">
         <v>365</v>
       </c>
@@ -16395,7 +16411,7 @@
         <v>-0.41</v>
       </c>
     </row>
-    <row r="127" spans="1:40" x14ac:dyDescent="0.2">
+    <row r="127" spans="1:40">
       <c r="A127" s="17" t="s">
         <v>365</v>
       </c>
@@ -16513,7 +16529,7 @@
         <v>-0.41</v>
       </c>
     </row>
-    <row r="128" spans="1:40" x14ac:dyDescent="0.2">
+    <row r="128" spans="1:40">
       <c r="A128" s="17" t="s">
         <v>365</v>
       </c>
@@ -16631,7 +16647,7 @@
         <v>-0.41</v>
       </c>
     </row>
-    <row r="129" spans="1:40" x14ac:dyDescent="0.2">
+    <row r="129" spans="1:40">
       <c r="A129" s="17" t="s">
         <v>365</v>
       </c>
@@ -16749,7 +16765,7 @@
         <v>-0.34</v>
       </c>
     </row>
-    <row r="130" spans="1:40" x14ac:dyDescent="0.2">
+    <row r="130" spans="1:40">
       <c r="A130" s="17" t="s">
         <v>365</v>
       </c>
@@ -16867,7 +16883,7 @@
         <v>-0.41</v>
       </c>
     </row>
-    <row r="131" spans="1:40" x14ac:dyDescent="0.2">
+    <row r="131" spans="1:40">
       <c r="A131" s="17" t="s">
         <v>365</v>
       </c>
@@ -16985,7 +17001,7 @@
         <v>-0.41</v>
       </c>
     </row>
-    <row r="132" spans="1:40" x14ac:dyDescent="0.2">
+    <row r="132" spans="1:40">
       <c r="A132" s="17" t="s">
         <v>365</v>
       </c>
@@ -17103,7 +17119,7 @@
         <v>-0.41</v>
       </c>
     </row>
-    <row r="133" spans="1:40" x14ac:dyDescent="0.2">
+    <row r="133" spans="1:40">
       <c r="A133" s="17" t="s">
         <v>365</v>
       </c>
@@ -17221,7 +17237,7 @@
         <v>-0.41</v>
       </c>
     </row>
-    <row r="134" spans="1:40" x14ac:dyDescent="0.2">
+    <row r="134" spans="1:40">
       <c r="A134" s="17" t="s">
         <v>365</v>
       </c>
@@ -17339,7 +17355,7 @@
         <v>-0.41</v>
       </c>
     </row>
-    <row r="135" spans="1:40" x14ac:dyDescent="0.2">
+    <row r="135" spans="1:40">
       <c r="A135" s="17" t="s">
         <v>365</v>
       </c>
@@ -17457,7 +17473,7 @@
         <v>-0.41</v>
       </c>
     </row>
-    <row r="136" spans="1:40" x14ac:dyDescent="0.2">
+    <row r="136" spans="1:40">
       <c r="A136" s="17" t="s">
         <v>365</v>
       </c>
@@ -17575,7 +17591,7 @@
         <v>-0.41</v>
       </c>
     </row>
-    <row r="137" spans="1:40" x14ac:dyDescent="0.2">
+    <row r="137" spans="1:40">
       <c r="A137" s="17" t="s">
         <v>365</v>
       </c>
@@ -17693,7 +17709,7 @@
         <v>-0.41</v>
       </c>
     </row>
-    <row r="138" spans="1:40" x14ac:dyDescent="0.2">
+    <row r="138" spans="1:40">
       <c r="A138" s="17" t="s">
         <v>365</v>
       </c>
@@ -17811,7 +17827,7 @@
         <v>-0.41</v>
       </c>
     </row>
-    <row r="139" spans="1:40" x14ac:dyDescent="0.2">
+    <row r="139" spans="1:40">
       <c r="A139" s="17" t="s">
         <v>365</v>
       </c>
@@ -17929,7 +17945,7 @@
         <v>-0.41</v>
       </c>
     </row>
-    <row r="140" spans="1:40" x14ac:dyDescent="0.2">
+    <row r="140" spans="1:40">
       <c r="A140" s="17" t="s">
         <v>365</v>
       </c>
@@ -18047,7 +18063,7 @@
         <v>-0.41</v>
       </c>
     </row>
-    <row r="141" spans="1:40" x14ac:dyDescent="0.2">
+    <row r="141" spans="1:40">
       <c r="A141" s="17" t="s">
         <v>365</v>
       </c>
@@ -18165,7 +18181,7 @@
         <v>-0.41</v>
       </c>
     </row>
-    <row r="142" spans="1:40" x14ac:dyDescent="0.2">
+    <row r="142" spans="1:40">
       <c r="A142" s="17" t="s">
         <v>365</v>
       </c>
@@ -18283,7 +18299,7 @@
         <v>-0.41</v>
       </c>
     </row>
-    <row r="143" spans="1:40" x14ac:dyDescent="0.2">
+    <row r="143" spans="1:40">
       <c r="A143" s="17" t="s">
         <v>365</v>
       </c>
@@ -18401,7 +18417,7 @@
         <v>-0.39</v>
       </c>
     </row>
-    <row r="144" spans="1:40" x14ac:dyDescent="0.2">
+    <row r="144" spans="1:40">
       <c r="A144" s="17" t="s">
         <v>365</v>
       </c>
@@ -18519,7 +18535,7 @@
         <v>-0.41</v>
       </c>
     </row>
-    <row r="145" spans="1:40" x14ac:dyDescent="0.2">
+    <row r="145" spans="1:40">
       <c r="A145" s="17" t="s">
         <v>365</v>
       </c>
@@ -18637,7 +18653,7 @@
         <v>-0.41</v>
       </c>
     </row>
-    <row r="146" spans="1:40" x14ac:dyDescent="0.2">
+    <row r="146" spans="1:40">
       <c r="A146" s="17" t="s">
         <v>365</v>
       </c>
@@ -18755,7 +18771,7 @@
         <v>-0.41</v>
       </c>
     </row>
-    <row r="147" spans="1:40" x14ac:dyDescent="0.2">
+    <row r="147" spans="1:40">
       <c r="A147" s="17" t="s">
         <v>365</v>
       </c>
@@ -18873,7 +18889,7 @@
         <v>-0.41</v>
       </c>
     </row>
-    <row r="148" spans="1:40" x14ac:dyDescent="0.2">
+    <row r="148" spans="1:40">
       <c r="A148" s="17" t="s">
         <v>365</v>
       </c>
@@ -18991,7 +19007,7 @@
         <v>-0.41</v>
       </c>
     </row>
-    <row r="149" spans="1:40" x14ac:dyDescent="0.2">
+    <row r="149" spans="1:40">
       <c r="A149" s="1" t="s">
         <v>393</v>
       </c>
@@ -19098,7 +19114,7 @@
         <v>-0.22</v>
       </c>
     </row>
-    <row r="150" spans="1:40" x14ac:dyDescent="0.2">
+    <row r="150" spans="1:40">
       <c r="A150" s="17" t="s">
         <v>393</v>
       </c>
@@ -19210,7 +19226,7 @@
         <v>-0.19</v>
       </c>
     </row>
-    <row r="151" spans="1:40" x14ac:dyDescent="0.2">
+    <row r="151" spans="1:40">
       <c r="A151" s="1" t="s">
         <v>401</v>
       </c>
@@ -19311,7 +19327,7 @@
         <v>0.06</v>
       </c>
     </row>
-    <row r="152" spans="1:40" x14ac:dyDescent="0.2">
+    <row r="152" spans="1:40">
       <c r="A152" s="17" t="s">
         <v>401</v>
       </c>
@@ -19419,7 +19435,7 @@
         <v>0.01</v>
       </c>
     </row>
-    <row r="153" spans="1:40" x14ac:dyDescent="0.2">
+    <row r="153" spans="1:40">
       <c r="A153" s="1" t="s">
         <v>409</v>
       </c>
@@ -19520,7 +19536,7 @@
         <v>-0.31</v>
       </c>
     </row>
-    <row r="154" spans="1:40" x14ac:dyDescent="0.2">
+    <row r="154" spans="1:40">
       <c r="A154" s="17" t="s">
         <v>409</v>
       </c>
@@ -19628,7 +19644,7 @@
         <v>-0.7</v>
       </c>
     </row>
-    <row r="155" spans="1:40" x14ac:dyDescent="0.2">
+    <row r="155" spans="1:40">
       <c r="A155" s="17" t="s">
         <v>409</v>
       </c>
@@ -19736,7 +19752,7 @@
         <v>-0.7</v>
       </c>
     </row>
-    <row r="156" spans="1:40" x14ac:dyDescent="0.2">
+    <row r="156" spans="1:40">
       <c r="A156" s="1" t="s">
         <v>417</v>
       </c>
@@ -19846,7 +19862,7 @@
         <v>0.31</v>
       </c>
     </row>
-    <row r="157" spans="1:40" x14ac:dyDescent="0.2">
+    <row r="157" spans="1:40">
       <c r="A157" s="17" t="s">
         <v>417</v>
       </c>
@@ -19960,7 +19976,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="158" spans="1:40" x14ac:dyDescent="0.2">
+    <row r="158" spans="1:40">
       <c r="A158" s="1" t="s">
         <v>427</v>
       </c>
@@ -20064,7 +20080,7 @@
         <v>-0.63</v>
       </c>
     </row>
-    <row r="159" spans="1:40" x14ac:dyDescent="0.2">
+    <row r="159" spans="1:40">
       <c r="A159" s="17" t="s">
         <v>427</v>
       </c>
@@ -20174,7 +20190,7 @@
         <v>-0.55000000000000004</v>
       </c>
     </row>
-    <row r="160" spans="1:40" x14ac:dyDescent="0.2">
+    <row r="160" spans="1:40">
       <c r="A160" s="1" t="s">
         <v>435</v>
       </c>
@@ -20272,7 +20288,7 @@
         <v>-0.59</v>
       </c>
     </row>
-    <row r="161" spans="1:40" x14ac:dyDescent="0.2">
+    <row r="161" spans="1:40">
       <c r="A161" s="17" t="s">
         <v>435</v>
       </c>
@@ -20378,7 +20394,7 @@
         <v>-0.39</v>
       </c>
     </row>
-    <row r="162" spans="1:40" x14ac:dyDescent="0.2">
+    <row r="162" spans="1:40">
       <c r="A162" s="1" t="s">
         <v>444</v>
       </c>
@@ -20476,7 +20492,7 @@
         <v>0.08</v>
       </c>
     </row>
-    <row r="163" spans="1:40" x14ac:dyDescent="0.2">
+    <row r="163" spans="1:40">
       <c r="A163" s="17" t="s">
         <v>444</v>
       </c>
@@ -20582,7 +20598,7 @@
         <v>0.49</v>
       </c>
     </row>
-    <row r="164" spans="1:40" x14ac:dyDescent="0.2">
+    <row r="164" spans="1:40">
       <c r="A164" s="1" t="s">
         <v>453</v>
       </c>
@@ -20683,7 +20699,7 @@
         <v>-0.26</v>
       </c>
     </row>
-    <row r="165" spans="1:40" x14ac:dyDescent="0.2">
+    <row r="165" spans="1:40">
       <c r="A165" s="17" t="s">
         <v>453</v>
       </c>
@@ -20791,7 +20807,7 @@
         <v>0.49</v>
       </c>
     </row>
-    <row r="166" spans="1:40" x14ac:dyDescent="0.2">
+    <row r="166" spans="1:40">
       <c r="A166" s="1" t="s">
         <v>460</v>
       </c>
@@ -20892,7 +20908,7 @@
         <v>-0.1</v>
       </c>
     </row>
-    <row r="167" spans="1:40" x14ac:dyDescent="0.2">
+    <row r="167" spans="1:40">
       <c r="A167" s="17" t="s">
         <v>460</v>
       </c>
@@ -21000,7 +21016,7 @@
         <v>-0.09</v>
       </c>
     </row>
-    <row r="168" spans="1:40" x14ac:dyDescent="0.2">
+    <row r="168" spans="1:40">
       <c r="A168" s="1" t="s">
         <v>467</v>
       </c>
@@ -21107,7 +21123,7 @@
         <v>-0.22</v>
       </c>
     </row>
-    <row r="169" spans="1:40" x14ac:dyDescent="0.2">
+    <row r="169" spans="1:40">
       <c r="A169" s="17" t="s">
         <v>467</v>
       </c>
@@ -21219,7 +21235,7 @@
         <v>0.08</v>
       </c>
     </row>
-    <row r="170" spans="1:40" x14ac:dyDescent="0.2">
+    <row r="170" spans="1:40">
       <c r="A170" s="1" t="s">
         <v>473</v>
       </c>
@@ -21329,7 +21345,7 @@
         <v>-0.22</v>
       </c>
     </row>
-    <row r="171" spans="1:40" x14ac:dyDescent="0.2">
+    <row r="171" spans="1:40">
       <c r="A171" s="17" t="s">
         <v>473</v>
       </c>
@@ -21443,7 +21459,7 @@
         <v>0.08</v>
       </c>
     </row>
-    <row r="172" spans="1:40" x14ac:dyDescent="0.2">
+    <row r="172" spans="1:40">
       <c r="A172" s="1" t="s">
         <v>475</v>
       </c>
@@ -21547,7 +21563,7 @@
         <v>2.69</v>
       </c>
     </row>
-    <row r="173" spans="1:40" x14ac:dyDescent="0.2">
+    <row r="173" spans="1:40">
       <c r="A173" s="17" t="s">
         <v>475</v>
       </c>
@@ -21657,7 +21673,7 @@
         <v>-7.0000000000000007E-2</v>
       </c>
     </row>
-    <row r="174" spans="1:40" x14ac:dyDescent="0.2">
+    <row r="174" spans="1:40">
       <c r="A174" s="1" t="s">
         <v>484</v>
       </c>
@@ -21761,7 +21777,7 @@
         <v>2.71</v>
       </c>
     </row>
-    <row r="175" spans="1:40" x14ac:dyDescent="0.2">
+    <row r="175" spans="1:40">
       <c r="A175" s="17" t="s">
         <v>484</v>
       </c>
@@ -21871,7 +21887,7 @@
         <v>-0.1</v>
       </c>
     </row>
-    <row r="176" spans="1:40" x14ac:dyDescent="0.2">
+    <row r="176" spans="1:40">
       <c r="A176" s="1" t="s">
         <v>488</v>
       </c>
@@ -21978,7 +21994,7 @@
         <v>2.0099999999999998</v>
       </c>
     </row>
-    <row r="177" spans="1:40" x14ac:dyDescent="0.2">
+    <row r="177" spans="1:40">
       <c r="A177" s="17" t="s">
         <v>488</v>
       </c>
@@ -22090,7 +22106,7 @@
         <v>-0.45</v>
       </c>
     </row>
-    <row r="178" spans="1:40" x14ac:dyDescent="0.2">
+    <row r="178" spans="1:40">
       <c r="A178" s="1" t="s">
         <v>496</v>
       </c>
@@ -22194,7 +22210,7 @@
         <v>2.4900000000000002</v>
       </c>
     </row>
-    <row r="179" spans="1:40" x14ac:dyDescent="0.2">
+    <row r="179" spans="1:40">
       <c r="A179" s="17" t="s">
         <v>496</v>
       </c>
@@ -22304,7 +22320,7 @@
         <v>-0.4</v>
       </c>
     </row>
-    <row r="180" spans="1:40" x14ac:dyDescent="0.2">
+    <row r="180" spans="1:40">
       <c r="A180" s="1" t="s">
         <v>503</v>
       </c>
@@ -22411,7 +22427,7 @@
         <v>2.64</v>
       </c>
     </row>
-    <row r="181" spans="1:40" x14ac:dyDescent="0.2">
+    <row r="181" spans="1:40">
       <c r="A181" s="17" t="s">
         <v>503</v>
       </c>
@@ -22523,7 +22539,7 @@
         <v>-0.46</v>
       </c>
     </row>
-    <row r="182" spans="1:40" x14ac:dyDescent="0.2">
+    <row r="182" spans="1:40">
       <c r="A182" s="1" t="s">
         <v>509</v>
       </c>
@@ -22624,7 +22640,7 @@
         <v>1.06</v>
       </c>
     </row>
-    <row r="183" spans="1:40" x14ac:dyDescent="0.2">
+    <row r="183" spans="1:40">
       <c r="A183" s="1" t="s">
         <v>509</v>
       </c>
@@ -22725,7 +22741,7 @@
         <v>1.06</v>
       </c>
     </row>
-    <row r="184" spans="1:40" x14ac:dyDescent="0.2">
+    <row r="184" spans="1:40">
       <c r="A184" s="1" t="s">
         <v>509</v>
       </c>
@@ -22826,7 +22842,7 @@
         <v>1.06</v>
       </c>
     </row>
-    <row r="185" spans="1:40" x14ac:dyDescent="0.2">
+    <row r="185" spans="1:40">
       <c r="A185" s="1" t="s">
         <v>509</v>
       </c>
@@ -22927,7 +22943,7 @@
         <v>1.06</v>
       </c>
     </row>
-    <row r="186" spans="1:40" x14ac:dyDescent="0.2">
+    <row r="186" spans="1:40">
       <c r="A186" s="1" t="s">
         <v>509</v>
       </c>
@@ -23028,7 +23044,7 @@
         <v>1.06</v>
       </c>
     </row>
-    <row r="187" spans="1:40" x14ac:dyDescent="0.2">
+    <row r="187" spans="1:40">
       <c r="A187" s="1" t="s">
         <v>509</v>
       </c>
@@ -23129,7 +23145,7 @@
         <v>1.25</v>
       </c>
     </row>
-    <row r="188" spans="1:40" x14ac:dyDescent="0.2">
+    <row r="188" spans="1:40">
       <c r="A188" s="17" t="s">
         <v>509</v>
       </c>
@@ -23237,7 +23253,7 @@
         <v>-0.32</v>
       </c>
     </row>
-    <row r="189" spans="1:40" x14ac:dyDescent="0.2">
+    <row r="189" spans="1:40">
       <c r="A189" s="17" t="s">
         <v>509</v>
       </c>
@@ -23345,7 +23361,7 @@
         <v>-0.32</v>
       </c>
     </row>
-    <row r="190" spans="1:40" x14ac:dyDescent="0.2">
+    <row r="190" spans="1:40">
       <c r="A190" s="17" t="s">
         <v>509</v>
       </c>
@@ -23453,7 +23469,7 @@
         <v>-0.32</v>
       </c>
     </row>
-    <row r="191" spans="1:40" x14ac:dyDescent="0.2">
+    <row r="191" spans="1:40">
       <c r="A191" s="17" t="s">
         <v>509</v>
       </c>
@@ -23561,7 +23577,7 @@
         <v>-0.32</v>
       </c>
     </row>
-    <row r="192" spans="1:40" x14ac:dyDescent="0.2">
+    <row r="192" spans="1:40">
       <c r="A192" s="17" t="s">
         <v>509</v>
       </c>
@@ -23669,7 +23685,7 @@
         <v>-0.32</v>
       </c>
     </row>
-    <row r="193" spans="1:40" x14ac:dyDescent="0.2">
+    <row r="193" spans="1:40">
       <c r="A193" s="17" t="s">
         <v>509</v>
       </c>
@@ -23777,7 +23793,7 @@
         <v>-0.32</v>
       </c>
     </row>
-    <row r="194" spans="1:40" ht="16" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="194" spans="1:40" ht="16" customHeight="1">
       <c r="A194" s="17" t="s">
         <v>509</v>
       </c>
@@ -23885,7 +23901,7 @@
         <v>-0.32</v>
       </c>
     </row>
-    <row r="195" spans="1:40" x14ac:dyDescent="0.2">
+    <row r="195" spans="1:40">
       <c r="A195" s="17" t="s">
         <v>509</v>
       </c>
@@ -24011,11 +24027,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:L52"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="92" zoomScaleNormal="92" workbookViewId="0">
-      <selection activeCell="G34" sqref="G34"/>
+    <sheetView topLeftCell="A13" zoomScale="92" zoomScaleNormal="92" workbookViewId="0">
+      <selection activeCell="K24" sqref="A1:L50"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
   <cols>
     <col min="2" max="2" width="6.1640625" customWidth="1"/>
     <col min="3" max="3" width="17.1640625" customWidth="1"/>
@@ -24026,7 +24042,7 @@
     <col min="16" max="16" width="4" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" s="31" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:12" s="31" customFormat="1">
       <c r="A1" s="33" t="s">
         <v>607</v>
       </c>
@@ -24064,7 +24080,7 @@
         <v>632</v>
       </c>
     </row>
-    <row r="2" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:12">
       <c r="A2" s="32" t="s">
         <v>0</v>
       </c>
@@ -24099,7 +24115,7 @@
         <v>568</v>
       </c>
     </row>
-    <row r="3" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:12">
       <c r="A3" s="32" t="s">
         <v>23</v>
       </c>
@@ -24130,7 +24146,7 @@
       </c>
       <c r="K3" s="7"/>
     </row>
-    <row r="4" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:12">
       <c r="A4" s="32" t="s">
         <v>38</v>
       </c>
@@ -24163,7 +24179,7 @@
       </c>
       <c r="K4" s="7"/>
     </row>
-    <row r="5" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:12">
       <c r="A5" s="32" t="s">
         <v>38</v>
       </c>
@@ -24198,7 +24214,7 @@
         <v>573</v>
       </c>
     </row>
-    <row r="6" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:12">
       <c r="A6" s="32" t="s">
         <v>54</v>
       </c>
@@ -24231,7 +24247,7 @@
         <v>574</v>
       </c>
     </row>
-    <row r="7" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:12">
       <c r="A7" s="32" t="s">
         <v>66</v>
       </c>
@@ -24262,7 +24278,7 @@
       </c>
       <c r="K7" s="7"/>
     </row>
-    <row r="8" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:12">
       <c r="A8" s="32" t="s">
         <v>75</v>
       </c>
@@ -24295,7 +24311,7 @@
         <v>578</v>
       </c>
     </row>
-    <row r="9" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:12">
       <c r="A9" s="32" t="s">
         <v>86</v>
       </c>
@@ -24330,7 +24346,7 @@
         <v>579</v>
       </c>
     </row>
-    <row r="10" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:12">
       <c r="A10" s="32" t="s">
         <v>95</v>
       </c>
@@ -24361,7 +24377,7 @@
       </c>
       <c r="K10" s="7"/>
     </row>
-    <row r="11" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:12">
       <c r="A11" s="32" t="s">
         <v>107</v>
       </c>
@@ -24396,7 +24412,7 @@
         <v>580</v>
       </c>
     </row>
-    <row r="12" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:12">
       <c r="A12" s="32" t="s">
         <v>118</v>
       </c>
@@ -24429,7 +24445,7 @@
       </c>
       <c r="K12" s="7"/>
     </row>
-    <row r="13" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:12" ht="15" customHeight="1">
       <c r="A13" s="32" t="s">
         <v>118</v>
       </c>
@@ -24462,7 +24478,7 @@
       </c>
       <c r="K13" s="7"/>
     </row>
-    <row r="14" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:12">
       <c r="A14" s="32" t="s">
         <v>132</v>
       </c>
@@ -24495,7 +24511,7 @@
       </c>
       <c r="K14" s="7"/>
     </row>
-    <row r="15" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:12" ht="15" customHeight="1">
       <c r="A15" s="32" t="s">
         <v>143</v>
       </c>
@@ -24528,7 +24544,7 @@
       </c>
       <c r="K15" s="7"/>
     </row>
-    <row r="16" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:12">
       <c r="A16" s="32" t="s">
         <v>598</v>
       </c>
@@ -24561,7 +24577,7 @@
       </c>
       <c r="K16" s="7"/>
     </row>
-    <row r="17" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:11">
       <c r="A17" s="32" t="s">
         <v>609</v>
       </c>
@@ -24594,7 +24610,7 @@
       </c>
       <c r="K17" s="7"/>
     </row>
-    <row r="18" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:11">
       <c r="A18" s="32" t="s">
         <v>162</v>
       </c>
@@ -24627,7 +24643,7 @@
         <v>583</v>
       </c>
     </row>
-    <row r="19" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:11">
       <c r="A19" s="32" t="s">
         <v>185</v>
       </c>
@@ -24660,7 +24676,7 @@
       </c>
       <c r="K19" s="7"/>
     </row>
-    <row r="20" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:11">
       <c r="A20" s="32" t="s">
         <v>194</v>
       </c>
@@ -24691,7 +24707,7 @@
       </c>
       <c r="K20" s="7"/>
     </row>
-    <row r="21" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:11">
       <c r="A21" s="32" t="s">
         <v>212</v>
       </c>
@@ -24724,7 +24740,7 @@
         <v>585</v>
       </c>
     </row>
-    <row r="22" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:11">
       <c r="A22" s="32" t="s">
         <v>222</v>
       </c>
@@ -24757,7 +24773,7 @@
         <v>587</v>
       </c>
     </row>
-    <row r="23" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:11">
       <c r="A23" s="32" t="s">
         <v>234</v>
       </c>
@@ -24790,7 +24806,7 @@
       </c>
       <c r="K23" s="7"/>
     </row>
-    <row r="24" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:11">
       <c r="A24" s="32" t="s">
         <v>245</v>
       </c>
@@ -24825,7 +24841,7 @@
         <v>588</v>
       </c>
     </row>
-    <row r="25" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:11">
       <c r="A25" s="32" t="s">
         <v>257</v>
       </c>
@@ -24860,7 +24876,7 @@
         <v>631</v>
       </c>
     </row>
-    <row r="26" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:11" ht="15" customHeight="1">
       <c r="A26" s="32" t="s">
         <v>267</v>
       </c>
@@ -24895,7 +24911,7 @@
         <v>589</v>
       </c>
     </row>
-    <row r="27" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:11">
       <c r="A27" s="32" t="s">
         <v>280</v>
       </c>
@@ -24928,7 +24944,7 @@
       </c>
       <c r="K27" s="7"/>
     </row>
-    <row r="28" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:11">
       <c r="A28" s="32" t="s">
         <v>289</v>
       </c>
@@ -24959,7 +24975,7 @@
       </c>
       <c r="K28" s="7"/>
     </row>
-    <row r="29" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:11">
       <c r="A29" s="32" t="s">
         <v>298</v>
       </c>
@@ -24992,7 +25008,7 @@
       </c>
       <c r="K29" s="7"/>
     </row>
-    <row r="30" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:11">
       <c r="A30" s="32" t="s">
         <v>608</v>
       </c>
@@ -25025,7 +25041,7 @@
       </c>
       <c r="K30" s="7"/>
     </row>
-    <row r="31" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:11">
       <c r="A31" s="32" t="s">
         <v>320</v>
       </c>
@@ -25058,7 +25074,7 @@
       </c>
       <c r="K31" s="7"/>
     </row>
-    <row r="32" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:11">
       <c r="A32" s="32" t="s">
         <v>334</v>
       </c>
@@ -25089,7 +25105,7 @@
       </c>
       <c r="K32" s="7"/>
     </row>
-    <row r="33" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:12">
       <c r="A33" s="32" t="s">
         <v>344</v>
       </c>
@@ -25120,7 +25136,7 @@
       </c>
       <c r="K33" s="7"/>
     </row>
-    <row r="34" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="34" spans="1:12">
       <c r="A34" s="32" t="s">
         <v>365</v>
       </c>
@@ -25151,7 +25167,7 @@
       <c r="J34" s="35"/>
       <c r="K34" s="7"/>
     </row>
-    <row r="35" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="35" spans="1:12">
       <c r="A35" s="32" t="s">
         <v>394</v>
       </c>
@@ -25184,7 +25200,7 @@
       </c>
       <c r="K35" s="7"/>
     </row>
-    <row r="36" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="36" spans="1:12">
       <c r="A36" s="32" t="s">
         <v>401</v>
       </c>
@@ -25215,7 +25231,7 @@
       </c>
       <c r="K36" s="7"/>
     </row>
-    <row r="37" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="37" spans="1:12">
       <c r="A37" s="32" t="s">
         <v>409</v>
       </c>
@@ -25246,7 +25262,7 @@
       </c>
       <c r="K37" s="7"/>
     </row>
-    <row r="38" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="38" spans="1:12">
       <c r="A38" s="32" t="s">
         <v>417</v>
       </c>
@@ -25279,7 +25295,7 @@
       </c>
       <c r="K38" s="7"/>
     </row>
-    <row r="39" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="39" spans="1:12" ht="15" customHeight="1">
       <c r="A39" s="32" t="s">
         <v>427</v>
       </c>
@@ -25312,7 +25328,7 @@
       </c>
       <c r="K39" s="7"/>
     </row>
-    <row r="40" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="40" spans="1:12">
       <c r="A40" s="32" t="s">
         <v>435</v>
       </c>
@@ -25345,7 +25361,7 @@
         <v>591</v>
       </c>
     </row>
-    <row r="41" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="41" spans="1:12">
       <c r="A41" s="32" t="s">
         <v>444</v>
       </c>
@@ -25378,7 +25394,7 @@
       </c>
       <c r="K41" s="7"/>
     </row>
-    <row r="42" spans="1:12" ht="16" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="42" spans="1:12" ht="16" customHeight="1">
       <c r="A42" s="32" t="s">
         <v>444</v>
       </c>
@@ -25411,7 +25427,7 @@
       </c>
       <c r="K42" s="7"/>
     </row>
-    <row r="43" spans="1:12" ht="16" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="43" spans="1:12" ht="16" customHeight="1">
       <c r="A43" s="32" t="s">
         <v>444</v>
       </c>
@@ -25446,7 +25462,7 @@
         <v>594</v>
       </c>
     </row>
-    <row r="44" spans="1:12" s="40" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="44" spans="1:12" s="40" customFormat="1" ht="15" customHeight="1">
       <c r="A44" s="41" t="s">
         <v>475</v>
       </c>
@@ -25479,7 +25495,7 @@
       </c>
       <c r="L44"/>
     </row>
-    <row r="45" spans="1:12" s="40" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="45" spans="1:12" s="40" customFormat="1">
       <c r="A45" s="41" t="s">
         <v>475</v>
       </c>
@@ -25512,7 +25528,7 @@
       </c>
       <c r="L45"/>
     </row>
-    <row r="46" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="46" spans="1:12">
       <c r="A46" s="32" t="s">
         <v>488</v>
       </c>
@@ -25545,7 +25561,7 @@
       </c>
       <c r="K46" s="7"/>
     </row>
-    <row r="47" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="47" spans="1:12">
       <c r="A47" s="32" t="s">
         <v>488</v>
       </c>
@@ -25578,7 +25594,7 @@
       </c>
       <c r="K47" s="7"/>
     </row>
-    <row r="48" spans="1:12" ht="16" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="48" spans="1:12" ht="16" customHeight="1">
       <c r="A48" s="32" t="s">
         <v>488</v>
       </c>
@@ -25611,7 +25627,7 @@
       </c>
       <c r="K48" s="7"/>
     </row>
-    <row r="49" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="49" spans="1:11">
       <c r="A49" s="32" t="s">
         <v>509</v>
       </c>
@@ -25644,7 +25660,7 @@
       </c>
       <c r="K49" s="7"/>
     </row>
-    <row r="50" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="50" spans="1:11">
       <c r="A50" s="32" t="s">
         <v>257</v>
       </c>
@@ -25679,7 +25695,7 @@
         <v>631</v>
       </c>
     </row>
-    <row r="52" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="52" spans="1:11">
       <c r="A52" s="32" t="s">
         <v>630</v>
       </c>
@@ -25696,4 +25712,1148 @@
     </ext>
   </extLst>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2D860635-8528-924E-9941-4AA3BC748BE2}">
+  <dimension ref="A1:I46"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
+  <sheetData>
+    <row r="1" spans="1:9">
+      <c r="A1" s="33" t="s">
+        <v>607</v>
+      </c>
+      <c r="B1" s="33" t="s">
+        <v>612</v>
+      </c>
+      <c r="C1" s="34" t="s">
+        <v>634</v>
+      </c>
+      <c r="D1" s="34" t="s">
+        <v>614</v>
+      </c>
+      <c r="E1" s="34" t="s">
+        <v>615</v>
+      </c>
+      <c r="F1" s="34" t="s">
+        <v>616</v>
+      </c>
+      <c r="G1" s="33" t="s">
+        <v>611</v>
+      </c>
+      <c r="H1" s="44" t="s">
+        <v>565</v>
+      </c>
+      <c r="I1" s="31" t="s">
+        <v>632</v>
+      </c>
+    </row>
+    <row r="2" spans="1:9">
+      <c r="A2" s="32" t="s">
+        <v>0</v>
+      </c>
+      <c r="B2" s="35" t="s">
+        <v>8</v>
+      </c>
+      <c r="C2" s="35" t="s">
+        <v>17</v>
+      </c>
+      <c r="D2" s="35" t="s">
+        <v>567</v>
+      </c>
+      <c r="E2" s="35" t="s">
+        <v>9</v>
+      </c>
+      <c r="F2" s="35" t="s">
+        <v>566</v>
+      </c>
+      <c r="G2" s="35" t="s">
+        <v>1</v>
+      </c>
+      <c r="H2" s="45" t="s">
+        <v>568</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9">
+      <c r="A3" s="32" t="s">
+        <v>23</v>
+      </c>
+      <c r="B3" s="35" t="s">
+        <v>26</v>
+      </c>
+      <c r="C3" s="35" t="s">
+        <v>33</v>
+      </c>
+      <c r="D3" s="35" t="s">
+        <v>569</v>
+      </c>
+      <c r="E3" s="35" t="s">
+        <v>27</v>
+      </c>
+      <c r="F3" s="35" t="s">
+        <v>567</v>
+      </c>
+      <c r="G3" s="35" t="s">
+        <v>622</v>
+      </c>
+      <c r="H3" s="45"/>
+    </row>
+    <row r="4" spans="1:9">
+      <c r="A4" s="32" t="s">
+        <v>38</v>
+      </c>
+      <c r="B4" s="35" t="s">
+        <v>39</v>
+      </c>
+      <c r="C4" s="35" t="s">
+        <v>50</v>
+      </c>
+      <c r="D4" s="35" t="s">
+        <v>572</v>
+      </c>
+      <c r="E4" s="35" t="s">
+        <v>46</v>
+      </c>
+      <c r="F4" s="35" t="s">
+        <v>567</v>
+      </c>
+      <c r="G4" s="35" t="s">
+        <v>622</v>
+      </c>
+      <c r="H4" s="45"/>
+    </row>
+    <row r="5" spans="1:9">
+      <c r="A5" s="32" t="s">
+        <v>38</v>
+      </c>
+      <c r="B5" s="35" t="s">
+        <v>39</v>
+      </c>
+      <c r="C5" s="35" t="s">
+        <v>50</v>
+      </c>
+      <c r="D5" s="35" t="s">
+        <v>572</v>
+      </c>
+      <c r="E5" s="35" t="s">
+        <v>40</v>
+      </c>
+      <c r="F5" s="35" t="s">
+        <v>570</v>
+      </c>
+      <c r="G5" s="35" t="s">
+        <v>1</v>
+      </c>
+      <c r="H5" s="45" t="s">
+        <v>573</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9">
+      <c r="A6" s="32" t="s">
+        <v>54</v>
+      </c>
+      <c r="B6" s="35" t="s">
+        <v>58</v>
+      </c>
+      <c r="C6" s="35" t="s">
+        <v>63</v>
+      </c>
+      <c r="D6" s="35" t="s">
+        <v>567</v>
+      </c>
+      <c r="E6" s="35" t="s">
+        <v>602</v>
+      </c>
+      <c r="F6" s="35" t="s">
+        <v>567</v>
+      </c>
+      <c r="G6" s="35" t="s">
+        <v>625</v>
+      </c>
+      <c r="H6" s="45" t="s">
+        <v>574</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9">
+      <c r="A7" s="32" t="s">
+        <v>66</v>
+      </c>
+      <c r="B7" s="35" t="s">
+        <v>67</v>
+      </c>
+      <c r="C7" s="35" t="s">
+        <v>71</v>
+      </c>
+      <c r="D7" s="35" t="s">
+        <v>575</v>
+      </c>
+      <c r="E7" s="35" t="s">
+        <v>68</v>
+      </c>
+      <c r="F7" s="35" t="s">
+        <v>570</v>
+      </c>
+      <c r="G7" s="35" t="s">
+        <v>625</v>
+      </c>
+      <c r="H7" s="45"/>
+    </row>
+    <row r="8" spans="1:9">
+      <c r="A8" s="32" t="s">
+        <v>75</v>
+      </c>
+      <c r="B8" s="35" t="s">
+        <v>79</v>
+      </c>
+      <c r="C8" s="35" t="s">
+        <v>82</v>
+      </c>
+      <c r="D8" s="35" t="s">
+        <v>567</v>
+      </c>
+      <c r="E8" s="35" t="s">
+        <v>80</v>
+      </c>
+      <c r="F8" s="35" t="s">
+        <v>566</v>
+      </c>
+      <c r="G8" s="35" t="s">
+        <v>619</v>
+      </c>
+      <c r="H8" s="45" t="s">
+        <v>578</v>
+      </c>
+    </row>
+    <row r="9" spans="1:9">
+      <c r="A9" s="32" t="s">
+        <v>86</v>
+      </c>
+      <c r="B9" s="35" t="s">
+        <v>87</v>
+      </c>
+      <c r="C9" s="35" t="s">
+        <v>92</v>
+      </c>
+      <c r="D9" s="35" t="s">
+        <v>567</v>
+      </c>
+      <c r="E9" s="35" t="s">
+        <v>88</v>
+      </c>
+      <c r="F9" s="35" t="s">
+        <v>577</v>
+      </c>
+      <c r="G9" s="35" t="s">
+        <v>619</v>
+      </c>
+      <c r="H9" s="45" t="s">
+        <v>579</v>
+      </c>
+    </row>
+    <row r="10" spans="1:9">
+      <c r="A10" s="32" t="s">
+        <v>95</v>
+      </c>
+      <c r="B10" s="35" t="s">
+        <v>98</v>
+      </c>
+      <c r="C10" s="35" t="s">
+        <v>103</v>
+      </c>
+      <c r="D10" s="35" t="s">
+        <v>576</v>
+      </c>
+      <c r="E10" s="35" t="s">
+        <v>99</v>
+      </c>
+      <c r="F10" s="35" t="s">
+        <v>570</v>
+      </c>
+      <c r="G10" s="35" t="s">
+        <v>626</v>
+      </c>
+      <c r="H10" s="45"/>
+    </row>
+    <row r="11" spans="1:9">
+      <c r="A11" s="32" t="s">
+        <v>107</v>
+      </c>
+      <c r="B11" s="35" t="s">
+        <v>110</v>
+      </c>
+      <c r="C11" s="35" t="s">
+        <v>115</v>
+      </c>
+      <c r="D11" s="35" t="s">
+        <v>571</v>
+      </c>
+      <c r="E11" s="35" t="s">
+        <v>111</v>
+      </c>
+      <c r="F11" s="35" t="s">
+        <v>567</v>
+      </c>
+      <c r="G11" s="35" t="s">
+        <v>1</v>
+      </c>
+      <c r="H11" s="45" t="s">
+        <v>580</v>
+      </c>
+    </row>
+    <row r="12" spans="1:9">
+      <c r="A12" s="32" t="s">
+        <v>118</v>
+      </c>
+      <c r="B12" s="35" t="s">
+        <v>120</v>
+      </c>
+      <c r="C12" s="35" t="s">
+        <v>124</v>
+      </c>
+      <c r="D12" s="35" t="s">
+        <v>567</v>
+      </c>
+      <c r="E12" s="35" t="s">
+        <v>121</v>
+      </c>
+      <c r="F12" s="35" t="s">
+        <v>570</v>
+      </c>
+      <c r="G12" s="35" t="s">
+        <v>1</v>
+      </c>
+      <c r="H12" s="45"/>
+    </row>
+    <row r="13" spans="1:9">
+      <c r="A13" s="32" t="s">
+        <v>118</v>
+      </c>
+      <c r="B13" s="35" t="s">
+        <v>120</v>
+      </c>
+      <c r="C13" s="35" t="s">
+        <v>124</v>
+      </c>
+      <c r="D13" s="35" t="s">
+        <v>567</v>
+      </c>
+      <c r="E13" s="35" t="s">
+        <v>129</v>
+      </c>
+      <c r="F13" s="35" t="s">
+        <v>570</v>
+      </c>
+      <c r="G13" s="35" t="s">
+        <v>626</v>
+      </c>
+      <c r="H13" s="45"/>
+    </row>
+    <row r="14" spans="1:9">
+      <c r="A14" s="32" t="s">
+        <v>132</v>
+      </c>
+      <c r="B14" s="35" t="s">
+        <v>134</v>
+      </c>
+      <c r="C14" s="35" t="s">
+        <v>141</v>
+      </c>
+      <c r="D14" s="35" t="s">
+        <v>570</v>
+      </c>
+      <c r="E14" s="35" t="s">
+        <v>135</v>
+      </c>
+      <c r="F14" s="35" t="s">
+        <v>567</v>
+      </c>
+      <c r="G14" s="35" t="s">
+        <v>1</v>
+      </c>
+      <c r="H14" s="45"/>
+    </row>
+    <row r="15" spans="1:9">
+      <c r="A15" s="32" t="s">
+        <v>143</v>
+      </c>
+      <c r="B15" s="35" t="s">
+        <v>144</v>
+      </c>
+      <c r="C15" s="35" t="s">
+        <v>148</v>
+      </c>
+      <c r="D15" s="35" t="s">
+        <v>567</v>
+      </c>
+      <c r="E15" s="35" t="s">
+        <v>145</v>
+      </c>
+      <c r="F15" s="35" t="s">
+        <v>570</v>
+      </c>
+      <c r="G15" s="35" t="s">
+        <v>619</v>
+      </c>
+      <c r="H15" s="45"/>
+    </row>
+    <row r="16" spans="1:9">
+      <c r="A16" s="32" t="s">
+        <v>598</v>
+      </c>
+      <c r="B16" s="35" t="s">
+        <v>599</v>
+      </c>
+      <c r="C16" s="35" t="s">
+        <v>601</v>
+      </c>
+      <c r="D16" s="35" t="s">
+        <v>567</v>
+      </c>
+      <c r="E16" s="35" t="s">
+        <v>600</v>
+      </c>
+      <c r="F16" s="35" t="s">
+        <v>570</v>
+      </c>
+      <c r="G16" s="35" t="s">
+        <v>1</v>
+      </c>
+      <c r="H16" s="45"/>
+    </row>
+    <row r="17" spans="1:8">
+      <c r="A17" s="32" t="s">
+        <v>609</v>
+      </c>
+      <c r="B17" s="35" t="s">
+        <v>156</v>
+      </c>
+      <c r="C17" s="35" t="s">
+        <v>160</v>
+      </c>
+      <c r="D17" s="35" t="s">
+        <v>581</v>
+      </c>
+      <c r="E17" s="35" t="s">
+        <v>157</v>
+      </c>
+      <c r="F17" s="35" t="s">
+        <v>570</v>
+      </c>
+      <c r="G17" s="35" t="s">
+        <v>1</v>
+      </c>
+      <c r="H17" s="45"/>
+    </row>
+    <row r="18" spans="1:8">
+      <c r="A18" s="32" t="s">
+        <v>185</v>
+      </c>
+      <c r="B18" s="35" t="s">
+        <v>186</v>
+      </c>
+      <c r="C18" s="35" t="s">
+        <v>191</v>
+      </c>
+      <c r="D18" s="35" t="s">
+        <v>576</v>
+      </c>
+      <c r="E18" s="35" t="s">
+        <v>187</v>
+      </c>
+      <c r="F18" s="35" t="s">
+        <v>570</v>
+      </c>
+      <c r="G18" s="35" t="s">
+        <v>622</v>
+      </c>
+      <c r="H18" s="45"/>
+    </row>
+    <row r="19" spans="1:8">
+      <c r="A19" s="32" t="s">
+        <v>194</v>
+      </c>
+      <c r="B19" s="35" t="s">
+        <v>196</v>
+      </c>
+      <c r="C19" s="35" t="s">
+        <v>203</v>
+      </c>
+      <c r="D19" s="35" t="s">
+        <v>570</v>
+      </c>
+      <c r="E19" s="35" t="s">
+        <v>197</v>
+      </c>
+      <c r="F19" s="35" t="s">
+        <v>567</v>
+      </c>
+      <c r="G19" s="35" t="s">
+        <v>620</v>
+      </c>
+      <c r="H19" s="45"/>
+    </row>
+    <row r="20" spans="1:8">
+      <c r="A20" s="32" t="s">
+        <v>212</v>
+      </c>
+      <c r="B20" s="35" t="s">
+        <v>213</v>
+      </c>
+      <c r="C20" s="35" t="s">
+        <v>218</v>
+      </c>
+      <c r="D20" s="35" t="s">
+        <v>567</v>
+      </c>
+      <c r="E20" s="35" t="s">
+        <v>214</v>
+      </c>
+      <c r="F20" s="35" t="s">
+        <v>584</v>
+      </c>
+      <c r="G20" s="35" t="s">
+        <v>622</v>
+      </c>
+      <c r="H20" s="45" t="s">
+        <v>585</v>
+      </c>
+    </row>
+    <row r="21" spans="1:8">
+      <c r="A21" s="32" t="s">
+        <v>222</v>
+      </c>
+      <c r="B21" s="35" t="s">
+        <v>223</v>
+      </c>
+      <c r="C21" s="35" t="s">
+        <v>229</v>
+      </c>
+      <c r="D21" s="35" t="s">
+        <v>572</v>
+      </c>
+      <c r="E21" s="35" t="s">
+        <v>224</v>
+      </c>
+      <c r="F21" s="35" t="s">
+        <v>586</v>
+      </c>
+      <c r="G21" s="35" t="s">
+        <v>622</v>
+      </c>
+      <c r="H21" s="45" t="s">
+        <v>635</v>
+      </c>
+    </row>
+    <row r="22" spans="1:8">
+      <c r="A22" s="32" t="s">
+        <v>234</v>
+      </c>
+      <c r="B22" s="35" t="s">
+        <v>237</v>
+      </c>
+      <c r="C22" s="35" t="s">
+        <v>242</v>
+      </c>
+      <c r="D22" s="35" t="s">
+        <v>567</v>
+      </c>
+      <c r="E22" s="35" t="s">
+        <v>238</v>
+      </c>
+      <c r="F22" s="35" t="s">
+        <v>570</v>
+      </c>
+      <c r="G22" s="35" t="s">
+        <v>1</v>
+      </c>
+      <c r="H22" s="45"/>
+    </row>
+    <row r="23" spans="1:8">
+      <c r="A23" s="32" t="s">
+        <v>245</v>
+      </c>
+      <c r="B23" s="35" t="s">
+        <v>249</v>
+      </c>
+      <c r="C23" s="35" t="s">
+        <v>254</v>
+      </c>
+      <c r="D23" s="35" t="s">
+        <v>570</v>
+      </c>
+      <c r="E23" s="35" t="s">
+        <v>250</v>
+      </c>
+      <c r="F23" s="35" t="s">
+        <v>567</v>
+      </c>
+      <c r="G23" s="35" t="s">
+        <v>623</v>
+      </c>
+      <c r="H23" s="45" t="s">
+        <v>636</v>
+      </c>
+    </row>
+    <row r="24" spans="1:8">
+      <c r="A24" s="32" t="s">
+        <v>267</v>
+      </c>
+      <c r="B24" s="35" t="s">
+        <v>268</v>
+      </c>
+      <c r="C24" s="35" t="s">
+        <v>273</v>
+      </c>
+      <c r="D24" s="35" t="s">
+        <v>576</v>
+      </c>
+      <c r="E24" s="35" t="s">
+        <v>269</v>
+      </c>
+      <c r="F24" s="35" t="s">
+        <v>567</v>
+      </c>
+      <c r="G24" s="35" t="s">
+        <v>619</v>
+      </c>
+      <c r="H24" s="45" t="s">
+        <v>589</v>
+      </c>
+    </row>
+    <row r="25" spans="1:8">
+      <c r="A25" s="32" t="s">
+        <v>280</v>
+      </c>
+      <c r="B25" s="35" t="s">
+        <v>281</v>
+      </c>
+      <c r="C25" s="35" t="s">
+        <v>287</v>
+      </c>
+      <c r="D25" s="35" t="s">
+        <v>584</v>
+      </c>
+      <c r="E25" s="35" t="s">
+        <v>282</v>
+      </c>
+      <c r="F25" s="35" t="s">
+        <v>567</v>
+      </c>
+      <c r="G25" s="35" t="s">
+        <v>619</v>
+      </c>
+      <c r="H25" s="45"/>
+    </row>
+    <row r="26" spans="1:8">
+      <c r="A26" s="32" t="s">
+        <v>289</v>
+      </c>
+      <c r="B26" s="35" t="s">
+        <v>290</v>
+      </c>
+      <c r="C26" s="35" t="s">
+        <v>295</v>
+      </c>
+      <c r="D26" s="35" t="s">
+        <v>567</v>
+      </c>
+      <c r="E26" s="35" t="s">
+        <v>291</v>
+      </c>
+      <c r="F26" s="35" t="s">
+        <v>586</v>
+      </c>
+      <c r="G26" s="35" t="s">
+        <v>1</v>
+      </c>
+      <c r="H26" s="45"/>
+    </row>
+    <row r="27" spans="1:8">
+      <c r="A27" s="32" t="s">
+        <v>298</v>
+      </c>
+      <c r="B27" s="35" t="s">
+        <v>299</v>
+      </c>
+      <c r="C27" s="35" t="s">
+        <v>303</v>
+      </c>
+      <c r="D27" s="35" t="s">
+        <v>567</v>
+      </c>
+      <c r="E27" s="35" t="s">
+        <v>300</v>
+      </c>
+      <c r="F27" s="35" t="s">
+        <v>586</v>
+      </c>
+      <c r="G27" s="35" t="s">
+        <v>622</v>
+      </c>
+      <c r="H27" s="45"/>
+    </row>
+    <row r="28" spans="1:8">
+      <c r="A28" s="32" t="s">
+        <v>608</v>
+      </c>
+      <c r="B28" s="35" t="s">
+        <v>314</v>
+      </c>
+      <c r="C28" s="35" t="s">
+        <v>318</v>
+      </c>
+      <c r="D28" s="35" t="s">
+        <v>567</v>
+      </c>
+      <c r="E28" s="35" t="s">
+        <v>315</v>
+      </c>
+      <c r="F28" s="35" t="s">
+        <v>586</v>
+      </c>
+      <c r="G28" s="35" t="s">
+        <v>620</v>
+      </c>
+      <c r="H28" s="45"/>
+    </row>
+    <row r="29" spans="1:8">
+      <c r="A29" s="32" t="s">
+        <v>320</v>
+      </c>
+      <c r="B29" s="35" t="s">
+        <v>321</v>
+      </c>
+      <c r="C29" s="35" t="s">
+        <v>328</v>
+      </c>
+      <c r="D29" s="35" t="s">
+        <v>567</v>
+      </c>
+      <c r="E29" s="35" t="s">
+        <v>322</v>
+      </c>
+      <c r="F29" s="35" t="s">
+        <v>570</v>
+      </c>
+      <c r="G29" s="35" t="s">
+        <v>622</v>
+      </c>
+      <c r="H29" s="45"/>
+    </row>
+    <row r="30" spans="1:8">
+      <c r="A30" s="32" t="s">
+        <v>334</v>
+      </c>
+      <c r="B30" s="35" t="s">
+        <v>336</v>
+      </c>
+      <c r="C30" s="35" t="s">
+        <v>341</v>
+      </c>
+      <c r="D30" s="35" t="s">
+        <v>586</v>
+      </c>
+      <c r="E30" s="35" t="s">
+        <v>337</v>
+      </c>
+      <c r="F30" s="35" t="s">
+        <v>567</v>
+      </c>
+      <c r="G30" s="35" t="s">
+        <v>624</v>
+      </c>
+      <c r="H30" s="45"/>
+    </row>
+    <row r="31" spans="1:8">
+      <c r="A31" s="32" t="s">
+        <v>344</v>
+      </c>
+      <c r="B31" s="35" t="s">
+        <v>347</v>
+      </c>
+      <c r="C31" s="35" t="s">
+        <v>354</v>
+      </c>
+      <c r="D31" s="35" t="s">
+        <v>586</v>
+      </c>
+      <c r="E31" s="35" t="s">
+        <v>348</v>
+      </c>
+      <c r="F31" s="35" t="s">
+        <v>567</v>
+      </c>
+      <c r="G31" s="35" t="s">
+        <v>345</v>
+      </c>
+      <c r="H31" s="45"/>
+    </row>
+    <row r="32" spans="1:8">
+      <c r="A32" s="32" t="s">
+        <v>365</v>
+      </c>
+      <c r="B32" s="35" t="s">
+        <v>368</v>
+      </c>
+      <c r="C32" s="35" t="s">
+        <v>373</v>
+      </c>
+      <c r="D32" s="35" t="s">
+        <v>570</v>
+      </c>
+      <c r="E32" s="35" t="s">
+        <v>369</v>
+      </c>
+      <c r="F32" s="35" t="s">
+        <v>590</v>
+      </c>
+      <c r="G32" s="35" t="s">
+        <v>1</v>
+      </c>
+      <c r="H32" s="45"/>
+    </row>
+    <row r="33" spans="1:8">
+      <c r="A33" s="32" t="s">
+        <v>394</v>
+      </c>
+      <c r="B33" s="35" t="s">
+        <v>395</v>
+      </c>
+      <c r="C33" s="35" t="s">
+        <v>398</v>
+      </c>
+      <c r="D33" s="35" t="s">
+        <v>576</v>
+      </c>
+      <c r="E33" s="35" t="s">
+        <v>396</v>
+      </c>
+      <c r="F33" s="35" t="s">
+        <v>570</v>
+      </c>
+      <c r="G33" s="35" t="s">
+        <v>1</v>
+      </c>
+      <c r="H33" s="45"/>
+    </row>
+    <row r="34" spans="1:8">
+      <c r="A34" s="32" t="s">
+        <v>401</v>
+      </c>
+      <c r="B34" s="35" t="s">
+        <v>402</v>
+      </c>
+      <c r="C34" s="35" t="s">
+        <v>406</v>
+      </c>
+      <c r="D34" s="35" t="s">
+        <v>567</v>
+      </c>
+      <c r="E34" s="35" t="s">
+        <v>403</v>
+      </c>
+      <c r="F34" s="35" t="s">
+        <v>586</v>
+      </c>
+      <c r="G34" s="35" t="s">
+        <v>622</v>
+      </c>
+      <c r="H34" s="45"/>
+    </row>
+    <row r="35" spans="1:8">
+      <c r="A35" s="32" t="s">
+        <v>409</v>
+      </c>
+      <c r="B35" s="35" t="s">
+        <v>410</v>
+      </c>
+      <c r="C35" s="35" t="s">
+        <v>413</v>
+      </c>
+      <c r="D35" s="35" t="s">
+        <v>567</v>
+      </c>
+      <c r="E35" s="35" t="s">
+        <v>411</v>
+      </c>
+      <c r="F35" s="35" t="s">
+        <v>570</v>
+      </c>
+      <c r="G35" s="35" t="s">
+        <v>619</v>
+      </c>
+      <c r="H35" s="45"/>
+    </row>
+    <row r="36" spans="1:8">
+      <c r="A36" s="32" t="s">
+        <v>417</v>
+      </c>
+      <c r="B36" s="35" t="s">
+        <v>418</v>
+      </c>
+      <c r="C36" s="35" t="s">
+        <v>424</v>
+      </c>
+      <c r="D36" s="35" t="s">
+        <v>586</v>
+      </c>
+      <c r="E36" s="35" t="s">
+        <v>419</v>
+      </c>
+      <c r="F36" s="35" t="s">
+        <v>567</v>
+      </c>
+      <c r="G36" s="35" t="s">
+        <v>624</v>
+      </c>
+      <c r="H36" s="45"/>
+    </row>
+    <row r="37" spans="1:8">
+      <c r="A37" s="32" t="s">
+        <v>427</v>
+      </c>
+      <c r="B37" s="35" t="s">
+        <v>429</v>
+      </c>
+      <c r="C37" s="35" t="s">
+        <v>432</v>
+      </c>
+      <c r="D37" s="35" t="s">
+        <v>570</v>
+      </c>
+      <c r="E37" s="35" t="s">
+        <v>430</v>
+      </c>
+      <c r="F37" s="35" t="s">
+        <v>567</v>
+      </c>
+      <c r="G37" s="35" t="s">
+        <v>428</v>
+      </c>
+      <c r="H37" s="45"/>
+    </row>
+    <row r="38" spans="1:8">
+      <c r="A38" s="32" t="s">
+        <v>444</v>
+      </c>
+      <c r="B38" s="35" t="s">
+        <v>446</v>
+      </c>
+      <c r="C38" s="35" t="s">
+        <v>447</v>
+      </c>
+      <c r="D38" s="35" t="s">
+        <v>595</v>
+      </c>
+      <c r="E38" s="35" t="s">
+        <v>606</v>
+      </c>
+      <c r="F38" s="35" t="s">
+        <v>570</v>
+      </c>
+      <c r="G38" s="35" t="s">
+        <v>619</v>
+      </c>
+      <c r="H38" s="45"/>
+    </row>
+    <row r="39" spans="1:8">
+      <c r="A39" s="32" t="s">
+        <v>444</v>
+      </c>
+      <c r="B39" s="35" t="s">
+        <v>446</v>
+      </c>
+      <c r="C39" s="35" t="s">
+        <v>603</v>
+      </c>
+      <c r="D39" s="35" t="s">
+        <v>567</v>
+      </c>
+      <c r="E39" s="35" t="s">
+        <v>604</v>
+      </c>
+      <c r="F39" s="35" t="s">
+        <v>593</v>
+      </c>
+      <c r="G39" s="35" t="s">
+        <v>621</v>
+      </c>
+      <c r="H39" s="45"/>
+    </row>
+    <row r="40" spans="1:8">
+      <c r="A40" s="32" t="s">
+        <v>444</v>
+      </c>
+      <c r="B40" s="35" t="s">
+        <v>446</v>
+      </c>
+      <c r="C40" s="35" t="s">
+        <v>455</v>
+      </c>
+      <c r="D40" s="35" t="s">
+        <v>596</v>
+      </c>
+      <c r="E40" s="35" t="s">
+        <v>605</v>
+      </c>
+      <c r="F40" s="35" t="s">
+        <v>590</v>
+      </c>
+      <c r="G40" s="35" t="s">
+        <v>622</v>
+      </c>
+      <c r="H40" s="45" t="s">
+        <v>594</v>
+      </c>
+    </row>
+    <row r="41" spans="1:8">
+      <c r="A41" s="46" t="s">
+        <v>475</v>
+      </c>
+      <c r="B41" s="47" t="s">
+        <v>476</v>
+      </c>
+      <c r="C41" s="48" t="s">
+        <v>477</v>
+      </c>
+      <c r="D41" s="47" t="s">
+        <v>567</v>
+      </c>
+      <c r="E41" s="48" t="s">
+        <v>633</v>
+      </c>
+      <c r="F41" s="47" t="s">
+        <v>586</v>
+      </c>
+      <c r="G41" s="47" t="s">
+        <v>619</v>
+      </c>
+      <c r="H41" s="49"/>
+    </row>
+    <row r="42" spans="1:8">
+      <c r="A42" s="46" t="s">
+        <v>475</v>
+      </c>
+      <c r="B42" s="47" t="s">
+        <v>476</v>
+      </c>
+      <c r="C42" s="48" t="s">
+        <v>481</v>
+      </c>
+      <c r="D42" s="47" t="s">
+        <v>567</v>
+      </c>
+      <c r="E42" s="48" t="s">
+        <v>633</v>
+      </c>
+      <c r="F42" s="47" t="s">
+        <v>586</v>
+      </c>
+      <c r="G42" s="47" t="s">
+        <v>622</v>
+      </c>
+      <c r="H42" s="49"/>
+    </row>
+    <row r="43" spans="1:8">
+      <c r="A43" s="32" t="s">
+        <v>488</v>
+      </c>
+      <c r="B43" s="35" t="s">
+        <v>489</v>
+      </c>
+      <c r="C43" s="35" t="s">
+        <v>494</v>
+      </c>
+      <c r="D43" s="35" t="s">
+        <v>592</v>
+      </c>
+      <c r="E43" s="35" t="s">
+        <v>504</v>
+      </c>
+      <c r="F43" s="35" t="s">
+        <v>586</v>
+      </c>
+      <c r="G43" s="35" t="s">
+        <v>619</v>
+      </c>
+      <c r="H43" s="45"/>
+    </row>
+    <row r="44" spans="1:8">
+      <c r="A44" s="32" t="s">
+        <v>488</v>
+      </c>
+      <c r="B44" s="35" t="s">
+        <v>489</v>
+      </c>
+      <c r="C44" s="35" t="s">
+        <v>494</v>
+      </c>
+      <c r="D44" s="35" t="s">
+        <v>567</v>
+      </c>
+      <c r="E44" s="35" t="s">
+        <v>490</v>
+      </c>
+      <c r="F44" s="35" t="s">
+        <v>586</v>
+      </c>
+      <c r="G44" s="35" t="s">
+        <v>621</v>
+      </c>
+      <c r="H44" s="45"/>
+    </row>
+    <row r="45" spans="1:8">
+      <c r="A45" s="32" t="s">
+        <v>488</v>
+      </c>
+      <c r="B45" s="35" t="s">
+        <v>489</v>
+      </c>
+      <c r="C45" s="35" t="s">
+        <v>494</v>
+      </c>
+      <c r="D45" s="35" t="s">
+        <v>567</v>
+      </c>
+      <c r="E45" s="35" t="s">
+        <v>497</v>
+      </c>
+      <c r="F45" s="35" t="s">
+        <v>570</v>
+      </c>
+      <c r="G45" s="35" t="s">
+        <v>622</v>
+      </c>
+      <c r="H45" s="45"/>
+    </row>
+    <row r="46" spans="1:8">
+      <c r="A46" s="32" t="s">
+        <v>509</v>
+      </c>
+      <c r="B46" s="35" t="s">
+        <v>510</v>
+      </c>
+      <c r="C46" s="35" t="s">
+        <v>520</v>
+      </c>
+      <c r="D46" s="35" t="s">
+        <v>567</v>
+      </c>
+      <c r="E46" s="35" t="s">
+        <v>511</v>
+      </c>
+      <c r="F46" s="35" t="s">
+        <v>597</v>
+      </c>
+      <c r="G46" s="35" t="s">
+        <v>621</v>
+      </c>
+      <c r="H46" s="45"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>